<commit_message>
Added things to do.
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="19950" windowHeight="8625"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="19950" windowHeight="8625" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="296">
   <si>
     <t>Time required</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Story</t>
   </si>
   <si>
-    <t>Produce mouse / keyboard / gamepad buttons images</t>
-  </si>
-  <si>
     <t>Modify the current texts to use the new font</t>
   </si>
   <si>
@@ -754,15 +751,6 @@
     <t>Use the camera for more grandiose effect. But how?</t>
   </si>
   <si>
-    <t>Mega sprint 1 : Better menu</t>
-  </si>
-  <si>
-    <t>Produce the help messages for the menu</t>
-  </si>
-  <si>
-    <t>Layout of the menu</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -800,13 +788,133 @@
   </si>
   <si>
     <t>World Scene -&gt; Game Scene -&gt; Die -&gt; World Scene : Help Bar Message not displayed</t>
+  </si>
+  <si>
+    <t>Produce mouse buttons images</t>
+  </si>
+  <si>
+    <t>Produce keyboard buttons images</t>
+  </si>
+  <si>
+    <t>Produce gamepad buttons images</t>
+  </si>
+  <si>
+    <t>Add tips that show randomly on the help bar</t>
+  </si>
+  <si>
+    <t>Produce the texts that will be included in the tutorial</t>
+  </si>
+  <si>
+    <t>Drop the Commodore?</t>
+  </si>
+  <si>
+    <t>Drop the Commodore and find a better way to display the tutorial</t>
+  </si>
+  <si>
+    <t>Show the tutorial ingame: game paused, the spaceship talking</t>
+  </si>
+  <si>
+    <t>Canceled</t>
+  </si>
+  <si>
+    <t>Produce help messages</t>
+  </si>
+  <si>
+    <t>Produce tutorial</t>
+  </si>
+  <si>
+    <t>Michael McIntyre</t>
+  </si>
+  <si>
+    <t>Make the spaceship shoot</t>
+  </si>
+  <si>
+    <t>Level design</t>
+  </si>
+  <si>
+    <t>"Be able to swap levels over time" -Michael McIntyre</t>
+  </si>
+  <si>
+    <t>Introduce the gravity first, then the spaceship shooting</t>
+  </si>
+  <si>
+    <t>"Identify what players like" - Micheal McIntyre</t>
+  </si>
+  <si>
+    <t>Identify which turrets make the core and which one are more specialized</t>
+  </si>
+  <si>
+    <t>Produce a level design document</t>
+  </si>
+  <si>
+    <t>Find more gameplay elements with the spaceship (ex: able to bend the path)</t>
+  </si>
+  <si>
+    <t>Find mechanics with money -&gt; upgrade spaceship?</t>
+  </si>
+  <si>
+    <t>Add the "skip" in the cutscene scene helpbar</t>
+  </si>
+  <si>
+    <t>"Design levels that fit in the bounds of the tv"</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>A more evident way to know what is selectable (what is mine)</t>
+  </si>
+  <si>
+    <t>A more evident way to know where am I (spaceship)</t>
+  </si>
+  <si>
+    <t>Remove hicups in loading scene &lt;-&gt; main menu transition</t>
+  </si>
+  <si>
+    <t>Remove hicups in world &lt;-&gt; level transition</t>
+  </si>
+  <si>
+    <t>Remove hicups in level finished</t>
+  </si>
+  <si>
+    <t>Better mouse input</t>
+  </si>
+  <si>
+    <t>Use the keyboard as primary input</t>
+  </si>
+  <si>
+    <t>In some levels, go back to World is not B but Start</t>
+  </si>
+  <si>
+    <t>Fade effect for level description in world</t>
+  </si>
+  <si>
+    <t>Give visual priority to CB/turrets/ etc. menus over help bar</t>
+  </si>
+  <si>
+    <t>When restarting a level, enemies don't give money</t>
+  </si>
+  <si>
+    <t>Concentrate on how to add replay value to levels</t>
+  </si>
+  <si>
+    <t>New game modes (replay value)</t>
+  </si>
+  <si>
+    <t>More than one difficulty per level (replay value)</t>
+  </si>
+  <si>
+    <t>Asset editor (replay value) -&gt; create your own space drama</t>
+  </si>
+  <si>
+    <t>Things to accomplish in a level, a-la achievements (replay value)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,18 +956,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -876,12 +996,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -903,12 +1025,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Accent3" xfId="2" builtinId="37"/>
+  <cellStyles count="5">
+    <cellStyle name="Accent2" xfId="3" builtinId="33"/>
+    <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Warning Text" xfId="2" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1207,65 +1337,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C205"/>
+  <dimension ref="A1:D222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="D199" sqref="D199"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="84.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5" s="7">
         <v>12</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="7"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1273,7 +1415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1281,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1289,7 +1431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1297,7 +1439,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1305,286 +1447,281 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="1">
         <v>6</v>
       </c>
-      <c r="C16" s="9"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
       </c>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>258</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>257</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>256</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B31" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>142</v>
       </c>
-      <c r="B26" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>143</v>
-      </c>
-      <c r="B27" s="1">
+      <c r="B33" s="1">
         <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>145</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>146</v>
-      </c>
-      <c r="B29" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>144</v>
       </c>
       <c r="B34" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
       <c r="B35" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>119</v>
-      </c>
-      <c r="B36" s="1">
-        <v>1</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="1">
-        <v>0.5</v>
+        <v>288</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="1">
-        <v>1</v>
+      <c r="A40" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B41" s="1">
-        <v>4</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>26</v>
+      <c r="A43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B44" s="1">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="B45" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="B46" s="1">
-        <v>2</v>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="B51" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="B52" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="B53" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>44</v>
-      </c>
-      <c r="B54" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B55" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="1">
-        <v>3</v>
-      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>29</v>
+      <c r="A58" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="B59" s="1">
         <v>4</v>
@@ -1592,15 +1729,15 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B60" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B61" s="1">
         <v>8</v>
@@ -1608,129 +1745,129 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B62" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="B63" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>44</v>
-      </c>
-      <c r="B64" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>62</v>
-      </c>
-      <c r="B65" s="1">
-        <v>3</v>
+      <c r="A65" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="B66" s="1">
-        <v>3</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>32</v>
+      </c>
+      <c r="B67" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>30</v>
+      <c r="A68" t="s">
+        <v>33</v>
+      </c>
+      <c r="B68" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B69" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B70" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B71" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B72" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B73" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>44</v>
-      </c>
-      <c r="B74" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>64</v>
-      </c>
-      <c r="B75" s="1">
-        <v>3</v>
+      <c r="A75" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B76" s="1">
-        <v>3</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>45</v>
+      </c>
+      <c r="B77" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>49</v>
+      <c r="A78" t="s">
+        <v>46</v>
+      </c>
+      <c r="B78" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B79" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B80" s="1">
         <v>8</v>
@@ -1738,47 +1875,36 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B81" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B82" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B83" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>53</v>
-      </c>
-      <c r="B84" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>54</v>
-      </c>
-      <c r="B85" s="1">
-        <v>8</v>
+      <c r="A85" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B86" s="1">
         <v>8</v>
@@ -1786,195 +1912,192 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B87" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>66</v>
+        <v>51</v>
+      </c>
+      <c r="B88" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>55</v>
+      </c>
+      <c r="B89" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>105</v>
+      <c r="A90" t="s">
+        <v>56</v>
       </c>
       <c r="B90" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="B91" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="B92" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="B93" s="1">
-        <v>1</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>54</v>
+      </c>
+      <c r="B94" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>114</v>
-      </c>
-      <c r="B96" s="1">
-        <v>1</v>
+      <c r="A95" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>115</v>
+      <c r="A97" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="B97" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B98" s="1">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="B99" s="1">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B100" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>113</v>
+      </c>
+      <c r="B104" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>114</v>
+      </c>
+      <c r="B105" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>109</v>
+      </c>
+      <c r="B106" s="1">
         <v>16</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>112</v>
-      </c>
-      <c r="B101" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>111</v>
-      </c>
-      <c r="B102" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>109</v>
-      </c>
-      <c r="B103" s="1">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="B107" s="1">
-        <v>0.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="B108" s="1">
-        <v>0.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="B109" s="1">
-        <v>0.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="B110" s="1">
-        <v>0.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="B111" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>74</v>
-      </c>
-      <c r="B112" s="1">
-        <v>0.5</v>
+        <v>72</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>79</v>
-      </c>
-      <c r="B113" s="1">
-        <v>0.5</v>
+      <c r="A113" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>186</v>
-      </c>
-      <c r="B114" s="1">
-        <v>0.5</v>
+      <c r="A114" s="5" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B115" s="1">
         <v>0.5</v>
@@ -1982,7 +2105,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B116" s="1">
         <v>0.5</v>
@@ -1990,7 +2113,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B117" s="1">
         <v>0.5</v>
@@ -1998,467 +2121,569 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B118" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B119" s="1">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B120" s="1">
-        <v>3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B121" s="1">
-        <v>6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>83</v>
+        <v>185</v>
       </c>
       <c r="B122" s="1">
-        <v>16</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B123" s="1">
-        <v>8</v>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>75</v>
+      </c>
+      <c r="B124" s="1">
+        <v>0.5</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
-        <v>93</v>
+      <c r="A125" t="s">
+        <v>76</v>
+      </c>
+      <c r="B125" s="1">
+        <v>0.5</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>86</v>
+        <v>77</v>
+      </c>
+      <c r="B126" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>87</v>
+        <v>79</v>
+      </c>
+      <c r="B127" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>89</v>
+        <v>80</v>
+      </c>
+      <c r="B128" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>90</v>
+      <c r="A130" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>227</v>
+        <v>89</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>228</v>
+        <v>121</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>229</v>
+        <v>122</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>230</v>
+        <v>90</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>241</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>177</v>
+      <c r="A141" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>178</v>
+        <v>228</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>179</v>
+        <v>240</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>180</v>
+        <v>265</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B152" s="1">
-        <v>4</v>
+      <c r="A152" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>94</v>
-      </c>
-      <c r="B153" s="1">
-        <v>1</v>
+        <v>179</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>96</v>
-      </c>
-      <c r="B154" s="1">
-        <v>3</v>
+        <v>180</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>97</v>
-      </c>
-      <c r="B155" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>98</v>
-      </c>
-      <c r="B156" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>99</v>
-      </c>
-      <c r="B157" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>100</v>
-      </c>
-      <c r="B158" s="1">
-        <v>3</v>
+        <v>182</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>101</v>
-      </c>
-      <c r="B159" s="1">
-        <v>3</v>
+      <c r="A159" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>102</v>
+      <c r="A160" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="B160" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B161" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B162" s="1">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="B163" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="B164" s="1">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>118</v>
+        <v>98</v>
+      </c>
+      <c r="B165" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>187</v>
+        <v>99</v>
+      </c>
+      <c r="B166" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>189</v>
+        <v>100</v>
+      </c>
+      <c r="B167" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>192</v>
+        <v>101</v>
+      </c>
+      <c r="B168" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>214</v>
+        <v>102</v>
+      </c>
+      <c r="B169" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>226</v>
+        <v>103</v>
+      </c>
+      <c r="B170" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>257</v>
+        <v>115</v>
+      </c>
+      <c r="B171" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>116</v>
+      </c>
+      <c r="B172" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="2" t="s">
-        <v>127</v>
+      <c r="A173" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="5" t="s">
-        <v>128</v>
+      <c r="A174" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>130</v>
-      </c>
-      <c r="B175" s="1">
-        <v>4</v>
+        <v>188</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>129</v>
+      </c>
+      <c r="B187" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="2" t="s">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="2" t="s">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>287</v>
+      </c>
+      <c r="C212" s="11"/>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>290</v>
+      </c>
+      <c r="C213" s="11"/>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
         <v>23</v>
       </c>
-      <c r="B199" s="1">
+      <c r="B216" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>12</v>
       </c>
-      <c r="B200" s="1">
+      <c r="B217" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>13</v>
       </c>
-      <c r="B201" s="1">
+      <c r="B218" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>14</v>
       </c>
-      <c r="B202" s="1">
+      <c r="B219" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
         <v>15</v>
       </c>
-      <c r="B203" s="1">
+      <c r="B220" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
         <v>24</v>
       </c>
-      <c r="B204" s="1">
+      <c r="B221" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
         <v>25</v>
       </c>
-      <c r="B205" s="1">
+      <c r="B222" s="1">
         <v>2</v>
       </c>
     </row>
@@ -2470,10 +2695,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2483,37 +2708,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>246</v>
-      </c>
+      <c r="A1" s="3"/>
+      <c r="B1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2523,10 +2719,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A50"/>
+  <dimension ref="A1:A70"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2536,205 +2732,292 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>243</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>85</v>
+      <c r="A13" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>161</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>140</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>195</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>217</v>
+      <c r="A23" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="A24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>26</v>
+      <c r="A27" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>95</v>
+      <c r="A40" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>215</v>
+        <v>261</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>216</v>
+      <c r="A43" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>219</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>194</v>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2745,10 +3028,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,82 +3041,112 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>173</v>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>174</v>
+      <c r="A19" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2858,70 +3171,70 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" t="s">
         <v>202</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" t="s">
         <v>200</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" t="s">
         <v>210</v>
-      </c>
-      <c r="C7" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2942,12 +3255,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2972,49 +3285,49 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>234</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorganized audio + more control tools + white for player
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="19950" windowHeight="8625" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="19050" windowHeight="8625" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="305">
   <si>
     <t>Time required</t>
   </si>
@@ -517,9 +517,6 @@
     <t>How to adapt the game interface for mobiles</t>
   </si>
   <si>
-    <t>Paul Warner</t>
-  </si>
-  <si>
     <t>Learn how to mix sounds together that will play well even if there is a lot</t>
   </si>
   <si>
@@ -908,13 +905,43 @@
   </si>
   <si>
     <t>Things to accomplish in a level, a-la achievements (replay value)</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Music not restarted when level restarted</t>
+  </si>
+  <si>
+    <t>When a custom asset is not found, there should be an exception thrown</t>
+  </si>
+  <si>
+    <t>Sometimes, pause &lt;-&gt; resume a game keeps the game simulation on paused state</t>
+  </si>
+  <si>
+    <t>Paul Williams</t>
+  </si>
+  <si>
+    <t>Tiego Francois-Brosseau</t>
+  </si>
+  <si>
+    <t>Make a business plan</t>
+  </si>
+  <si>
+    <t>Stop what you're doing and focus on where you want to go with your game</t>
+  </si>
+  <si>
+    <t>Avoid feature creep</t>
+  </si>
+  <si>
+    <t>White only for players so : path black to red, remove white enemy, change battleship color</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -968,8 +995,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -986,6 +1020,42 @@
         <fgColor theme="6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -996,14 +1066,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1032,8 +1108,32 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="10"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
+    <cellStyle name="20% - Accent2" xfId="5" builtinId="34"/>
+    <cellStyle name="20% - Accent3" xfId="8" builtinId="38"/>
+    <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="7" builtinId="36"/>
+    <cellStyle name="60% - Accent3" xfId="10" builtinId="40"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1337,11 +1437,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D222"/>
+  <dimension ref="A1:E225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,9 +1450,10 @@
     <col min="2" max="2" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>124</v>
       </c>
@@ -1360,18 +1461,21 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>125</v>
       </c>
@@ -1379,7 +1483,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>128</v>
       </c>
@@ -1387,9 +1491,9 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B5" s="7">
         <v>12</v>
@@ -1397,17 +1501,17 @@
       <c r="C5" s="7"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1415,7 +1519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1423,7 +1527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1431,7 +1535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1439,7 +1543,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1447,7 +1551,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1456,12 +1560,12 @@
       </c>
       <c r="D13" s="9"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1487,7 +1591,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1507,12 +1611,12 @@
         <v>3</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -1521,7 +1625,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
@@ -1529,7 +1633,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
@@ -1537,12 +1641,12 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1600,12 +1704,12 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2018,7 +2122,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2085,127 +2189,151 @@
         <v>72</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>68</v>
       </c>
       <c r="B115" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C115" s="11"/>
+      <c r="E115" s="18"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>69</v>
       </c>
       <c r="B116" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C116" s="11"/>
+      <c r="E116" s="19"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>71</v>
       </c>
       <c r="B117" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C117" s="11"/>
+      <c r="E117" s="15"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>70</v>
       </c>
       <c r="B118" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C118" s="11"/>
+      <c r="E118" s="18"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>72</v>
       </c>
       <c r="B119" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C119" s="11"/>
+      <c r="E119" s="15"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>73</v>
       </c>
       <c r="B120" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C120" s="11"/>
+      <c r="E120" s="19"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>78</v>
       </c>
       <c r="B121" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C121" s="11"/>
+      <c r="E121" s="21"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B122" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C122" s="11"/>
+      <c r="E122" s="14"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>74</v>
       </c>
       <c r="B123" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C123" s="11"/>
+      <c r="E123" s="20"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>75</v>
       </c>
       <c r="B124" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C124" s="11"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>76</v>
       </c>
       <c r="B125" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C125" s="11"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>77</v>
       </c>
       <c r="B126" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C126" s="11"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>79</v>
       </c>
       <c r="B127" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C127" s="11"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>80</v>
       </c>
       <c r="B128" s="1">
         <v>3</v>
       </c>
+      <c r="C128" s="11"/>
+      <c r="D128" s="9"/>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
@@ -2259,77 +2387,77 @@
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -2448,52 +2576,52 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -2516,7 +2644,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -2529,161 +2657,189 @@
         <v>133</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="2" t="s">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="2" t="s">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C205" s="12"/>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
+        <v>186</v>
+      </c>
+      <c r="C206" s="11"/>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>188</v>
+      </c>
+      <c r="C207" s="11"/>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C208" s="16"/>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
+        <v>210</v>
+      </c>
+      <c r="C209" s="11"/>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>250</v>
+      </c>
+      <c r="C210" s="13"/>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C211" s="13"/>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>287</v>
-      </c>
-      <c r="C212" s="11"/>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="C212" s="17"/>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C213" s="11"/>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" s="2" t="s">
+      <c r="D213" s="9"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>289</v>
+      </c>
+      <c r="C214" s="11"/>
+      <c r="D214" s="9"/>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>296</v>
+      </c>
+      <c r="C215" s="11"/>
+      <c r="D215" s="9"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>298</v>
+      </c>
+      <c r="C216"/>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>23</v>
-      </c>
-      <c r="B216" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>12</v>
-      </c>
-      <c r="B217" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>13</v>
-      </c>
-      <c r="B218" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>14</v>
       </c>
       <c r="B219" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
+        <v>12</v>
+      </c>
+      <c r="B220" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>13</v>
+      </c>
+      <c r="B221" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>14</v>
+      </c>
+      <c r="B222" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>15</v>
       </c>
-      <c r="B220" s="1">
+      <c r="B223" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
         <v>24</v>
       </c>
-      <c r="B221" s="1">
+      <c r="B224" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>25</v>
       </c>
-      <c r="B222" s="1">
+      <c r="B225" s="1">
         <v>2</v>
       </c>
     </row>
@@ -2719,10 +2875,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A70"/>
+  <dimension ref="A1:A72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2772,32 +2928,32 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -2852,27 +3008,27 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -2892,17 +3048,17 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
@@ -2937,87 +3093,92 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>259</v>
-      </c>
-    </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+      <c r="A66" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>272</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3028,15 +3189,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3056,101 +3217,122 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>165</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>276</v>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3171,70 +3353,70 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" t="s">
         <v>201</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" t="s">
         <v>199</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" t="s">
         <v>209</v>
-      </c>
-      <c r="C7" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3255,12 +3437,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3285,49 +3467,49 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>233</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B5" t="s">
         <v>247</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>248</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>249</v>
-      </c>
-      <c r="D5" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nice flow between menu -> intro -> world 1 + new way to handle save games (to test)
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="19050" windowHeight="8625" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="19050" windowHeight="8625"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="401">
   <si>
     <t>Tweaking System</t>
   </si>
@@ -1206,6 +1206,24 @@
   </si>
   <si>
     <t>In World, the turrets around the celestial bodies are those available in the level</t>
+  </si>
+  <si>
+    <t>When connecting, the sound is higher because the player is not logged in</t>
+  </si>
+  <si>
+    <t>Visual cue for the temporary power-up (little bar that indicates when it will stop)</t>
+  </si>
+  <si>
+    <t>When different enemies are packed, use the same speed</t>
+  </si>
+  <si>
+    <t>Adapt the spaceship cursor and the power-up stats to the level</t>
+  </si>
+  <si>
+    <t>Produce the layout of the menu</t>
+  </si>
+  <si>
+    <t>Produce the layout of the World 1</t>
   </si>
 </sst>
 </file>
@@ -1670,11 +1688,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D236"/>
+  <dimension ref="A1:D239"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A225" sqref="A225"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,53 +2323,53 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>104</v>
+      <c r="A92" s="8" t="s">
+        <v>399</v>
       </c>
       <c r="B92" s="10"/>
-      <c r="C92" s="16"/>
+      <c r="C92" s="9"/>
       <c r="D92" s="12"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>105</v>
+      <c r="A93" s="8" t="s">
+        <v>400</v>
       </c>
       <c r="B93" s="10"/>
-      <c r="C93" s="16"/>
+      <c r="C93" s="9"/>
       <c r="D93" s="12"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>104</v>
+      </c>
+      <c r="B94" s="10"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="12"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>105</v>
+      </c>
+      <c r="B95" s="10"/>
+      <c r="C95" s="16"/>
+      <c r="D95" s="12"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>109</v>
       </c>
-      <c r="B94" s="10"/>
-      <c r="C94" s="9"/>
-      <c r="D94" s="12"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
+      <c r="B96" s="10"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="12"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="8" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="8" t="s">
         <v>265</v>
-      </c>
-      <c r="B97" s="10"/>
-      <c r="C97" s="9"/>
-      <c r="D97" s="12"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>110</v>
-      </c>
-      <c r="B98" s="10"/>
-      <c r="C98" s="9"/>
-      <c r="D98" s="12"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>308</v>
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="9"/>
@@ -2359,23 +2377,23 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>309</v>
+        <v>110</v>
       </c>
       <c r="B100" s="10"/>
       <c r="C100" s="9"/>
-      <c r="D100" s="9"/>
+      <c r="D100" s="12"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B101" s="10"/>
       <c r="C101" s="9"/>
-      <c r="D101" s="9"/>
+      <c r="D101" s="12"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B102" s="10"/>
       <c r="C102" s="9"/>
@@ -2383,31 +2401,31 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B103" s="10"/>
-      <c r="C103" s="16"/>
-      <c r="D103" s="16"/>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B104" s="10"/>
-      <c r="C104" s="16"/>
-      <c r="D104" s="12"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="9"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="B105" s="10"/>
-      <c r="C105" s="9"/>
+      <c r="C105" s="16"/>
       <c r="D105" s="9"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="B106" s="10"/>
       <c r="C106" s="16"/>
@@ -2415,71 +2433,71 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B107" s="10"/>
       <c r="C107" s="9"/>
-      <c r="D107" s="12"/>
+      <c r="D107" s="9"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B108" s="10"/>
       <c r="C108" s="16"/>
-      <c r="D108" s="12"/>
+      <c r="D108" s="16"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="B109" s="10"/>
-      <c r="C109" s="12"/>
+      <c r="C109" s="9"/>
       <c r="D109" s="12"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="B110" s="10"/>
-      <c r="C110" s="12"/>
+      <c r="C110" s="16"/>
       <c r="D110" s="12"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B111" s="10"/>
-      <c r="C111" s="16"/>
-      <c r="D111" s="12"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="16"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B112" s="10"/>
-      <c r="C112" s="16"/>
+      <c r="C112" s="12"/>
       <c r="D112" s="12"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>107</v>
-      </c>
-      <c r="B113" s="14"/>
-      <c r="C113" s="17"/>
-      <c r="D113" s="12"/>
+        <v>316</v>
+      </c>
+      <c r="B113" s="10"/>
+      <c r="C113" s="16"/>
+      <c r="D113" s="9"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>318</v>
-      </c>
-      <c r="B114" s="14"/>
-      <c r="C114" s="17"/>
+        <v>317</v>
+      </c>
+      <c r="B114" s="10"/>
+      <c r="C114" s="16"/>
       <c r="D114" s="12"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B115" s="14"/>
       <c r="C115" s="17"/>
@@ -2487,7 +2505,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B116" s="14"/>
       <c r="C116" s="17"/>
@@ -2495,7 +2513,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>320</v>
+        <v>108</v>
       </c>
       <c r="B117" s="14"/>
       <c r="C117" s="17"/>
@@ -2503,41 +2521,41 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B118" s="14"/>
       <c r="C118" s="17"/>
       <c r="D118" s="12"/>
     </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>320</v>
+      </c>
+      <c r="B119" s="14"/>
+      <c r="C119" s="17"/>
+      <c r="D119" s="12"/>
+    </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+      <c r="A120" t="s">
+        <v>321</v>
+      </c>
+      <c r="B120" s="14"/>
+      <c r="C120" s="17"/>
+      <c r="D120" s="12"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>67</v>
-      </c>
-      <c r="B122" s="15"/>
-      <c r="C122" s="9"/>
-      <c r="D122" s="12"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>68</v>
-      </c>
-      <c r="B123" s="15"/>
-      <c r="C123" s="12"/>
-      <c r="D123" s="12"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B124" s="15"/>
       <c r="C124" s="9"/>
@@ -2545,15 +2563,15 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B125" s="15"/>
-      <c r="C125" s="16"/>
+      <c r="C125" s="12"/>
       <c r="D125" s="12"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B126" s="15"/>
       <c r="C126" s="9"/>
@@ -2561,31 +2579,31 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B127" s="15"/>
-      <c r="C127" s="12"/>
+      <c r="C127" s="16"/>
       <c r="D127" s="12"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B128" s="15"/>
-      <c r="C128" s="12"/>
+      <c r="C128" s="9"/>
       <c r="D128" s="12"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>177</v>
+        <v>72</v>
       </c>
       <c r="B129" s="15"/>
-      <c r="C129" s="9"/>
+      <c r="C129" s="12"/>
       <c r="D129" s="12"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B130" s="15"/>
       <c r="C130" s="12"/>
@@ -2593,31 +2611,31 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="B131" s="15"/>
-      <c r="C131" s="16"/>
+      <c r="C131" s="9"/>
       <c r="D131" s="12"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B132" s="15"/>
-      <c r="C132" s="9"/>
+      <c r="C132" s="12"/>
       <c r="D132" s="12"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B133" s="15"/>
-      <c r="C133" s="9"/>
+      <c r="C133" s="16"/>
       <c r="D133" s="12"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B134" s="15"/>
       <c r="C134" s="9"/>
@@ -2625,52 +2643,52 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
+        <v>76</v>
+      </c>
+      <c r="B135" s="15"/>
+      <c r="C135" s="9"/>
+      <c r="D135" s="12"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>78</v>
+      </c>
+      <c r="B136" s="15"/>
+      <c r="C136" s="9"/>
+      <c r="D136" s="12"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>79</v>
       </c>
-      <c r="B135" s="15"/>
-      <c r="C135" s="16"/>
-      <c r="D135" s="9"/>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
+      <c r="B137" s="15"/>
+      <c r="C137" s="16"/>
+      <c r="D137" s="9"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>84</v>
-      </c>
-      <c r="B138" s="14"/>
-      <c r="C138" s="16"/>
-      <c r="D138" s="12"/>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>85</v>
-      </c>
-      <c r="B139" s="14"/>
-      <c r="C139" s="12"/>
-      <c r="D139" s="12"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>298</v>
+        <v>84</v>
       </c>
       <c r="B140" s="14"/>
-      <c r="C140" s="9"/>
+      <c r="C140" s="16"/>
       <c r="D140" s="12"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B141" s="14"/>
-      <c r="C141" s="16"/>
+      <c r="C141" s="12"/>
       <c r="D141" s="12"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>87</v>
+        <v>298</v>
       </c>
       <c r="B142" s="14"/>
       <c r="C142" s="9"/>
@@ -2678,23 +2696,23 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>88</v>
-      </c>
-      <c r="B143" s="11"/>
+        <v>86</v>
+      </c>
+      <c r="B143" s="14"/>
       <c r="C143" s="16"/>
       <c r="D143" s="12"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>117</v>
-      </c>
-      <c r="B144" s="11"/>
+        <v>87</v>
+      </c>
+      <c r="B144" s="14"/>
       <c r="C144" s="9"/>
       <c r="D144" s="12"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="B145" s="11"/>
       <c r="C145" s="16"/>
@@ -2702,7 +2720,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="B146" s="11"/>
       <c r="C146" s="9"/>
@@ -2710,105 +2728,105 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="B147" s="11"/>
-      <c r="C147" s="9"/>
+      <c r="C147" s="16"/>
       <c r="D147" s="12"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>215</v>
-      </c>
-      <c r="B148" s="14"/>
+        <v>89</v>
+      </c>
+      <c r="B148" s="11"/>
       <c r="C148" s="9"/>
       <c r="D148" s="12"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>216</v>
-      </c>
-      <c r="B149" s="14"/>
+        <v>90</v>
+      </c>
+      <c r="B149" s="11"/>
       <c r="C149" s="9"/>
       <c r="D149" s="12"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>217</v>
-      </c>
-      <c r="B150" s="15"/>
+        <v>215</v>
+      </c>
+      <c r="B150" s="14"/>
       <c r="C150" s="9"/>
       <c r="D150" s="12"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>218</v>
-      </c>
-      <c r="B151" s="10"/>
+        <v>216</v>
+      </c>
+      <c r="B151" s="14"/>
       <c r="C151" s="9"/>
       <c r="D151" s="12"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>228</v>
-      </c>
-      <c r="B152" s="10"/>
+        <v>217</v>
+      </c>
+      <c r="B152" s="15"/>
       <c r="C152" s="9"/>
       <c r="D152" s="12"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>253</v>
-      </c>
-      <c r="B153" s="14"/>
-      <c r="C153" s="12"/>
+        <v>218</v>
+      </c>
+      <c r="B153" s="10"/>
+      <c r="C153" s="9"/>
       <c r="D153" s="12"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>228</v>
+      </c>
+      <c r="B154" s="10"/>
+      <c r="C154" s="9"/>
+      <c r="D154" s="12"/>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>253</v>
+      </c>
+      <c r="B155" s="14"/>
+      <c r="C155" s="12"/>
+      <c r="D155" s="12"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>254</v>
       </c>
-      <c r="B154" s="14"/>
-      <c r="C154" s="12"/>
-      <c r="D154" s="12"/>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="s">
+      <c r="B156" s="14"/>
+      <c r="C156" s="12"/>
+      <c r="D156" s="12"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="5" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="8" t="s">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="B158" s="10"/>
-      <c r="C158" s="16"/>
-      <c r="D158" s="12"/>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="8" t="s">
+      <c r="B160" s="10"/>
+      <c r="C160" s="16"/>
+      <c r="D160" s="12"/>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="8" t="s">
         <v>299</v>
-      </c>
-      <c r="B159" s="15"/>
-      <c r="C159" s="12"/>
-      <c r="D159" s="12"/>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>300</v>
-      </c>
-      <c r="B160" s="15"/>
-      <c r="C160" s="12"/>
-      <c r="D160" s="12"/>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>301</v>
       </c>
       <c r="B161" s="15"/>
       <c r="C161" s="12"/>
@@ -2816,7 +2834,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B162" s="15"/>
       <c r="C162" s="12"/>
@@ -2824,23 +2842,23 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>171</v>
-      </c>
-      <c r="B163" s="11"/>
-      <c r="C163" s="16"/>
+        <v>301</v>
+      </c>
+      <c r="B163" s="15"/>
+      <c r="C163" s="12"/>
       <c r="D163" s="12"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>174</v>
-      </c>
-      <c r="B164" s="11"/>
-      <c r="C164" s="16"/>
+        <v>302</v>
+      </c>
+      <c r="B164" s="15"/>
+      <c r="C164" s="12"/>
       <c r="D164" s="12"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B165" s="11"/>
       <c r="C165" s="16"/>
@@ -2848,7 +2866,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B166" s="11"/>
       <c r="C166" s="16"/>
@@ -2856,60 +2874,60 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>303</v>
+        <v>172</v>
       </c>
       <c r="B167" s="11"/>
       <c r="C167" s="16"/>
       <c r="D167" s="12"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B168"/>
+      <c r="A168" t="s">
+        <v>173</v>
+      </c>
+      <c r="B168" s="11"/>
+      <c r="C168" s="16"/>
+      <c r="D168" s="12"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>303</v>
+      </c>
+      <c r="B169" s="11"/>
+      <c r="C169" s="16"/>
+      <c r="D169" s="12"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="2" t="s">
+      <c r="B170"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="5" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="5" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>92</v>
-      </c>
-      <c r="B172" s="10"/>
-      <c r="C172" s="16"/>
-      <c r="D172" s="12"/>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>94</v>
-      </c>
-      <c r="B173" s="15"/>
-      <c r="C173" s="9"/>
-      <c r="D173" s="12"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B174" s="10"/>
-      <c r="C174" s="9"/>
+      <c r="C174" s="16"/>
       <c r="D174" s="12"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>96</v>
-      </c>
-      <c r="B175" s="10"/>
+        <v>94</v>
+      </c>
+      <c r="B175" s="15"/>
       <c r="C175" s="9"/>
       <c r="D175" s="12"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B176" s="10"/>
       <c r="C176" s="9"/>
@@ -2917,7 +2935,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B177" s="10"/>
       <c r="C177" s="9"/>
@@ -2925,7 +2943,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B178" s="10"/>
       <c r="C178" s="9"/>
@@ -2933,7 +2951,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B179" s="10"/>
       <c r="C179" s="9"/>
@@ -2941,7 +2959,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B180" s="10"/>
       <c r="C180" s="9"/>
@@ -2949,95 +2967,95 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B181" s="10"/>
-      <c r="C181" s="16"/>
-      <c r="D181" s="16"/>
+      <c r="C181" s="9"/>
+      <c r="D181" s="12"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B182" s="10"/>
-      <c r="C182" s="16"/>
+      <c r="C182" s="9"/>
       <c r="D182" s="12"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B183" s="10"/>
-      <c r="C183" s="9"/>
-      <c r="D183" s="12"/>
+      <c r="C183" s="16"/>
+      <c r="D183" s="16"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B184" s="10"/>
-      <c r="C184" s="9"/>
+      <c r="C184" s="16"/>
       <c r="D184" s="12"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>178</v>
+        <v>112</v>
       </c>
       <c r="B185" s="10"/>
       <c r="C185" s="9"/>
-      <c r="D185" s="9"/>
+      <c r="D185" s="12"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>180</v>
+        <v>113</v>
       </c>
       <c r="B186" s="10"/>
-      <c r="C186" s="16"/>
+      <c r="C186" s="9"/>
       <c r="D186" s="12"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B187" s="10"/>
-      <c r="C187" s="16"/>
+      <c r="C187" s="9"/>
       <c r="D187" s="9"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>214</v>
-      </c>
-      <c r="B188" s="15"/>
-      <c r="C188" s="9"/>
+        <v>180</v>
+      </c>
+      <c r="B188" s="10"/>
+      <c r="C188" s="16"/>
       <c r="D188" s="12"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>241</v>
+        <v>183</v>
       </c>
       <c r="B189" s="10"/>
       <c r="C189" s="16"/>
-      <c r="D189" s="12"/>
+      <c r="D189" s="9"/>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>268</v>
-      </c>
-      <c r="B190" s="10"/>
-      <c r="C190" s="12"/>
+        <v>214</v>
+      </c>
+      <c r="B190" s="15"/>
+      <c r="C190" s="9"/>
       <c r="D190" s="12"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
       <c r="B191" s="10"/>
       <c r="C191" s="16"/>
-      <c r="D191" s="16"/>
+      <c r="D191" s="12"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B192" s="10"/>
       <c r="C192" s="12"/>
@@ -3045,176 +3063,176 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>277</v>
-      </c>
-      <c r="B193" s="15"/>
+        <v>269</v>
+      </c>
+      <c r="B193" s="10"/>
       <c r="C193" s="16"/>
-      <c r="D193" s="12"/>
+      <c r="D193" s="16"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>294</v>
-      </c>
-      <c r="B194" s="15"/>
+        <v>273</v>
+      </c>
+      <c r="B194" s="10"/>
       <c r="C194" s="12"/>
       <c r="D194" s="12"/>
     </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>277</v>
+      </c>
+      <c r="B195" s="15"/>
+      <c r="C195" s="16"/>
+      <c r="D195" s="12"/>
+    </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="2" t="s">
+      <c r="A196" t="s">
+        <v>294</v>
+      </c>
+      <c r="B196" s="15"/>
+      <c r="C196" s="12"/>
+      <c r="D196" s="12"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="5" t="s">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
         <v>124</v>
       </c>
-      <c r="B198" s="11"/>
-      <c r="C198" s="16"/>
-      <c r="D198" s="12"/>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+      <c r="B200" s="11"/>
+      <c r="C200" s="16"/>
+      <c r="D200" s="12"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
         <v>242</v>
       </c>
-      <c r="B199" s="11"/>
-      <c r="C199" s="9"/>
-      <c r="D199" s="12"/>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="2" t="s">
+      <c r="B201" s="11"/>
+      <c r="C201" s="9"/>
+      <c r="D201" s="12"/>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
         <v>129</v>
       </c>
-      <c r="B203" s="11"/>
-      <c r="C203" s="9"/>
-      <c r="D203" s="12"/>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="2" t="s">
+      <c r="B205" s="11"/>
+      <c r="C205" s="9"/>
+      <c r="D205" s="12"/>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>270</v>
-      </c>
-      <c r="B206" s="10"/>
-      <c r="C206" s="16"/>
-      <c r="D206" s="12"/>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>271</v>
-      </c>
-      <c r="B207" s="10"/>
-      <c r="C207" s="16"/>
-      <c r="D207" s="12"/>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B208" s="10"/>
       <c r="C208" s="16"/>
       <c r="D208" s="12"/>
     </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>271</v>
+      </c>
+      <c r="B209" s="10"/>
+      <c r="C209" s="16"/>
+      <c r="D209" s="12"/>
+    </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="2" t="s">
+      <c r="A210" t="s">
+        <v>272</v>
+      </c>
+      <c r="B210" s="10"/>
+      <c r="C210" s="16"/>
+      <c r="D210" s="12"/>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>133</v>
-      </c>
-      <c r="B211" s="17"/>
-      <c r="C211" s="9"/>
-      <c r="D211" s="12"/>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>179</v>
-      </c>
-      <c r="B212" s="10"/>
-      <c r="C212" s="9"/>
-      <c r="D212" s="12"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>181</v>
-      </c>
-      <c r="B213" s="10"/>
+        <v>133</v>
+      </c>
+      <c r="B213" s="17"/>
       <c r="C213" s="9"/>
       <c r="D213" s="12"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B214" s="10"/>
-      <c r="C214" s="16"/>
+      <c r="C214" s="9"/>
       <c r="D214" s="12"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="B215" s="10"/>
-      <c r="C215" s="16"/>
+      <c r="C215" s="9"/>
       <c r="D215" s="12"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>239</v>
-      </c>
-      <c r="B216" s="11"/>
-      <c r="C216" s="12"/>
+        <v>182</v>
+      </c>
+      <c r="B216" s="10"/>
+      <c r="C216" s="16"/>
       <c r="D216" s="12"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>240</v>
-      </c>
-      <c r="B217" s="11"/>
-      <c r="C217" s="12"/>
+        <v>203</v>
+      </c>
+      <c r="B217" s="10"/>
+      <c r="C217" s="16"/>
       <c r="D217" s="12"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B218" s="11"/>
-      <c r="C218" s="16"/>
+      <c r="C218" s="12"/>
       <c r="D218" s="12"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>275</v>
-      </c>
-      <c r="B219" s="10"/>
-      <c r="C219" s="9"/>
-      <c r="D219" s="9"/>
+        <v>240</v>
+      </c>
+      <c r="B219" s="11"/>
+      <c r="C219" s="12"/>
+      <c r="D219" s="12"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>278</v>
-      </c>
-      <c r="B220" s="10"/>
-      <c r="C220" s="9"/>
-      <c r="D220" s="9"/>
+        <v>243</v>
+      </c>
+      <c r="B220" s="11"/>
+      <c r="C220" s="16"/>
+      <c r="D220" s="12"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="B221" s="10"/>
       <c r="C221" s="9"/>
@@ -3222,60 +3240,58 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>286</v>
-      </c>
-      <c r="B222" s="12"/>
-      <c r="C222" s="12"/>
-      <c r="D222" s="12"/>
+        <v>278</v>
+      </c>
+      <c r="B222" s="10"/>
+      <c r="C222" s="9"/>
+      <c r="D222" s="9"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>293</v>
-      </c>
-      <c r="B223" s="12"/>
-      <c r="C223" s="12"/>
-      <c r="D223" s="12"/>
+        <v>284</v>
+      </c>
+      <c r="B223" s="10"/>
+      <c r="C223" s="9"/>
+      <c r="D223" s="9"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
+        <v>286</v>
+      </c>
+      <c r="B224" s="12"/>
+      <c r="C224" s="12"/>
+      <c r="D224" s="12"/>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>293</v>
+      </c>
+      <c r="B225" s="12"/>
+      <c r="C225" s="12"/>
+      <c r="D225" s="12"/>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
         <v>390</v>
       </c>
-      <c r="B224" s="12"/>
-      <c r="C224" s="16"/>
-      <c r="D224" s="12"/>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A226" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="B226" s="12"/>
+      <c r="C226" s="16"/>
+      <c r="D226" s="12"/>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>22</v>
-      </c>
-      <c r="B227" s="14"/>
-      <c r="C227" s="17"/>
-      <c r="D227" s="12"/>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
-        <v>11</v>
-      </c>
-      <c r="B228" s="14"/>
-      <c r="C228" s="17"/>
-      <c r="D228" s="12"/>
+        <v>395</v>
+      </c>
+      <c r="B227"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>12</v>
-      </c>
-      <c r="B229" s="14"/>
-      <c r="C229" s="17"/>
-      <c r="D229" s="12"/>
+      <c r="A229" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B230" s="14"/>
       <c r="C230" s="17"/>
@@ -3283,7 +3299,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B231" s="14"/>
       <c r="C231" s="17"/>
@@ -3291,7 +3307,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B232" s="14"/>
       <c r="C232" s="17"/>
@@ -3299,24 +3315,48 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B233" s="14"/>
       <c r="C233" s="17"/>
       <c r="D233" s="12"/>
     </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>14</v>
+      </c>
+      <c r="B234" s="14"/>
+      <c r="C234" s="17"/>
+      <c r="D234" s="12"/>
+    </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="2" t="s">
-        <v>145</v>
-      </c>
+      <c r="A235" t="s">
+        <v>23</v>
+      </c>
+      <c r="B235" s="14"/>
+      <c r="C235" s="17"/>
+      <c r="D235" s="12"/>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
+        <v>24</v>
+      </c>
+      <c r="B236" s="14"/>
+      <c r="C236" s="17"/>
+      <c r="D236" s="12"/>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
         <v>149</v>
       </c>
-      <c r="B236" s="11"/>
-      <c r="C236" s="16"/>
-      <c r="D236" s="9"/>
+      <c r="B239" s="11"/>
+      <c r="C239" s="16"/>
+      <c r="D239" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3357,10 +3397,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A98"/>
+  <dimension ref="A1:A101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3453,333 +3493,348 @@
         <v>306</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>397</v>
+      </c>
+    </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>341</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>369</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>229</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>249</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>8</v>
+      <c r="A48" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>125</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>205</v>
+        <v>125</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>206</v>
+      <c r="A58" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>274</v>
+        <v>210</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>292</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>371</v>
+        <v>212</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>374</v>
+        <v>274</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>370</v>
+        <v>292</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>375</v>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>184</v>
+      <c r="A72" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>185</v>
+        <v>375</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>15</v>
+        <v>184</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>247</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>259</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>144</v>
+        <v>261</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>127</v>
+        <v>307</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>131</v>
+      <c r="A90" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>285</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>338</v>
+      <c r="A93" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>339</v>
+        <v>285</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>337</v>
       </c>
     </row>

</xml_diff>

<commit_message>
First version of Main Menu "new game" menu
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="19050" windowHeight="8625"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="19050" windowHeight="8625" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="402">
   <si>
     <t>Tweaking System</t>
   </si>
@@ -1224,6 +1224,9 @@
   </si>
   <si>
     <t>Produce the layout of the World 1</t>
+  </si>
+  <si>
+    <t>Add bullets fired in the score</t>
   </si>
 </sst>
 </file>
@@ -1690,7 +1693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D239"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
     </sheetView>
@@ -3397,10 +3400,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A101"/>
+  <dimension ref="A1:A102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3503,338 +3506,343 @@
         <v>398</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>186</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>341</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>369</v>
+        <v>341</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>394</v>
+        <v>369</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>250</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>225</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>274</v>
+        <v>212</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>371</v>
+        <v>292</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>257</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>340</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>337</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Before messing up with turret input.
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="19050" windowHeight="8625" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="19050" windowHeight="8625"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="408">
   <si>
     <t>Tweaking System</t>
   </si>
@@ -1227,6 +1227,24 @@
   </si>
   <si>
     <t>Add bullets fired in the score</t>
+  </si>
+  <si>
+    <t>A level where sounds are made with the mouth</t>
+  </si>
+  <si>
+    <t>Helpbar fucked</t>
+  </si>
+  <si>
+    <t>Contextual menus size fucked</t>
+  </si>
+  <si>
+    <t>To classify</t>
+  </si>
+  <si>
+    <t>The 3-stars should be associated to the player score, not the highscores</t>
+  </si>
+  <si>
+    <t>Game paused The resistance fucked</t>
   </si>
 </sst>
 </file>
@@ -1691,11 +1709,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D239"/>
+  <dimension ref="A1:D242"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A230" sqref="A230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3285,40 +3303,42 @@
       <c r="A227" t="s">
         <v>395</v>
       </c>
-      <c r="B227"/>
+      <c r="B227" s="12"/>
+      <c r="C227" s="16"/>
+      <c r="D227" s="9"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>403</v>
+      </c>
+      <c r="B228" s="12"/>
+      <c r="C228" s="9"/>
+      <c r="D228" s="12"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A229" t="s">
+        <v>404</v>
+      </c>
+      <c r="B229" s="12"/>
+      <c r="C229" s="9"/>
+      <c r="D229" s="12"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>22</v>
-      </c>
-      <c r="B230" s="14"/>
-      <c r="C230" s="17"/>
+        <v>407</v>
+      </c>
+      <c r="B230" s="12"/>
+      <c r="C230" s="9"/>
       <c r="D230" s="12"/>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>11</v>
-      </c>
-      <c r="B231" s="14"/>
-      <c r="C231" s="17"/>
-      <c r="D231" s="12"/>
-    </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>12</v>
-      </c>
-      <c r="B232" s="14"/>
-      <c r="C232" s="17"/>
-      <c r="D232" s="12"/>
+      <c r="A232" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B233" s="14"/>
       <c r="C233" s="17"/>
@@ -3326,7 +3346,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B234" s="14"/>
       <c r="C234" s="17"/>
@@ -3334,7 +3354,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B235" s="14"/>
       <c r="C235" s="17"/>
@@ -3342,24 +3362,48 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B236" s="14"/>
       <c r="C236" s="17"/>
       <c r="D236" s="12"/>
     </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>14</v>
+      </c>
+      <c r="B237" s="14"/>
+      <c r="C237" s="17"/>
+      <c r="D237" s="12"/>
+    </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="2" t="s">
-        <v>145</v>
-      </c>
+      <c r="A238" t="s">
+        <v>23</v>
+      </c>
+      <c r="B238" s="14"/>
+      <c r="C238" s="17"/>
+      <c r="D238" s="12"/>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
+        <v>24</v>
+      </c>
+      <c r="B239" s="14"/>
+      <c r="C239" s="17"/>
+      <c r="D239" s="12"/>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
         <v>149</v>
       </c>
-      <c r="B239" s="11"/>
-      <c r="C239" s="16"/>
-      <c r="D239" s="9"/>
+      <c r="B242" s="11"/>
+      <c r="C242" s="16"/>
+      <c r="D242" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3400,10 +3444,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A102"/>
+  <dimension ref="A1:A107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3546,304 +3590,319 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>186</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>341</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>369</v>
+        <v>341</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>394</v>
+        <v>369</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>250</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>225</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>274</v>
+        <v>212</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>371</v>
+        <v>292</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>337</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Organized assets in progress
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="19050" windowHeight="8625"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="19050" windowHeight="8625" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="410">
   <si>
     <t>Tweaking System</t>
   </si>
@@ -1245,13 +1245,19 @@
   </si>
   <si>
     <t>Game paused The resistance fucked</t>
+  </si>
+  <si>
+    <t>When updating a turret, the Help Bar Message is not displayed</t>
+  </si>
+  <si>
+    <t> STScI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1313,6 +1319,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1359,7 +1371,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1403,6 +1415,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent2" xfId="2" builtinId="33"/>
@@ -1709,11 +1722,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D242"/>
+  <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A230" sqref="A230"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1914,7 +1927,9 @@
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="16"/>
-      <c r="D28" s="12"/>
+      <c r="D28" s="11" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1922,7 +1937,9 @@
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="16"/>
-      <c r="D29" s="12"/>
+      <c r="D29" s="11" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1930,7 +1947,7 @@
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="16"/>
-      <c r="D30" s="12"/>
+      <c r="D30" s="16"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -2031,7 +2048,9 @@
       </c>
       <c r="B44" s="14"/>
       <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
+      <c r="D44" s="11" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
@@ -2349,7 +2368,7 @@
       </c>
       <c r="B92" s="10"/>
       <c r="C92" s="9"/>
-      <c r="D92" s="12"/>
+      <c r="D92" s="9"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
@@ -2394,7 +2413,7 @@
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="9"/>
-      <c r="D99" s="12"/>
+      <c r="D99" s="9"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
@@ -2402,7 +2421,7 @@
       </c>
       <c r="B100" s="10"/>
       <c r="C100" s="9"/>
-      <c r="D100" s="12"/>
+      <c r="D100" s="9"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
@@ -2936,7 +2955,7 @@
       </c>
       <c r="B174" s="10"/>
       <c r="C174" s="16"/>
-      <c r="D174" s="12"/>
+      <c r="D174" s="9"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
@@ -2952,7 +2971,7 @@
       </c>
       <c r="B176" s="10"/>
       <c r="C176" s="9"/>
-      <c r="D176" s="12"/>
+      <c r="D176" s="16"/>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
@@ -2960,7 +2979,7 @@
       </c>
       <c r="B177" s="10"/>
       <c r="C177" s="9"/>
-      <c r="D177" s="12"/>
+      <c r="D177" s="9"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
@@ -2992,7 +3011,7 @@
       </c>
       <c r="B181" s="10"/>
       <c r="C181" s="9"/>
-      <c r="D181" s="12"/>
+      <c r="D181" s="9"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
@@ -3000,7 +3019,7 @@
       </c>
       <c r="B182" s="10"/>
       <c r="C182" s="9"/>
-      <c r="D182" s="12"/>
+      <c r="D182" s="9"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
@@ -3016,7 +3035,7 @@
       </c>
       <c r="B184" s="10"/>
       <c r="C184" s="16"/>
-      <c r="D184" s="12"/>
+      <c r="D184" s="9"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
@@ -3032,7 +3051,7 @@
       </c>
       <c r="B186" s="10"/>
       <c r="C186" s="9"/>
-      <c r="D186" s="12"/>
+      <c r="D186" s="16"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
@@ -3048,7 +3067,7 @@
       </c>
       <c r="B188" s="10"/>
       <c r="C188" s="16"/>
-      <c r="D188" s="12"/>
+      <c r="D188" s="9"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
@@ -3245,15 +3264,15 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>243</v>
-      </c>
-      <c r="B220" s="11"/>
+        <v>408</v>
+      </c>
+      <c r="B220" s="10"/>
       <c r="C220" s="16"/>
       <c r="D220" s="12"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="B221" s="10"/>
       <c r="C221" s="9"/>
@@ -3261,7 +3280,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B222" s="10"/>
       <c r="C222" s="9"/>
@@ -3269,7 +3288,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B223" s="10"/>
       <c r="C223" s="9"/>
@@ -3277,15 +3296,15 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B224" s="12"/>
       <c r="C224" s="12"/>
-      <c r="D224" s="12"/>
+      <c r="D224" s="9"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B225" s="12"/>
       <c r="C225" s="12"/>
@@ -3293,7 +3312,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>390</v>
+        <v>293</v>
       </c>
       <c r="B226" s="12"/>
       <c r="C226" s="16"/>
@@ -3301,7 +3320,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="B227" s="12"/>
       <c r="C227" s="16"/>
@@ -3309,36 +3328,39 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B228" s="12"/>
       <c r="C228" s="9"/>
-      <c r="D228" s="12"/>
+      <c r="D228" s="9"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B229" s="12"/>
       <c r="C229" s="9"/>
-      <c r="D229" s="12"/>
+      <c r="D229" s="9"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B230" s="12"/>
       <c r="C230" s="9"/>
       <c r="D230" s="12"/>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="2" t="s">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>407</v>
+      </c>
+      <c r="B231" s="12"/>
+      <c r="C231" s="9"/>
+      <c r="D231" s="12"/>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>22</v>
       </c>
       <c r="B233" s="14"/>
       <c r="C233" s="17"/>
@@ -3346,7 +3368,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B234" s="14"/>
       <c r="C234" s="17"/>
@@ -3354,7 +3376,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B235" s="14"/>
       <c r="C235" s="17"/>
@@ -3362,7 +3384,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B236" s="14"/>
       <c r="C236" s="17"/>
@@ -3370,7 +3392,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B237" s="14"/>
       <c r="C237" s="17"/>
@@ -3378,7 +3400,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B238" s="14"/>
       <c r="C238" s="17"/>
@@ -3386,24 +3408,29 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B239" s="14"/>
       <c r="C239" s="17"/>
       <c r="D239" s="12"/>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="2" t="s">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
         <v>149</v>
       </c>
-      <c r="B242" s="11"/>
-      <c r="C242" s="16"/>
-      <c r="D242" s="9"/>
+      <c r="B243" s="11"/>
+      <c r="C243" s="16"/>
+      <c r="D243" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4332,10 +4359,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4390,6 +4417,17 @@
       </c>
       <c r="D4" t="s">
         <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="C5" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added World 2 (which suck right now)
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="19050" windowHeight="8625" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="19050" windowHeight="8625"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="415">
   <si>
     <t>Tweaking System</t>
   </si>
@@ -335,12 +335,6 @@
     <t>Worlds</t>
   </si>
   <si>
-    <t>Produce the layout of the 8 worlds</t>
-  </si>
-  <si>
-    <t>Tweak the layout of the 8 worlds</t>
-  </si>
-  <si>
     <t>Cutscenes</t>
   </si>
   <si>
@@ -1121,9 +1115,6 @@
     <t>Sprint #1</t>
   </si>
   <si>
-    <t>Find all the gameplay elements of your game</t>
-  </si>
-  <si>
     <t>Mentors gave me really good advice =&gt; more job, feel like I'm more planning than doing</t>
   </si>
   <si>
@@ -1251,6 +1242,30 @@
   </si>
   <si>
     <t> STScI</t>
+  </si>
+  <si>
+    <t>Visual cue for temporary spaceship addon (depleting bar)</t>
+  </si>
+  <si>
+    <t>Rotate the planets =&gt; rotate the turrets</t>
+  </si>
+  <si>
+    <t>Produce the layout of the World 2</t>
+  </si>
+  <si>
+    <t>Produce the layout of the World 3</t>
+  </si>
+  <si>
+    <t>Produce the layout of the 5 worlds</t>
+  </si>
+  <si>
+    <t>Tweak the layout of the 5 worlds</t>
+  </si>
+  <si>
+    <t>Finish the intro cutscene</t>
+  </si>
+  <si>
+    <t>Polish the intro cutscene</t>
   </si>
 </sst>
 </file>
@@ -1722,11 +1737,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D243"/>
+  <dimension ref="A1:D247"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F196" sqref="F196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,35 +1754,35 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B2" s="2"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="12"/>
@@ -1858,7 +1873,7 @@
       <c r="B17" s="10"/>
       <c r="C17" s="12"/>
       <c r="D17" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1876,12 +1891,12 @@
       <c r="B19" s="10"/>
       <c r="C19" s="9"/>
       <c r="D19" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="9"/>
@@ -1889,7 +1904,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="16"/>
@@ -1897,7 +1912,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="16"/>
@@ -1905,12 +1920,12 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="16"/>
@@ -1918,7 +1933,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1928,7 +1943,7 @@
       <c r="B28" s="11"/>
       <c r="C28" s="16"/>
       <c r="D28" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1938,12 +1953,12 @@
       <c r="B29" s="11"/>
       <c r="C29" s="16"/>
       <c r="D29" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="16"/>
@@ -1951,7 +1966,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="9"/>
@@ -1959,7 +1974,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="16"/>
@@ -1967,7 +1982,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="16"/>
@@ -1975,7 +1990,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="9"/>
@@ -2004,7 +2019,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="9"/>
@@ -2049,7 +2064,7 @@
       <c r="B44" s="14"/>
       <c r="C44" s="12"/>
       <c r="D44" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2088,7 +2103,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B52" s="14"/>
       <c r="C52" s="9"/>
@@ -2096,7 +2111,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B53" s="10"/>
       <c r="C53" s="16"/>
@@ -2214,7 +2229,9 @@
       </c>
       <c r="B70" s="14"/>
       <c r="C70" s="17"/>
-      <c r="D70" s="12"/>
+      <c r="D70" s="11" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -2222,7 +2239,9 @@
       </c>
       <c r="B71" s="14"/>
       <c r="C71" s="17"/>
-      <c r="D71" s="12"/>
+      <c r="D71" s="11" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
@@ -2230,7 +2249,9 @@
       </c>
       <c r="B72" s="14"/>
       <c r="C72" s="17"/>
-      <c r="D72" s="12"/>
+      <c r="D72" s="11" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
@@ -2238,7 +2259,9 @@
       </c>
       <c r="B73" s="14"/>
       <c r="C73" s="17"/>
-      <c r="D73" s="12"/>
+      <c r="D73" s="11" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
@@ -2246,7 +2269,9 @@
       </c>
       <c r="B74" s="14"/>
       <c r="C74" s="17"/>
-      <c r="D74" s="12"/>
+      <c r="D74" s="11" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
@@ -2254,7 +2279,9 @@
       </c>
       <c r="B75" s="14"/>
       <c r="C75" s="17"/>
-      <c r="D75" s="12"/>
+      <c r="D75" s="11" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
@@ -2262,7 +2289,9 @@
       </c>
       <c r="B76" s="14"/>
       <c r="C76" s="17"/>
-      <c r="D76" s="12"/>
+      <c r="D76" s="11" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
@@ -2270,7 +2299,9 @@
       </c>
       <c r="B77" s="14"/>
       <c r="C77" s="17"/>
-      <c r="D77" s="12"/>
+      <c r="D77" s="11" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
@@ -2364,7 +2395,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B92" s="10"/>
       <c r="C92" s="9"/>
@@ -2372,68 +2403,68 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B93" s="10"/>
       <c r="C93" s="9"/>
-      <c r="D93" s="12"/>
+      <c r="D93" s="9"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>104</v>
+      <c r="A94" s="8" t="s">
+        <v>409</v>
       </c>
       <c r="B94" s="10"/>
-      <c r="C94" s="16"/>
+      <c r="C94" s="9"/>
       <c r="D94" s="12"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>105</v>
+      <c r="A95" s="8" t="s">
+        <v>410</v>
       </c>
       <c r="B95" s="10"/>
-      <c r="C95" s="16"/>
+      <c r="C95" s="9"/>
       <c r="D95" s="12"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>109</v>
+        <v>411</v>
       </c>
       <c r="B96" s="10"/>
-      <c r="C96" s="9"/>
+      <c r="C96" s="16"/>
       <c r="D96" s="12"/>
     </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>412</v>
+      </c>
+      <c r="B97" s="10"/>
+      <c r="C97" s="16"/>
+      <c r="D97" s="12"/>
+    </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="B99" s="10"/>
-      <c r="C99" s="9"/>
-      <c r="D99" s="9"/>
+      <c r="A98" t="s">
+        <v>107</v>
+      </c>
+      <c r="B98" s="10"/>
+      <c r="C98" s="9"/>
+      <c r="D98" s="9"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>110</v>
-      </c>
-      <c r="B100" s="10"/>
-      <c r="C100" s="9"/>
-      <c r="D100" s="9"/>
+      <c r="A100" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>308</v>
+      <c r="A101" s="8" t="s">
+        <v>263</v>
       </c>
       <c r="B101" s="10"/>
       <c r="C101" s="9"/>
-      <c r="D101" s="12"/>
+      <c r="D101" s="9"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>309</v>
+        <v>108</v>
       </c>
       <c r="B102" s="10"/>
       <c r="C102" s="9"/>
@@ -2441,15 +2472,15 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B103" s="10"/>
       <c r="C103" s="9"/>
-      <c r="D103" s="9"/>
+      <c r="D103" s="12"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B104" s="10"/>
       <c r="C104" s="9"/>
@@ -2457,103 +2488,103 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B105" s="10"/>
-      <c r="C105" s="16"/>
+      <c r="C105" s="9"/>
       <c r="D105" s="9"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B106" s="10"/>
-      <c r="C106" s="16"/>
-      <c r="D106" s="12"/>
+      <c r="C106" s="9"/>
+      <c r="D106" s="9"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="B107" s="10"/>
-      <c r="C107" s="9"/>
+      <c r="C107" s="16"/>
       <c r="D107" s="9"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="B108" s="10"/>
       <c r="C108" s="16"/>
-      <c r="D108" s="16"/>
+      <c r="D108" s="12"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B109" s="10"/>
       <c r="C109" s="9"/>
-      <c r="D109" s="12"/>
+      <c r="D109" s="9"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B110" s="10"/>
       <c r="C110" s="16"/>
-      <c r="D110" s="12"/>
+      <c r="D110" s="16"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="B111" s="10"/>
-      <c r="C111" s="12"/>
-      <c r="D111" s="16"/>
+      <c r="C111" s="9"/>
+      <c r="D111" s="12"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="B112" s="10"/>
-      <c r="C112" s="12"/>
+      <c r="C112" s="16"/>
       <c r="D112" s="12"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B113" s="10"/>
-      <c r="C113" s="16"/>
-      <c r="D113" s="9"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="16"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B114" s="10"/>
-      <c r="C114" s="16"/>
+      <c r="C114" s="12"/>
       <c r="D114" s="12"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>107</v>
-      </c>
-      <c r="B115" s="14"/>
-      <c r="C115" s="17"/>
-      <c r="D115" s="12"/>
+        <v>314</v>
+      </c>
+      <c r="B115" s="10"/>
+      <c r="C115" s="16"/>
+      <c r="D115" s="9"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>318</v>
-      </c>
-      <c r="B116" s="14"/>
-      <c r="C116" s="17"/>
+        <v>315</v>
+      </c>
+      <c r="B116" s="10"/>
+      <c r="C116" s="16"/>
       <c r="D116" s="12"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B117" s="14"/>
       <c r="C117" s="17"/>
@@ -2561,7 +2592,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B118" s="14"/>
       <c r="C118" s="17"/>
@@ -2569,7 +2600,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>320</v>
+        <v>106</v>
       </c>
       <c r="B119" s="14"/>
       <c r="C119" s="17"/>
@@ -2577,57 +2608,57 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B120" s="14"/>
       <c r="C120" s="17"/>
       <c r="D120" s="12"/>
     </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>318</v>
+      </c>
+      <c r="B121" s="14"/>
+      <c r="C121" s="17"/>
+      <c r="D121" s="12"/>
+    </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="A122" t="s">
+        <v>319</v>
+      </c>
+      <c r="B122" s="14"/>
+      <c r="C122" s="17"/>
+      <c r="D122" s="12"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="5" t="s">
-        <v>156</v>
-      </c>
+      <c r="A123" t="s">
+        <v>413</v>
+      </c>
+      <c r="B123" s="10"/>
+      <c r="C123" s="16"/>
+      <c r="D123" s="12"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>67</v>
-      </c>
-      <c r="B124" s="15"/>
-      <c r="C124" s="9"/>
+        <v>414</v>
+      </c>
+      <c r="B124" s="10"/>
+      <c r="C124" s="16"/>
       <c r="D124" s="12"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>68</v>
-      </c>
-      <c r="B125" s="15"/>
-      <c r="C125" s="12"/>
-      <c r="D125" s="12"/>
-    </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>70</v>
-      </c>
-      <c r="B126" s="15"/>
-      <c r="C126" s="9"/>
-      <c r="D126" s="12"/>
+      <c r="A126" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>69</v>
-      </c>
-      <c r="B127" s="15"/>
-      <c r="C127" s="16"/>
-      <c r="D127" s="12"/>
+      <c r="A127" s="5" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B128" s="15"/>
       <c r="C128" s="9"/>
@@ -2635,7 +2666,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B129" s="15"/>
       <c r="C129" s="12"/>
@@ -2643,47 +2674,47 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B130" s="15"/>
-      <c r="C130" s="12"/>
+      <c r="C130" s="9"/>
       <c r="D130" s="12"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>177</v>
+        <v>69</v>
       </c>
       <c r="B131" s="15"/>
-      <c r="C131" s="9"/>
+      <c r="C131" s="16"/>
       <c r="D131" s="12"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B132" s="15"/>
-      <c r="C132" s="12"/>
+      <c r="C132" s="9"/>
       <c r="D132" s="12"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B133" s="15"/>
-      <c r="C133" s="16"/>
+      <c r="C133" s="12"/>
       <c r="D133" s="12"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B134" s="15"/>
-      <c r="C134" s="9"/>
+      <c r="C134" s="12"/>
       <c r="D134" s="12"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>76</v>
+        <v>175</v>
       </c>
       <c r="B135" s="15"/>
       <c r="C135" s="9"/>
@@ -2691,323 +2722,323 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B136" s="15"/>
-      <c r="C136" s="9"/>
+      <c r="C136" s="12"/>
       <c r="D136" s="12"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B137" s="15"/>
       <c r="C137" s="16"/>
-      <c r="D137" s="9"/>
+      <c r="D137" s="12"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>75</v>
+      </c>
+      <c r="B138" s="15"/>
+      <c r="C138" s="9"/>
+      <c r="D138" s="12"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
-        <v>91</v>
-      </c>
+      <c r="A139" t="s">
+        <v>76</v>
+      </c>
+      <c r="B139" s="15"/>
+      <c r="C139" s="9"/>
+      <c r="D139" s="12"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>84</v>
-      </c>
-      <c r="B140" s="14"/>
-      <c r="C140" s="16"/>
+        <v>78</v>
+      </c>
+      <c r="B140" s="15"/>
+      <c r="C140" s="9"/>
       <c r="D140" s="12"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>85</v>
-      </c>
-      <c r="B141" s="14"/>
-      <c r="C141" s="12"/>
-      <c r="D141" s="12"/>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>298</v>
-      </c>
-      <c r="B142" s="14"/>
-      <c r="C142" s="9"/>
-      <c r="D142" s="12"/>
+        <v>79</v>
+      </c>
+      <c r="B141" s="15"/>
+      <c r="C141" s="16"/>
+      <c r="D141" s="9"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>86</v>
-      </c>
-      <c r="B143" s="14"/>
-      <c r="C143" s="16"/>
-      <c r="D143" s="12"/>
+      <c r="A143" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B144" s="14"/>
-      <c r="C144" s="9"/>
+      <c r="C144" s="16"/>
       <c r="D144" s="12"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>88</v>
-      </c>
-      <c r="B145" s="11"/>
-      <c r="C145" s="16"/>
+        <v>85</v>
+      </c>
+      <c r="B145" s="14"/>
+      <c r="C145" s="12"/>
       <c r="D145" s="12"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>117</v>
-      </c>
-      <c r="B146" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="B146" s="14"/>
       <c r="C146" s="9"/>
       <c r="D146" s="12"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>118</v>
-      </c>
-      <c r="B147" s="11"/>
+        <v>86</v>
+      </c>
+      <c r="B147" s="14"/>
       <c r="C147" s="16"/>
       <c r="D147" s="12"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>89</v>
-      </c>
-      <c r="B148" s="11"/>
+        <v>87</v>
+      </c>
+      <c r="B148" s="14"/>
       <c r="C148" s="9"/>
       <c r="D148" s="12"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B149" s="11"/>
-      <c r="C149" s="9"/>
+      <c r="C149" s="16"/>
       <c r="D149" s="12"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>215</v>
-      </c>
-      <c r="B150" s="14"/>
+        <v>115</v>
+      </c>
+      <c r="B150" s="11"/>
       <c r="C150" s="9"/>
       <c r="D150" s="12"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>216</v>
-      </c>
-      <c r="B151" s="14"/>
-      <c r="C151" s="9"/>
+        <v>116</v>
+      </c>
+      <c r="B151" s="11"/>
+      <c r="C151" s="16"/>
       <c r="D151" s="12"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>217</v>
-      </c>
-      <c r="B152" s="15"/>
+        <v>89</v>
+      </c>
+      <c r="B152" s="11"/>
       <c r="C152" s="9"/>
       <c r="D152" s="12"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>218</v>
-      </c>
-      <c r="B153" s="10"/>
+        <v>90</v>
+      </c>
+      <c r="B153" s="11"/>
       <c r="C153" s="9"/>
       <c r="D153" s="12"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>228</v>
-      </c>
-      <c r="B154" s="10"/>
+        <v>213</v>
+      </c>
+      <c r="B154" s="14"/>
       <c r="C154" s="9"/>
       <c r="D154" s="12"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>253</v>
+        <v>214</v>
       </c>
       <c r="B155" s="14"/>
-      <c r="C155" s="12"/>
+      <c r="C155" s="9"/>
       <c r="D155" s="12"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>254</v>
-      </c>
-      <c r="B156" s="14"/>
-      <c r="C156" s="12"/>
+        <v>215</v>
+      </c>
+      <c r="B156" s="15"/>
+      <c r="C156" s="9"/>
       <c r="D156" s="12"/>
     </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>216</v>
+      </c>
+      <c r="B157" s="10"/>
+      <c r="C157" s="9"/>
+      <c r="D157" s="12"/>
+    </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="2" t="s">
-        <v>170</v>
-      </c>
+      <c r="A158" t="s">
+        <v>226</v>
+      </c>
+      <c r="B158" s="10"/>
+      <c r="C158" s="9"/>
+      <c r="D158" s="12"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="5" t="s">
-        <v>266</v>
-      </c>
+      <c r="A159" t="s">
+        <v>251</v>
+      </c>
+      <c r="B159" s="14"/>
+      <c r="C159" s="12"/>
+      <c r="D159" s="12"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="B160" s="10"/>
-      <c r="C160" s="16"/>
+      <c r="A160" t="s">
+        <v>252</v>
+      </c>
+      <c r="B160" s="14"/>
+      <c r="C160" s="12"/>
       <c r="D160" s="12"/>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="B161" s="15"/>
-      <c r="C161" s="12"/>
-      <c r="D161" s="12"/>
-    </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>300</v>
-      </c>
-      <c r="B162" s="15"/>
-      <c r="C162" s="12"/>
-      <c r="D162" s="12"/>
+      <c r="A162" s="2" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>301</v>
-      </c>
-      <c r="B163" s="15"/>
-      <c r="C163" s="12"/>
-      <c r="D163" s="12"/>
+      <c r="A163" s="5" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="A164" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="B164" s="15"/>
-      <c r="C164" s="12"/>
+      <c r="B164" s="10"/>
+      <c r="C164" s="16"/>
       <c r="D164" s="12"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>171</v>
-      </c>
-      <c r="B165" s="11"/>
-      <c r="C165" s="16"/>
+      <c r="A165" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B165" s="15"/>
+      <c r="C165" s="12"/>
       <c r="D165" s="12"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>174</v>
-      </c>
-      <c r="B166" s="11"/>
-      <c r="C166" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="B166" s="15"/>
+      <c r="C166" s="12"/>
       <c r="D166" s="12"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>172</v>
-      </c>
-      <c r="B167" s="11"/>
-      <c r="C167" s="16"/>
+        <v>299</v>
+      </c>
+      <c r="B167" s="15"/>
+      <c r="C167" s="12"/>
       <c r="D167" s="12"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>173</v>
-      </c>
-      <c r="B168" s="11"/>
-      <c r="C168" s="16"/>
+        <v>300</v>
+      </c>
+      <c r="B168" s="15"/>
+      <c r="C168" s="12"/>
       <c r="D168" s="12"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>303</v>
+        <v>169</v>
       </c>
       <c r="B169" s="11"/>
       <c r="C169" s="16"/>
       <c r="D169" s="12"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B170"/>
+      <c r="A170" t="s">
+        <v>172</v>
+      </c>
+      <c r="B170" s="11"/>
+      <c r="C170" s="16"/>
+      <c r="D170" s="12"/>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>170</v>
+      </c>
+      <c r="B171" s="11"/>
+      <c r="C171" s="16"/>
+      <c r="D171" s="12"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="2" t="s">
+      <c r="A172" t="s">
+        <v>171</v>
+      </c>
+      <c r="B172" s="11"/>
+      <c r="C172" s="16"/>
+      <c r="D172" s="12"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>301</v>
+      </c>
+      <c r="B173" s="11"/>
+      <c r="C173" s="16"/>
+      <c r="D173" s="12"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B174"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>92</v>
-      </c>
-      <c r="B174" s="10"/>
-      <c r="C174" s="16"/>
-      <c r="D174" s="9"/>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>94</v>
-      </c>
-      <c r="B175" s="15"/>
-      <c r="C175" s="9"/>
-      <c r="D175" s="12"/>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>95</v>
-      </c>
-      <c r="B176" s="10"/>
-      <c r="C176" s="9"/>
-      <c r="D176" s="16"/>
-    </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>96</v>
-      </c>
-      <c r="B177" s="10"/>
-      <c r="C177" s="9"/>
-      <c r="D177" s="9"/>
+      <c r="A177" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B178" s="10"/>
-      <c r="C178" s="9"/>
-      <c r="D178" s="12"/>
+      <c r="C178" s="16"/>
+      <c r="D178" s="9"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>98</v>
-      </c>
-      <c r="B179" s="10"/>
+        <v>94</v>
+      </c>
+      <c r="B179" s="15"/>
       <c r="C179" s="9"/>
       <c r="D179" s="12"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B180" s="10"/>
       <c r="C180" s="9"/>
-      <c r="D180" s="12"/>
+      <c r="D180" s="16"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B181" s="10"/>
       <c r="C181" s="9"/>
@@ -3015,55 +3046,55 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B182" s="10"/>
       <c r="C182" s="9"/>
-      <c r="D182" s="9"/>
+      <c r="D182" s="12"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B183" s="10"/>
-      <c r="C183" s="16"/>
-      <c r="D183" s="16"/>
+      <c r="C183" s="9"/>
+      <c r="D183" s="12"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B184" s="10"/>
-      <c r="C184" s="16"/>
-      <c r="D184" s="9"/>
+      <c r="C184" s="9"/>
+      <c r="D184" s="12"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B185" s="10"/>
       <c r="C185" s="9"/>
-      <c r="D185" s="12"/>
+      <c r="D185" s="9"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B186" s="10"/>
       <c r="C186" s="9"/>
-      <c r="D186" s="16"/>
+      <c r="D186" s="9"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>178</v>
+        <v>102</v>
       </c>
       <c r="B187" s="10"/>
-      <c r="C187" s="9"/>
-      <c r="D187" s="9"/>
+      <c r="C187" s="16"/>
+      <c r="D187" s="16"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>180</v>
+        <v>109</v>
       </c>
       <c r="B188" s="10"/>
       <c r="C188" s="16"/>
@@ -3071,200 +3102,200 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>183</v>
+        <v>110</v>
       </c>
       <c r="B189" s="10"/>
-      <c r="C189" s="16"/>
-      <c r="D189" s="9"/>
+      <c r="C189" s="9"/>
+      <c r="D189" s="12"/>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>214</v>
-      </c>
-      <c r="B190" s="15"/>
+        <v>111</v>
+      </c>
+      <c r="B190" s="10"/>
       <c r="C190" s="9"/>
-      <c r="D190" s="12"/>
+      <c r="D190" s="16"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>241</v>
+        <v>176</v>
       </c>
       <c r="B191" s="10"/>
-      <c r="C191" s="16"/>
-      <c r="D191" s="12"/>
+      <c r="C191" s="9"/>
+      <c r="D191" s="9"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>268</v>
+        <v>178</v>
       </c>
       <c r="B192" s="10"/>
-      <c r="C192" s="12"/>
-      <c r="D192" s="12"/>
+      <c r="C192" s="16"/>
+      <c r="D192" s="9"/>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>269</v>
+        <v>181</v>
       </c>
       <c r="B193" s="10"/>
       <c r="C193" s="16"/>
-      <c r="D193" s="16"/>
+      <c r="D193" s="9"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>273</v>
-      </c>
-      <c r="B194" s="10"/>
-      <c r="C194" s="12"/>
+        <v>212</v>
+      </c>
+      <c r="B194" s="15"/>
+      <c r="C194" s="9"/>
       <c r="D194" s="12"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>277</v>
-      </c>
-      <c r="B195" s="15"/>
+        <v>239</v>
+      </c>
+      <c r="B195" s="10"/>
       <c r="C195" s="16"/>
       <c r="D195" s="12"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>294</v>
-      </c>
-      <c r="B196" s="15"/>
+        <v>266</v>
+      </c>
+      <c r="B196" s="10"/>
       <c r="C196" s="12"/>
       <c r="D196" s="12"/>
     </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>267</v>
+      </c>
+      <c r="B197" s="10"/>
+      <c r="C197" s="16"/>
+      <c r="D197" s="16"/>
+    </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="2" t="s">
-        <v>121</v>
-      </c>
+      <c r="A198" t="s">
+        <v>271</v>
+      </c>
+      <c r="B198" s="10"/>
+      <c r="C198" s="12"/>
+      <c r="D198" s="12"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="5" t="s">
-        <v>122</v>
-      </c>
+      <c r="A199" t="s">
+        <v>275</v>
+      </c>
+      <c r="B199" s="15"/>
+      <c r="C199" s="16"/>
+      <c r="D199" s="12"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>124</v>
-      </c>
-      <c r="B200" s="11"/>
-      <c r="C200" s="16"/>
+        <v>292</v>
+      </c>
+      <c r="B200" s="15"/>
+      <c r="C200" s="12"/>
       <c r="D200" s="12"/>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>242</v>
-      </c>
-      <c r="B201" s="11"/>
-      <c r="C201" s="9"/>
-      <c r="D201" s="12"/>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="5" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="2" t="s">
-        <v>127</v>
-      </c>
+      <c r="A204" t="s">
+        <v>122</v>
+      </c>
+      <c r="B204" s="11"/>
+      <c r="C204" s="16"/>
+      <c r="D204" s="12"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>129</v>
+        <v>240</v>
       </c>
       <c r="B205" s="11"/>
       <c r="C205" s="9"/>
       <c r="D205" s="12"/>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>270</v>
-      </c>
-      <c r="B208" s="10"/>
-      <c r="C208" s="16"/>
-      <c r="D208" s="12"/>
+      <c r="A208" s="2" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>271</v>
-      </c>
-      <c r="B209" s="10"/>
-      <c r="C209" s="16"/>
+        <v>127</v>
+      </c>
+      <c r="B209" s="11"/>
+      <c r="C209" s="9"/>
       <c r="D209" s="12"/>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
-        <v>272</v>
-      </c>
-      <c r="B210" s="10"/>
-      <c r="C210" s="16"/>
-      <c r="D210" s="12"/>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="A212" t="s">
+        <v>268</v>
+      </c>
+      <c r="B212" s="10"/>
+      <c r="C212" s="16"/>
+      <c r="D212" s="12"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>133</v>
-      </c>
-      <c r="B213" s="17"/>
-      <c r="C213" s="9"/>
+        <v>269</v>
+      </c>
+      <c r="B213" s="10"/>
+      <c r="C213" s="16"/>
       <c r="D213" s="12"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>179</v>
+        <v>270</v>
       </c>
       <c r="B214" s="10"/>
-      <c r="C214" s="9"/>
+      <c r="C214" s="16"/>
       <c r="D214" s="12"/>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
-        <v>181</v>
-      </c>
-      <c r="B215" s="10"/>
-      <c r="C215" s="9"/>
-      <c r="D215" s="12"/>
-    </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
-        <v>182</v>
-      </c>
-      <c r="B216" s="10"/>
-      <c r="C216" s="16"/>
-      <c r="D216" s="12"/>
+      <c r="A216" s="2" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>203</v>
-      </c>
-      <c r="B217" s="10"/>
-      <c r="C217" s="16"/>
+        <v>131</v>
+      </c>
+      <c r="B217" s="17"/>
+      <c r="C217" s="9"/>
       <c r="D217" s="12"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>239</v>
-      </c>
-      <c r="B218" s="11"/>
-      <c r="C218" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="B218" s="10"/>
+      <c r="C218" s="9"/>
       <c r="D218" s="12"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>240</v>
-      </c>
-      <c r="B219" s="11"/>
-      <c r="C219" s="12"/>
+        <v>179</v>
+      </c>
+      <c r="B219" s="10"/>
+      <c r="C219" s="9"/>
       <c r="D219" s="12"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>408</v>
+        <v>180</v>
       </c>
       <c r="B220" s="10"/>
       <c r="C220" s="16"/>
@@ -3272,135 +3303,133 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>243</v>
+        <v>201</v>
       </c>
       <c r="B221" s="10"/>
-      <c r="C221" s="9"/>
-      <c r="D221" s="9"/>
+      <c r="C221" s="16"/>
+      <c r="D221" s="12"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>275</v>
-      </c>
-      <c r="B222" s="10"/>
-      <c r="C222" s="9"/>
-      <c r="D222" s="9"/>
+        <v>237</v>
+      </c>
+      <c r="B222" s="11"/>
+      <c r="C222" s="12"/>
+      <c r="D222" s="12"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>278</v>
-      </c>
-      <c r="B223" s="10"/>
-      <c r="C223" s="9"/>
-      <c r="D223" s="9"/>
+        <v>238</v>
+      </c>
+      <c r="B223" s="11"/>
+      <c r="C223" s="12"/>
+      <c r="D223" s="12"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>284</v>
-      </c>
-      <c r="B224" s="12"/>
-      <c r="C224" s="12"/>
-      <c r="D224" s="9"/>
+        <v>405</v>
+      </c>
+      <c r="B224" s="10"/>
+      <c r="C224" s="16"/>
+      <c r="D224" s="12"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>286</v>
-      </c>
-      <c r="B225" s="12"/>
-      <c r="C225" s="12"/>
-      <c r="D225" s="12"/>
+        <v>241</v>
+      </c>
+      <c r="B225" s="10"/>
+      <c r="C225" s="9"/>
+      <c r="D225" s="9"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>293</v>
-      </c>
-      <c r="B226" s="12"/>
-      <c r="C226" s="16"/>
-      <c r="D226" s="12"/>
+        <v>273</v>
+      </c>
+      <c r="B226" s="10"/>
+      <c r="C226" s="9"/>
+      <c r="D226" s="9"/>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>390</v>
-      </c>
-      <c r="B227" s="12"/>
-      <c r="C227" s="16"/>
+        <v>276</v>
+      </c>
+      <c r="B227" s="10"/>
+      <c r="C227" s="9"/>
       <c r="D227" s="9"/>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>395</v>
+        <v>282</v>
       </c>
       <c r="B228" s="12"/>
-      <c r="C228" s="9"/>
+      <c r="C228" s="12"/>
       <c r="D228" s="9"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>403</v>
+        <v>284</v>
       </c>
       <c r="B229" s="12"/>
-      <c r="C229" s="9"/>
-      <c r="D229" s="9"/>
+      <c r="C229" s="12"/>
+      <c r="D229" s="12"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>404</v>
+        <v>291</v>
       </c>
       <c r="B230" s="12"/>
-      <c r="C230" s="9"/>
+      <c r="C230" s="16"/>
       <c r="D230" s="12"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
       <c r="B231" s="12"/>
-      <c r="C231" s="9"/>
-      <c r="D231" s="12"/>
+      <c r="C231" s="16"/>
+      <c r="D231" s="9"/>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>392</v>
+      </c>
+      <c r="B232" s="12"/>
+      <c r="C232" s="9"/>
+      <c r="D232" s="9"/>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B233" s="14"/>
-      <c r="C233" s="17"/>
-      <c r="D233" s="12"/>
+      <c r="A233" t="s">
+        <v>400</v>
+      </c>
+      <c r="B233" s="12"/>
+      <c r="C233" s="9"/>
+      <c r="D233" s="9"/>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>22</v>
-      </c>
-      <c r="B234" s="14"/>
-      <c r="C234" s="17"/>
+        <v>401</v>
+      </c>
+      <c r="B234" s="12"/>
+      <c r="C234" s="9"/>
       <c r="D234" s="12"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>11</v>
-      </c>
-      <c r="B235" s="14"/>
-      <c r="C235" s="17"/>
+        <v>404</v>
+      </c>
+      <c r="B235" s="12"/>
+      <c r="C235" s="9"/>
       <c r="D235" s="12"/>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
-        <v>12</v>
-      </c>
-      <c r="B236" s="14"/>
-      <c r="C236" s="17"/>
-      <c r="D236" s="12"/>
-    </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
-        <v>13</v>
-      </c>
-      <c r="B237" s="14"/>
-      <c r="C237" s="17"/>
-      <c r="D237" s="12"/>
+      <c r="A237" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B237"/>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B238" s="14"/>
       <c r="C238" s="17"/>
@@ -3408,7 +3437,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B239" s="14"/>
       <c r="C239" s="17"/>
@@ -3416,21 +3445,53 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>24</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B240" s="14"/>
+      <c r="C240" s="17"/>
+      <c r="D240" s="12"/>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>13</v>
+      </c>
+      <c r="B241" s="14"/>
+      <c r="C241" s="17"/>
+      <c r="D241" s="12"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="2" t="s">
-        <v>145</v>
-      </c>
+      <c r="A242" t="s">
+        <v>14</v>
+      </c>
+      <c r="B242" s="14"/>
+      <c r="C242" s="17"/>
+      <c r="D242" s="12"/>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>149</v>
-      </c>
-      <c r="B243" s="11"/>
-      <c r="C243" s="16"/>
-      <c r="D243" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B243" s="14"/>
+      <c r="C243" s="17"/>
+      <c r="D243" s="12"/>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>147</v>
+      </c>
+      <c r="B247" s="11"/>
+      <c r="C247" s="16"/>
+      <c r="D247" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3440,10 +3501,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3454,14 +3515,9 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>366</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3471,10 +3527,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A107"/>
+  <dimension ref="A1:A109"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3484,452 +3540,462 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>134</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>135</v>
+      <c r="A33" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>341</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>369</v>
+        <v>339</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>394</v>
+        <v>366</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>207</v>
+        <v>391</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>208</v>
+      <c r="A42" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>250</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>225</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="A58" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>209</v>
+        <v>407</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>274</v>
+        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>292</v>
+        <v>210</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>371</v>
+        <v>272</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>374</v>
+        <v>290</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>375</v>
+        <v>369</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+      <c r="A77" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>247</v>
-      </c>
-    </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+      <c r="A84" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>144</v>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>128</v>
+      <c r="A93" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>130</v>
+      <c r="A95" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>285</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
+      <c r="A99" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>337</v>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>406</v>
+      <c r="A106" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -3955,24 +4021,24 @@
   <sheetData>
     <row r="1" spans="1:3" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B3" s="19">
         <v>40743</v>
@@ -3981,10 +4047,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C4" s="17"/>
     </row>
@@ -3993,13 +4059,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B7" s="19">
         <v>40765</v>
@@ -4008,7 +4074,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B8" s="19">
         <v>40765</v>
@@ -4017,7 +4083,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B9" s="19">
         <v>40765</v>
@@ -4026,7 +4092,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B10" s="19">
         <v>40765</v>
@@ -4035,7 +4101,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B11" s="19">
         <v>40765</v>
@@ -4047,13 +4113,13 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B14" s="19">
         <v>40738</v>
@@ -4062,7 +4128,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B15" s="19">
         <v>40738</v>
@@ -4071,7 +4137,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B16" s="19">
         <v>40738</v>
@@ -4080,21 +4146,21 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="12"/>
@@ -4104,13 +4170,13 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B22" s="19">
         <v>40749</v>
@@ -4119,7 +4185,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B23" s="19">
         <v>40749</v>
@@ -4128,7 +4194,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B24" s="19">
         <v>40749</v>
@@ -4140,25 +4206,25 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B26" s="7"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C28" s="16"/>
     </row>
@@ -4167,13 +4233,13 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B30" s="7"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B31" s="19">
         <v>40749</v>
@@ -4182,7 +4248,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B32" s="19">
         <v>40749</v>
@@ -4191,7 +4257,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B33" s="19">
         <v>40749</v>
@@ -4200,7 +4266,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B34" s="19">
         <v>40749</v>
@@ -4212,13 +4278,13 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B36" s="7"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B37" s="19">
         <v>40765</v>
@@ -4227,7 +4293,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B38" s="19">
         <v>40765</v>
@@ -4236,7 +4302,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B39" s="19">
         <v>40765</v>
@@ -4274,79 +4340,79 @@
   <sheetData>
     <row r="1" spans="1:4" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4361,7 +4427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -4374,60 +4440,60 @@
   <sheetData>
     <row r="1" spans="1:4" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>222</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" t="s">
         <v>235</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>236</v>
-      </c>
-      <c r="C4" t="s">
-        <v>237</v>
-      </c>
-      <c r="D4" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -4453,127 +4519,127 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -4597,76 +4663,76 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B3" t="s">
         <v>377</v>
-      </c>
-      <c r="B3" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B4" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B5" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B6" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B7" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B11" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added enemies stats to the tweaking controller
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -1740,8 +1740,8 @@
   <dimension ref="A1:D247"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F196" sqref="F196"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,7 +1803,7 @@
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="16"/>
-      <c r="D7" s="12"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Modified the editor and now the bullets of the player are proportional to the level
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="424">
   <si>
     <t>Tweaking System</t>
   </si>
@@ -1266,6 +1266,33 @@
   </si>
   <si>
     <t>Polish the intro cutscene</t>
+  </si>
+  <si>
+    <t>Call next wave: directly on the starting path</t>
+  </si>
+  <si>
+    <t>Next wave composition: directly on the starting path</t>
+  </si>
+  <si>
+    <t>Wave composition not showing the first time</t>
+  </si>
+  <si>
+    <t>Basic bullets visual priority</t>
+  </si>
+  <si>
+    <t>Explosion visual priority near the planet to protect</t>
+  </si>
+  <si>
+    <t>Waves submenu selection sometimes doesn't appear</t>
+  </si>
+  <si>
+    <t>CanSelect planet override so you can always select a planet in editor mode</t>
+  </si>
+  <si>
+    <t>Load and modify a previously made level</t>
+  </si>
+  <si>
+    <t>Visual priority of panels is fucked</t>
   </si>
 </sst>
 </file>
@@ -1737,11 +1764,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D247"/>
+  <dimension ref="A1:D256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A165" sqref="A165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2795,7 +2822,7 @@
       </c>
       <c r="B146" s="14"/>
       <c r="C146" s="9"/>
-      <c r="D146" s="12"/>
+      <c r="D146" s="9"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
@@ -2909,168 +2936,160 @@
       <c r="C160" s="12"/>
       <c r="D160" s="12"/>
     </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>420</v>
+      </c>
+      <c r="B161"/>
+    </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="2" t="s">
+      <c r="A162" t="s">
+        <v>421</v>
+      </c>
+      <c r="B162"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>422</v>
+      </c>
+      <c r="B163"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>423</v>
+      </c>
+      <c r="B164"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="5" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="8" t="s">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="B164" s="10"/>
-      <c r="C164" s="16"/>
-      <c r="D164" s="12"/>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="8" t="s">
+      <c r="B168" s="10"/>
+      <c r="C168" s="16"/>
+      <c r="D168" s="12"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="B165" s="15"/>
-      <c r="C165" s="12"/>
-      <c r="D165" s="12"/>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>298</v>
-      </c>
-      <c r="B166" s="15"/>
-      <c r="C166" s="12"/>
-      <c r="D166" s="12"/>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>299</v>
-      </c>
-      <c r="B167" s="15"/>
-      <c r="C167" s="12"/>
-      <c r="D167" s="12"/>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>300</v>
-      </c>
-      <c r="B168" s="15"/>
-      <c r="C168" s="12"/>
-      <c r="D168" s="12"/>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>169</v>
-      </c>
-      <c r="B169" s="11"/>
-      <c r="C169" s="16"/>
+      <c r="B169" s="15"/>
+      <c r="C169" s="12"/>
       <c r="D169" s="12"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>172</v>
-      </c>
-      <c r="B170" s="11"/>
-      <c r="C170" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="B170" s="15"/>
+      <c r="C170" s="12"/>
       <c r="D170" s="12"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>170</v>
-      </c>
-      <c r="B171" s="11"/>
-      <c r="C171" s="16"/>
+        <v>299</v>
+      </c>
+      <c r="B171" s="15"/>
+      <c r="C171" s="12"/>
       <c r="D171" s="12"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>171</v>
-      </c>
-      <c r="B172" s="11"/>
-      <c r="C172" s="16"/>
+        <v>300</v>
+      </c>
+      <c r="B172" s="15"/>
+      <c r="C172" s="12"/>
       <c r="D172" s="12"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>301</v>
+        <v>169</v>
       </c>
       <c r="B173" s="11"/>
       <c r="C173" s="16"/>
       <c r="D173" s="12"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B174"/>
+      <c r="A174" t="s">
+        <v>172</v>
+      </c>
+      <c r="B174" s="11"/>
+      <c r="C174" s="16"/>
+      <c r="D174" s="12"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>170</v>
+      </c>
+      <c r="B175" s="11"/>
+      <c r="C175" s="16"/>
+      <c r="D175" s="12"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="s">
+      <c r="A176" t="s">
+        <v>171</v>
+      </c>
+      <c r="B176" s="11"/>
+      <c r="C176" s="16"/>
+      <c r="D176" s="12"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>301</v>
+      </c>
+      <c r="B177" s="11"/>
+      <c r="C177" s="16"/>
+      <c r="D177" s="12"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B178"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="5" t="s">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="5" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>92</v>
-      </c>
-      <c r="B178" s="10"/>
-      <c r="C178" s="16"/>
-      <c r="D178" s="9"/>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>94</v>
-      </c>
-      <c r="B179" s="15"/>
-      <c r="C179" s="9"/>
-      <c r="D179" s="12"/>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>95</v>
-      </c>
-      <c r="B180" s="10"/>
-      <c r="C180" s="9"/>
-      <c r="D180" s="16"/>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>96</v>
-      </c>
-      <c r="B181" s="10"/>
-      <c r="C181" s="9"/>
-      <c r="D181" s="9"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B182" s="10"/>
-      <c r="C182" s="9"/>
-      <c r="D182" s="12"/>
+      <c r="C182" s="16"/>
+      <c r="D182" s="9"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>98</v>
-      </c>
-      <c r="B183" s="10"/>
+        <v>94</v>
+      </c>
+      <c r="B183" s="15"/>
       <c r="C183" s="9"/>
       <c r="D183" s="12"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B184" s="10"/>
       <c r="C184" s="9"/>
-      <c r="D184" s="12"/>
+      <c r="D184" s="16"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B185" s="10"/>
       <c r="C185" s="9"/>
@@ -3078,55 +3097,55 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B186" s="10"/>
       <c r="C186" s="9"/>
-      <c r="D186" s="9"/>
+      <c r="D186" s="12"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B187" s="10"/>
-      <c r="C187" s="16"/>
-      <c r="D187" s="16"/>
+      <c r="C187" s="9"/>
+      <c r="D187" s="12"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B188" s="10"/>
-      <c r="C188" s="16"/>
-      <c r="D188" s="9"/>
+      <c r="C188" s="9"/>
+      <c r="D188" s="12"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B189" s="10"/>
       <c r="C189" s="9"/>
-      <c r="D189" s="12"/>
+      <c r="D189" s="9"/>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B190" s="10"/>
       <c r="C190" s="9"/>
-      <c r="D190" s="16"/>
+      <c r="D190" s="9"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>176</v>
+        <v>102</v>
       </c>
       <c r="B191" s="10"/>
-      <c r="C191" s="9"/>
-      <c r="D191" s="9"/>
+      <c r="C191" s="16"/>
+      <c r="D191" s="16"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>178</v>
+        <v>109</v>
       </c>
       <c r="B192" s="10"/>
       <c r="C192" s="16"/>
@@ -3134,364 +3153,426 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>181</v>
+        <v>110</v>
       </c>
       <c r="B193" s="10"/>
-      <c r="C193" s="16"/>
-      <c r="D193" s="9"/>
+      <c r="C193" s="9"/>
+      <c r="D193" s="12"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>212</v>
-      </c>
-      <c r="B194" s="15"/>
+        <v>111</v>
+      </c>
+      <c r="B194" s="10"/>
       <c r="C194" s="9"/>
-      <c r="D194" s="12"/>
+      <c r="D194" s="16"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>239</v>
+        <v>176</v>
       </c>
       <c r="B195" s="10"/>
-      <c r="C195" s="16"/>
-      <c r="D195" s="12"/>
+      <c r="C195" s="9"/>
+      <c r="D195" s="9"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>266</v>
+        <v>178</v>
       </c>
       <c r="B196" s="10"/>
-      <c r="C196" s="12"/>
-      <c r="D196" s="12"/>
+      <c r="C196" s="16"/>
+      <c r="D196" s="9"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>267</v>
+        <v>181</v>
       </c>
       <c r="B197" s="10"/>
       <c r="C197" s="16"/>
-      <c r="D197" s="16"/>
+      <c r="D197" s="9"/>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>271</v>
-      </c>
-      <c r="B198" s="10"/>
-      <c r="C198" s="12"/>
+        <v>212</v>
+      </c>
+      <c r="B198" s="15"/>
+      <c r="C198" s="9"/>
       <c r="D198" s="12"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>275</v>
-      </c>
-      <c r="B199" s="15"/>
+        <v>239</v>
+      </c>
+      <c r="B199" s="10"/>
       <c r="C199" s="16"/>
       <c r="D199" s="12"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>292</v>
-      </c>
-      <c r="B200" s="15"/>
+        <v>266</v>
+      </c>
+      <c r="B200" s="10"/>
       <c r="C200" s="12"/>
       <c r="D200" s="12"/>
     </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>267</v>
+      </c>
+      <c r="B201" s="10"/>
+      <c r="C201" s="16"/>
+      <c r="D201" s="16"/>
+    </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="2" t="s">
-        <v>119</v>
-      </c>
+      <c r="A202" t="s">
+        <v>271</v>
+      </c>
+      <c r="B202" s="10"/>
+      <c r="C202" s="12"/>
+      <c r="D202" s="12"/>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="5" t="s">
-        <v>120</v>
-      </c>
+      <c r="A203" t="s">
+        <v>275</v>
+      </c>
+      <c r="B203" s="15"/>
+      <c r="C203" s="16"/>
+      <c r="D203" s="12"/>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>122</v>
-      </c>
-      <c r="B204" s="11"/>
-      <c r="C204" s="16"/>
+        <v>292</v>
+      </c>
+      <c r="B204" s="15"/>
+      <c r="C204" s="12"/>
       <c r="D204" s="12"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>240</v>
-      </c>
-      <c r="B205" s="11"/>
-      <c r="C205" s="9"/>
-      <c r="D205" s="12"/>
+        <v>416</v>
+      </c>
+      <c r="B205"/>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>415</v>
+      </c>
+      <c r="B206"/>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>122</v>
+      </c>
+      <c r="B210" s="11"/>
+      <c r="C210" s="16"/>
+      <c r="D210" s="12"/>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>240</v>
+      </c>
+      <c r="B211" s="11"/>
+      <c r="C211" s="9"/>
+      <c r="D211" s="12"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>127</v>
       </c>
-      <c r="B209" s="11"/>
-      <c r="C209" s="9"/>
-      <c r="D209" s="12"/>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="2" t="s">
+      <c r="B215" s="11"/>
+      <c r="C215" s="9"/>
+      <c r="D215" s="12"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>268</v>
-      </c>
-      <c r="B212" s="10"/>
-      <c r="C212" s="16"/>
-      <c r="D212" s="12"/>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>269</v>
-      </c>
-      <c r="B213" s="10"/>
-      <c r="C213" s="16"/>
-      <c r="D213" s="12"/>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
-        <v>270</v>
-      </c>
-      <c r="B214" s="10"/>
-      <c r="C214" s="16"/>
-      <c r="D214" s="12"/>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>131</v>
-      </c>
-      <c r="B217" s="17"/>
-      <c r="C217" s="9"/>
-      <c r="D217" s="12"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>177</v>
+        <v>268</v>
       </c>
       <c r="B218" s="10"/>
-      <c r="C218" s="9"/>
+      <c r="C218" s="16"/>
       <c r="D218" s="12"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>179</v>
+        <v>269</v>
       </c>
       <c r="B219" s="10"/>
-      <c r="C219" s="9"/>
+      <c r="C219" s="16"/>
       <c r="D219" s="12"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="B220" s="10"/>
       <c r="C220" s="16"/>
       <c r="D220" s="12"/>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>201</v>
-      </c>
-      <c r="B221" s="10"/>
-      <c r="C221" s="16"/>
-      <c r="D221" s="12"/>
-    </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>237</v>
-      </c>
-      <c r="B222" s="11"/>
-      <c r="C222" s="12"/>
-      <c r="D222" s="12"/>
+      <c r="A222" s="2" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>238</v>
-      </c>
-      <c r="B223" s="11"/>
-      <c r="C223" s="12"/>
+        <v>131</v>
+      </c>
+      <c r="B223" s="17"/>
+      <c r="C223" s="9"/>
       <c r="D223" s="12"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>405</v>
+        <v>177</v>
       </c>
       <c r="B224" s="10"/>
-      <c r="C224" s="16"/>
+      <c r="C224" s="9"/>
       <c r="D224" s="12"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>241</v>
+        <v>179</v>
       </c>
       <c r="B225" s="10"/>
       <c r="C225" s="9"/>
-      <c r="D225" s="9"/>
+      <c r="D225" s="12"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>273</v>
+        <v>180</v>
       </c>
       <c r="B226" s="10"/>
-      <c r="C226" s="9"/>
-      <c r="D226" s="9"/>
+      <c r="C226" s="16"/>
+      <c r="D226" s="12"/>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>276</v>
+        <v>201</v>
       </c>
       <c r="B227" s="10"/>
-      <c r="C227" s="9"/>
-      <c r="D227" s="9"/>
+      <c r="C227" s="16"/>
+      <c r="D227" s="12"/>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>282</v>
-      </c>
-      <c r="B228" s="12"/>
+        <v>237</v>
+      </c>
+      <c r="B228" s="11"/>
       <c r="C228" s="12"/>
-      <c r="D228" s="9"/>
+      <c r="D228" s="12"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>284</v>
-      </c>
-      <c r="B229" s="12"/>
+        <v>238</v>
+      </c>
+      <c r="B229" s="11"/>
       <c r="C229" s="12"/>
       <c r="D229" s="12"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>291</v>
-      </c>
-      <c r="B230" s="12"/>
+        <v>405</v>
+      </c>
+      <c r="B230" s="10"/>
       <c r="C230" s="16"/>
       <c r="D230" s="12"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>387</v>
-      </c>
-      <c r="B231" s="12"/>
-      <c r="C231" s="16"/>
+        <v>241</v>
+      </c>
+      <c r="B231" s="10"/>
+      <c r="C231" s="9"/>
       <c r="D231" s="9"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>392</v>
-      </c>
-      <c r="B232" s="12"/>
+        <v>273</v>
+      </c>
+      <c r="B232" s="10"/>
       <c r="C232" s="9"/>
       <c r="D232" s="9"/>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>400</v>
-      </c>
-      <c r="B233" s="12"/>
+        <v>276</v>
+      </c>
+      <c r="B233" s="10"/>
       <c r="C233" s="9"/>
       <c r="D233" s="9"/>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>401</v>
+        <v>282</v>
       </c>
       <c r="B234" s="12"/>
-      <c r="C234" s="9"/>
-      <c r="D234" s="12"/>
+      <c r="C234" s="12"/>
+      <c r="D234" s="9"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>404</v>
+        <v>284</v>
       </c>
       <c r="B235" s="12"/>
-      <c r="C235" s="9"/>
+      <c r="C235" s="12"/>
       <c r="D235" s="12"/>
     </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>291</v>
+      </c>
+      <c r="B236" s="12"/>
+      <c r="C236" s="16"/>
+      <c r="D236" s="12"/>
+    </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B237"/>
+      <c r="A237" t="s">
+        <v>387</v>
+      </c>
+      <c r="B237" s="12"/>
+      <c r="C237" s="16"/>
+      <c r="D237" s="9"/>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>22</v>
-      </c>
-      <c r="B238" s="14"/>
-      <c r="C238" s="17"/>
-      <c r="D238" s="12"/>
+        <v>392</v>
+      </c>
+      <c r="B238" s="12"/>
+      <c r="C238" s="9"/>
+      <c r="D238" s="9"/>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>11</v>
-      </c>
-      <c r="B239" s="14"/>
-      <c r="C239" s="17"/>
-      <c r="D239" s="12"/>
+        <v>400</v>
+      </c>
+      <c r="B239" s="12"/>
+      <c r="C239" s="9"/>
+      <c r="D239" s="9"/>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>12</v>
-      </c>
-      <c r="B240" s="14"/>
-      <c r="C240" s="17"/>
+        <v>401</v>
+      </c>
+      <c r="B240" s="12"/>
+      <c r="C240" s="9"/>
       <c r="D240" s="12"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>13</v>
-      </c>
-      <c r="B241" s="14"/>
-      <c r="C241" s="17"/>
+        <v>404</v>
+      </c>
+      <c r="B241" s="12"/>
+      <c r="C241" s="9"/>
       <c r="D241" s="12"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>14</v>
-      </c>
-      <c r="B242" s="14"/>
-      <c r="C242" s="17"/>
-      <c r="D242" s="12"/>
+        <v>417</v>
+      </c>
+      <c r="B242"/>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>23</v>
-      </c>
-      <c r="B243" s="14"/>
-      <c r="C243" s="17"/>
-      <c r="D243" s="12"/>
+        <v>418</v>
+      </c>
+      <c r="B243"/>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>24</v>
-      </c>
+        <v>419</v>
+      </c>
+      <c r="B244"/>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>143</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B246"/>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
+        <v>22</v>
+      </c>
+      <c r="B247" s="14"/>
+      <c r="C247" s="17"/>
+      <c r="D247" s="12"/>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>11</v>
+      </c>
+      <c r="B248" s="14"/>
+      <c r="C248" s="17"/>
+      <c r="D248" s="12"/>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>12</v>
+      </c>
+      <c r="B249" s="14"/>
+      <c r="C249" s="17"/>
+      <c r="D249" s="12"/>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>13</v>
+      </c>
+      <c r="B250" s="14"/>
+      <c r="C250" s="17"/>
+      <c r="D250" s="12"/>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>14</v>
+      </c>
+      <c r="B251" s="14"/>
+      <c r="C251" s="17"/>
+      <c r="D251" s="12"/>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>23</v>
+      </c>
+      <c r="B252" s="14"/>
+      <c r="C252" s="17"/>
+      <c r="D252" s="12"/>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
         <v>147</v>
       </c>
-      <c r="B247" s="11"/>
-      <c r="C247" s="16"/>
-      <c r="D247" s="9"/>
+      <c r="B256" s="11"/>
+      <c r="C256" s="16"/>
+      <c r="D256" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modified level ended announciation and more. Like usual.
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="19050" windowHeight="8625"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18990" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="431">
   <si>
     <t>Tweaking System</t>
   </si>
@@ -668,9 +668,6 @@
     <t>Bug: the visual priorities of celestial bodies are rising too fast</t>
   </si>
   <si>
-    <t>Put the delay, switch every, etc. is seconds</t>
-  </si>
-  <si>
     <t>Bug: panels not reinitialized on new level</t>
   </si>
   <si>
@@ -1293,6 +1290,30 @@
   </si>
   <si>
     <t>Visual priority of panels is fucked</t>
+  </si>
+  <si>
+    <t>Sync of wave type is fucked</t>
+  </si>
+  <si>
+    <t>Put the delay, switch every, etc. in seconds</t>
+  </si>
+  <si>
+    <t>Redefine how wave types are described in the XML</t>
+  </si>
+  <si>
+    <t>Gravitational turret previewing is fucked</t>
+  </si>
+  <si>
+    <t>Money sync in level editor seems fucked at times</t>
+  </si>
+  <si>
+    <t>Next wave annunciation is not appearing for the first wave</t>
+  </si>
+  <si>
+    <t>When the level is finished, the animation is fucked</t>
+  </si>
+  <si>
+    <t>Revisit the Windows control scheme to include the mouse back (right button for speed?)</t>
   </si>
 </sst>
 </file>
@@ -1764,11 +1785,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D256"/>
+  <dimension ref="A1:D262"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A165" sqref="A165"/>
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1784,13 +1805,13 @@
         <v>117</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1900,7 +1921,7 @@
       <c r="B17" s="10"/>
       <c r="C17" s="12"/>
       <c r="D17" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1918,12 +1939,12 @@
       <c r="B19" s="10"/>
       <c r="C19" s="9"/>
       <c r="D19" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="9"/>
@@ -1931,7 +1952,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="16"/>
@@ -1939,7 +1960,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="16"/>
@@ -1952,7 +1973,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="16"/>
@@ -1970,7 +1991,7 @@
       <c r="B28" s="11"/>
       <c r="C28" s="16"/>
       <c r="D28" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1980,7 +2001,7 @@
       <c r="B29" s="11"/>
       <c r="C29" s="16"/>
       <c r="D29" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2017,7 +2038,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="9"/>
@@ -2091,7 +2112,7 @@
       <c r="B44" s="14"/>
       <c r="C44" s="12"/>
       <c r="D44" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2257,7 +2278,7 @@
       <c r="B70" s="14"/>
       <c r="C70" s="17"/>
       <c r="D70" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2267,7 +2288,7 @@
       <c r="B71" s="14"/>
       <c r="C71" s="17"/>
       <c r="D71" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2277,7 +2298,7 @@
       <c r="B72" s="14"/>
       <c r="C72" s="17"/>
       <c r="D72" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2287,7 +2308,7 @@
       <c r="B73" s="14"/>
       <c r="C73" s="17"/>
       <c r="D73" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2297,7 +2318,7 @@
       <c r="B74" s="14"/>
       <c r="C74" s="17"/>
       <c r="D74" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2307,7 +2328,7 @@
       <c r="B75" s="14"/>
       <c r="C75" s="17"/>
       <c r="D75" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2317,7 +2338,7 @@
       <c r="B76" s="14"/>
       <c r="C76" s="17"/>
       <c r="D76" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2327,7 +2348,7 @@
       <c r="B77" s="14"/>
       <c r="C77" s="17"/>
       <c r="D77" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2422,7 +2443,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B92" s="10"/>
       <c r="C92" s="9"/>
@@ -2430,7 +2451,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B93" s="10"/>
       <c r="C93" s="9"/>
@@ -2438,7 +2459,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B94" s="10"/>
       <c r="C94" s="9"/>
@@ -2446,7 +2467,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B95" s="10"/>
       <c r="C95" s="9"/>
@@ -2454,7 +2475,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="16"/>
@@ -2462,7 +2483,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B97" s="10"/>
       <c r="C97" s="16"/>
@@ -2483,7 +2504,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B101" s="10"/>
       <c r="C101" s="9"/>
@@ -2499,7 +2520,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B103" s="10"/>
       <c r="C103" s="9"/>
@@ -2507,7 +2528,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B104" s="10"/>
       <c r="C104" s="9"/>
@@ -2515,7 +2536,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B105" s="10"/>
       <c r="C105" s="9"/>
@@ -2523,7 +2544,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B106" s="10"/>
       <c r="C106" s="9"/>
@@ -2531,7 +2552,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B107" s="10"/>
       <c r="C107" s="16"/>
@@ -2539,7 +2560,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B108" s="10"/>
       <c r="C108" s="16"/>
@@ -2547,7 +2568,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B109" s="10"/>
       <c r="C109" s="9"/>
@@ -2555,7 +2576,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B110" s="10"/>
       <c r="C110" s="16"/>
@@ -2563,7 +2584,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B111" s="10"/>
       <c r="C111" s="9"/>
@@ -2571,7 +2592,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B112" s="10"/>
       <c r="C112" s="16"/>
@@ -2579,7 +2600,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B113" s="10"/>
       <c r="C113" s="12"/>
@@ -2587,7 +2608,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B114" s="10"/>
       <c r="C114" s="12"/>
@@ -2595,7 +2616,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B115" s="10"/>
       <c r="C115" s="16"/>
@@ -2603,7 +2624,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B116" s="10"/>
       <c r="C116" s="16"/>
@@ -2619,7 +2640,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B118" s="14"/>
       <c r="C118" s="17"/>
@@ -2635,7 +2656,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B120" s="14"/>
       <c r="C120" s="17"/>
@@ -2643,7 +2664,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B121" s="14"/>
       <c r="C121" s="17"/>
@@ -2651,7 +2672,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B122" s="14"/>
       <c r="C122" s="17"/>
@@ -2659,7 +2680,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B123" s="10"/>
       <c r="C123" s="16"/>
@@ -2667,7 +2688,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B124" s="10"/>
       <c r="C124" s="16"/>
@@ -2818,7 +2839,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B146" s="14"/>
       <c r="C146" s="9"/>
@@ -2870,7 +2891,7 @@
       </c>
       <c r="B152" s="11"/>
       <c r="C152" s="9"/>
-      <c r="D152" s="12"/>
+      <c r="D152" s="9"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
@@ -2878,7 +2899,7 @@
       </c>
       <c r="B153" s="11"/>
       <c r="C153" s="9"/>
-      <c r="D153" s="12"/>
+      <c r="D153" s="9"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
@@ -2898,7 +2919,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>215</v>
+        <v>424</v>
       </c>
       <c r="B156" s="15"/>
       <c r="C156" s="9"/>
@@ -2906,23 +2927,23 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B157" s="10"/>
       <c r="C157" s="9"/>
-      <c r="D157" s="12"/>
+      <c r="D157" s="9"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B158" s="10"/>
       <c r="C158" s="9"/>
-      <c r="D158" s="12"/>
+      <c r="D158" s="9"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B159" s="14"/>
       <c r="C159" s="12"/>
@@ -2930,7 +2951,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B160" s="14"/>
       <c r="C160" s="12"/>
@@ -2938,65 +2959,73 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>420</v>
-      </c>
-      <c r="B161"/>
+        <v>419</v>
+      </c>
+      <c r="B161" s="11"/>
+      <c r="C161" s="9"/>
+      <c r="D161" s="10"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>421</v>
-      </c>
-      <c r="B162"/>
+        <v>420</v>
+      </c>
+      <c r="B162" s="10"/>
+      <c r="C162" s="9"/>
+      <c r="D162" s="9"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>422</v>
-      </c>
-      <c r="B163"/>
+        <v>421</v>
+      </c>
+      <c r="B163" s="10"/>
+      <c r="C163" s="12"/>
+      <c r="D163" s="10"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>422</v>
+      </c>
+      <c r="B164" s="11"/>
+      <c r="C164" s="9"/>
+      <c r="D164" s="10"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>423</v>
       </c>
-      <c r="B164"/>
+      <c r="B165" s="10"/>
+      <c r="C165" s="9"/>
+      <c r="D165" s="9"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="2" t="s">
+      <c r="A166" t="s">
+        <v>425</v>
+      </c>
+      <c r="B166" s="10"/>
+      <c r="C166" s="9"/>
+      <c r="D166" s="9"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="5" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="B168" s="10"/>
-      <c r="C168" s="16"/>
-      <c r="D168" s="12"/>
-    </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="B169" s="15"/>
-      <c r="C169" s="12"/>
-      <c r="D169" s="12"/>
+      <c r="A169" s="5" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>298</v>
-      </c>
-      <c r="B170" s="15"/>
-      <c r="C170" s="12"/>
+      <c r="A170" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="B170" s="10"/>
+      <c r="C170" s="16"/>
       <c r="D170" s="12"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>299</v>
+      <c r="A171" s="8" t="s">
+        <v>296</v>
       </c>
       <c r="B171" s="15"/>
       <c r="C171" s="12"/>
@@ -3004,7 +3033,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B172" s="15"/>
       <c r="C172" s="12"/>
@@ -3012,23 +3041,23 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>169</v>
-      </c>
-      <c r="B173" s="11"/>
-      <c r="C173" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="B173" s="15"/>
+      <c r="C173" s="12"/>
       <c r="D173" s="12"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>172</v>
-      </c>
-      <c r="B174" s="11"/>
-      <c r="C174" s="16"/>
+        <v>299</v>
+      </c>
+      <c r="B174" s="15"/>
+      <c r="C174" s="12"/>
       <c r="D174" s="12"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B175" s="11"/>
       <c r="C175" s="16"/>
@@ -3036,7 +3065,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B176" s="11"/>
       <c r="C176" s="16"/>
@@ -3044,76 +3073,76 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>301</v>
+        <v>170</v>
       </c>
       <c r="B177" s="11"/>
       <c r="C177" s="16"/>
       <c r="D177" s="12"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B178"/>
+      <c r="A178" t="s">
+        <v>171</v>
+      </c>
+      <c r="B178" s="11"/>
+      <c r="C178" s="16"/>
+      <c r="D178" s="12"/>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>300</v>
+      </c>
+      <c r="B179" s="11"/>
+      <c r="C179" s="16"/>
+      <c r="D179" s="12"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="2" t="s">
+      <c r="B180"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="5" t="s">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="5" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>92</v>
-      </c>
-      <c r="B182" s="10"/>
-      <c r="C182" s="16"/>
-      <c r="D182" s="9"/>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>94</v>
-      </c>
-      <c r="B183" s="15"/>
-      <c r="C183" s="9"/>
-      <c r="D183" s="12"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B184" s="10"/>
-      <c r="C184" s="9"/>
-      <c r="D184" s="16"/>
+      <c r="C184" s="16"/>
+      <c r="D184" s="9"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>96</v>
-      </c>
-      <c r="B185" s="10"/>
+        <v>94</v>
+      </c>
+      <c r="B185" s="15"/>
       <c r="C185" s="9"/>
-      <c r="D185" s="9"/>
+      <c r="D185" s="12"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B186" s="10"/>
       <c r="C186" s="9"/>
-      <c r="D186" s="12"/>
+      <c r="D186" s="16"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B187" s="10"/>
       <c r="C187" s="9"/>
-      <c r="D187" s="12"/>
+      <c r="D187" s="9"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B188" s="10"/>
       <c r="C188" s="9"/>
@@ -3121,111 +3150,111 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B189" s="10"/>
       <c r="C189" s="9"/>
-      <c r="D189" s="9"/>
+      <c r="D189" s="12"/>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B190" s="10"/>
       <c r="C190" s="9"/>
-      <c r="D190" s="9"/>
+      <c r="D190" s="12"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B191" s="10"/>
-      <c r="C191" s="16"/>
-      <c r="D191" s="16"/>
+      <c r="C191" s="9"/>
+      <c r="D191" s="9"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B192" s="10"/>
-      <c r="C192" s="16"/>
+      <c r="C192" s="9"/>
       <c r="D192" s="9"/>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B193" s="10"/>
-      <c r="C193" s="9"/>
-      <c r="D193" s="12"/>
+      <c r="C193" s="16"/>
+      <c r="D193" s="16"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B194" s="10"/>
-      <c r="C194" s="9"/>
-      <c r="D194" s="16"/>
+      <c r="C194" s="16"/>
+      <c r="D194" s="9"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>176</v>
+        <v>110</v>
       </c>
       <c r="B195" s="10"/>
       <c r="C195" s="9"/>
-      <c r="D195" s="9"/>
+      <c r="D195" s="12"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>178</v>
+        <v>111</v>
       </c>
       <c r="B196" s="10"/>
-      <c r="C196" s="16"/>
-      <c r="D196" s="9"/>
+      <c r="C196" s="9"/>
+      <c r="D196" s="16"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B197" s="10"/>
-      <c r="C197" s="16"/>
+      <c r="C197" s="9"/>
       <c r="D197" s="9"/>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>212</v>
-      </c>
-      <c r="B198" s="15"/>
-      <c r="C198" s="9"/>
-      <c r="D198" s="12"/>
+        <v>178</v>
+      </c>
+      <c r="B198" s="10"/>
+      <c r="C198" s="16"/>
+      <c r="D198" s="9"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>239</v>
+        <v>181</v>
       </c>
       <c r="B199" s="10"/>
       <c r="C199" s="16"/>
-      <c r="D199" s="12"/>
+      <c r="D199" s="9"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>266</v>
-      </c>
-      <c r="B200" s="10"/>
-      <c r="C200" s="12"/>
+        <v>212</v>
+      </c>
+      <c r="B200" s="15"/>
+      <c r="C200" s="9"/>
       <c r="D200" s="12"/>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>267</v>
+        <v>238</v>
       </c>
       <c r="B201" s="10"/>
       <c r="C201" s="16"/>
-      <c r="D201" s="16"/>
+      <c r="D201" s="12"/>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B202" s="10"/>
       <c r="C202" s="12"/>
@@ -3233,188 +3262,188 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>275</v>
-      </c>
-      <c r="B203" s="15"/>
+        <v>266</v>
+      </c>
+      <c r="B203" s="10"/>
       <c r="C203" s="16"/>
-      <c r="D203" s="12"/>
+      <c r="D203" s="16"/>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>292</v>
-      </c>
-      <c r="B204" s="15"/>
+        <v>270</v>
+      </c>
+      <c r="B204" s="10"/>
       <c r="C204" s="12"/>
       <c r="D204" s="12"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>416</v>
-      </c>
-      <c r="B205"/>
+        <v>274</v>
+      </c>
+      <c r="B205" s="15"/>
+      <c r="C205" s="16"/>
+      <c r="D205" s="12"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
+        <v>291</v>
+      </c>
+      <c r="B206" s="15"/>
+      <c r="C206" s="12"/>
+      <c r="D206" s="12"/>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
         <v>415</v>
       </c>
-      <c r="B206"/>
+      <c r="B207"/>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="2" t="s">
+      <c r="A208" t="s">
+        <v>414</v>
+      </c>
+      <c r="B208"/>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="5" t="s">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>122</v>
       </c>
-      <c r="B210" s="11"/>
-      <c r="C210" s="16"/>
-      <c r="D210" s="12"/>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>240</v>
-      </c>
-      <c r="B211" s="11"/>
-      <c r="C211" s="9"/>
-      <c r="D211" s="12"/>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="2" t="s">
+      <c r="B212" s="11"/>
+      <c r="C212" s="16"/>
+      <c r="D212" s="12"/>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>239</v>
+      </c>
+      <c r="B213" s="11"/>
+      <c r="C213" s="9"/>
+      <c r="D213" s="12"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>127</v>
       </c>
-      <c r="B215" s="11"/>
-      <c r="C215" s="9"/>
-      <c r="D215" s="12"/>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="2" t="s">
+      <c r="B217" s="11"/>
+      <c r="C217" s="9"/>
+      <c r="D217" s="12"/>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>268</v>
-      </c>
-      <c r="B218" s="10"/>
-      <c r="C218" s="16"/>
-      <c r="D218" s="12"/>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>269</v>
-      </c>
-      <c r="B219" s="10"/>
-      <c r="C219" s="16"/>
-      <c r="D219" s="12"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B220" s="10"/>
       <c r="C220" s="16"/>
       <c r="D220" s="12"/>
     </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>268</v>
+      </c>
+      <c r="B221" s="10"/>
+      <c r="C221" s="16"/>
+      <c r="D221" s="12"/>
+    </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="2" t="s">
+      <c r="A222" t="s">
+        <v>269</v>
+      </c>
+      <c r="B222" s="10"/>
+      <c r="C222" s="16"/>
+      <c r="D222" s="12"/>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>131</v>
-      </c>
-      <c r="B223" s="17"/>
-      <c r="C223" s="9"/>
-      <c r="D223" s="12"/>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>177</v>
-      </c>
-      <c r="B224" s="10"/>
-      <c r="C224" s="9"/>
-      <c r="D224" s="12"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>179</v>
-      </c>
-      <c r="B225" s="10"/>
+        <v>131</v>
+      </c>
+      <c r="B225" s="17"/>
       <c r="C225" s="9"/>
       <c r="D225" s="12"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B226" s="10"/>
-      <c r="C226" s="16"/>
+      <c r="C226" s="9"/>
       <c r="D226" s="12"/>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="B227" s="10"/>
-      <c r="C227" s="16"/>
+      <c r="C227" s="9"/>
       <c r="D227" s="12"/>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>237</v>
-      </c>
-      <c r="B228" s="11"/>
-      <c r="C228" s="12"/>
+        <v>180</v>
+      </c>
+      <c r="B228" s="10"/>
+      <c r="C228" s="16"/>
       <c r="D228" s="12"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>238</v>
-      </c>
-      <c r="B229" s="11"/>
-      <c r="C229" s="12"/>
+        <v>201</v>
+      </c>
+      <c r="B229" s="10"/>
+      <c r="C229" s="16"/>
       <c r="D229" s="12"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>405</v>
-      </c>
-      <c r="B230" s="10"/>
-      <c r="C230" s="16"/>
+        <v>236</v>
+      </c>
+      <c r="B230" s="11"/>
+      <c r="C230" s="12"/>
       <c r="D230" s="12"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>241</v>
-      </c>
-      <c r="B231" s="10"/>
-      <c r="C231" s="9"/>
-      <c r="D231" s="9"/>
+        <v>237</v>
+      </c>
+      <c r="B231" s="11"/>
+      <c r="C231" s="12"/>
+      <c r="D231" s="12"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>273</v>
+        <v>404</v>
       </c>
       <c r="B232" s="10"/>
-      <c r="C232" s="9"/>
-      <c r="D232" s="9"/>
+      <c r="C232" s="16"/>
+      <c r="D232" s="12"/>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>276</v>
+        <v>240</v>
       </c>
       <c r="B233" s="10"/>
       <c r="C233" s="9"/>
@@ -3422,157 +3451,196 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>282</v>
-      </c>
-      <c r="B234" s="12"/>
-      <c r="C234" s="12"/>
+        <v>272</v>
+      </c>
+      <c r="B234" s="10"/>
+      <c r="C234" s="9"/>
       <c r="D234" s="9"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>284</v>
-      </c>
-      <c r="B235" s="12"/>
-      <c r="C235" s="12"/>
-      <c r="D235" s="12"/>
+        <v>275</v>
+      </c>
+      <c r="B235" s="10"/>
+      <c r="C235" s="9"/>
+      <c r="D235" s="9"/>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="B236" s="12"/>
-      <c r="C236" s="16"/>
-      <c r="D236" s="12"/>
+      <c r="C236" s="12"/>
+      <c r="D236" s="9"/>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>387</v>
+        <v>283</v>
       </c>
       <c r="B237" s="12"/>
-      <c r="C237" s="16"/>
-      <c r="D237" s="9"/>
+      <c r="C237" s="12"/>
+      <c r="D237" s="12"/>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>392</v>
+        <v>290</v>
       </c>
       <c r="B238" s="12"/>
-      <c r="C238" s="9"/>
-      <c r="D238" s="9"/>
+      <c r="C238" s="16"/>
+      <c r="D238" s="12"/>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="B239" s="12"/>
-      <c r="C239" s="9"/>
+      <c r="C239" s="16"/>
       <c r="D239" s="9"/>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="B240" s="12"/>
       <c r="C240" s="9"/>
-      <c r="D240" s="12"/>
+      <c r="D240" s="9"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B241" s="12"/>
       <c r="C241" s="9"/>
-      <c r="D241" s="12"/>
+      <c r="D241" s="9"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>417</v>
-      </c>
-      <c r="B242"/>
+        <v>400</v>
+      </c>
+      <c r="B242" s="12"/>
+      <c r="C242" s="9"/>
+      <c r="D242" s="12"/>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>418</v>
-      </c>
-      <c r="B243"/>
+        <v>403</v>
+      </c>
+      <c r="B243" s="12"/>
+      <c r="C243" s="9"/>
+      <c r="D243" s="12"/>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B244"/>
     </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>417</v>
+      </c>
+      <c r="B245"/>
+    </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246" s="2" t="s">
-        <v>7</v>
+      <c r="A246" t="s">
+        <v>418</v>
       </c>
       <c r="B246"/>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>22</v>
-      </c>
-      <c r="B247" s="14"/>
-      <c r="C247" s="17"/>
-      <c r="D247" s="12"/>
+        <v>426</v>
+      </c>
+      <c r="B247"/>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>11</v>
-      </c>
-      <c r="B248" s="14"/>
-      <c r="C248" s="17"/>
-      <c r="D248" s="12"/>
+        <v>427</v>
+      </c>
+      <c r="B248"/>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>12</v>
-      </c>
-      <c r="B249" s="14"/>
-      <c r="C249" s="17"/>
-      <c r="D249" s="12"/>
+        <v>428</v>
+      </c>
+      <c r="B249"/>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>13</v>
-      </c>
-      <c r="B250" s="14"/>
-      <c r="C250" s="17"/>
-      <c r="D250" s="12"/>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>14</v>
-      </c>
-      <c r="B251" s="14"/>
-      <c r="C251" s="17"/>
-      <c r="D251" s="12"/>
+        <v>429</v>
+      </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>23</v>
-      </c>
-      <c r="B252" s="14"/>
-      <c r="C252" s="17"/>
-      <c r="D252" s="12"/>
+      <c r="A252" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B252"/>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B253" s="14"/>
+      <c r="C253" s="17"/>
+      <c r="D253" s="12"/>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>11</v>
+      </c>
+      <c r="B254" s="14"/>
+      <c r="C254" s="17"/>
+      <c r="D254" s="12"/>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A255" s="2" t="s">
-        <v>143</v>
-      </c>
+      <c r="A255" t="s">
+        <v>12</v>
+      </c>
+      <c r="B255" s="14"/>
+      <c r="C255" s="17"/>
+      <c r="D255" s="12"/>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
+        <v>13</v>
+      </c>
+      <c r="B256" s="14"/>
+      <c r="C256" s="17"/>
+      <c r="D256" s="12"/>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>14</v>
+      </c>
+      <c r="B257" s="14"/>
+      <c r="C257" s="17"/>
+      <c r="D257" s="12"/>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>23</v>
+      </c>
+      <c r="B258" s="14"/>
+      <c r="C258" s="17"/>
+      <c r="D258" s="12"/>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
         <v>147</v>
       </c>
-      <c r="B256" s="11"/>
-      <c r="C256" s="16"/>
-      <c r="D256" s="9"/>
+      <c r="B262" s="11"/>
+      <c r="C262" s="16"/>
+      <c r="D262" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3596,7 +3664,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -3608,10 +3676,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A109"/>
+  <dimension ref="A1:A110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3641,7 +3709,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -3666,27 +3734,27 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -3696,32 +3764,32 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
@@ -3761,7 +3829,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -3786,22 +3854,22 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -3816,12 +3884,12 @@
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
@@ -3841,17 +3909,17 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
@@ -3896,7 +3964,7 @@
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
@@ -3926,42 +3994,42 @@
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
@@ -3981,37 +4049,37 @@
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
@@ -4041,42 +4109,47 @@
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>402</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -4102,13 +4175,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4131,7 +4204,7 @@
         <v>157</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C4" s="17"/>
     </row>
@@ -4140,7 +4213,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B6" s="7"/>
     </row>
@@ -4164,7 +4237,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B9" s="19">
         <v>40765</v>
@@ -4173,7 +4246,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B10" s="19">
         <v>40765</v>
@@ -4182,7 +4255,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B11" s="19">
         <v>40765</v>
@@ -4227,21 +4300,21 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="12"/>
@@ -4251,13 +4324,13 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B22" s="19">
         <v>40749</v>
@@ -4266,7 +4339,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B23" s="19">
         <v>40749</v>
@@ -4275,7 +4348,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B24" s="19">
         <v>40749</v>
@@ -4314,13 +4387,13 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B30" s="7"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B31" s="19">
         <v>40749</v>
@@ -4329,7 +4402,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B32" s="19">
         <v>40749</v>
@@ -4338,7 +4411,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B33" s="19">
         <v>40749</v>
@@ -4347,7 +4420,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B34" s="19">
         <v>40749</v>
@@ -4359,13 +4432,13 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B36" s="7"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B37" s="19">
         <v>40765</v>
@@ -4374,7 +4447,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B38" s="19">
         <v>40765</v>
@@ -4383,7 +4456,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B39" s="19">
         <v>40765</v>
@@ -4430,7 +4503,7 @@
         <v>186</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4455,7 +4528,7 @@
         <v>190</v>
       </c>
       <c r="D3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4482,7 +4555,7 @@
         <v>187</v>
       </c>
       <c r="D6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4521,60 +4594,60 @@
   <sheetData>
     <row r="1" spans="1:4" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" t="s">
         <v>233</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>234</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>235</v>
-      </c>
-      <c r="D4" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -4600,127 +4673,127 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -4744,60 +4817,60 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>375</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B4" t="s">
         <v>378</v>
-      </c>
-      <c r="B4" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>379</v>
+      </c>
+      <c r="B5" t="s">
         <v>380</v>
-      </c>
-      <c r="B5" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>381</v>
+      </c>
+      <c r="B6" t="s">
         <v>382</v>
-      </c>
-      <c r="B6" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>383</v>
+      </c>
+      <c r="B7" t="s">
         <v>384</v>
-      </c>
-      <c r="B7" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B8" t="s">
         <v>195</v>
@@ -4805,15 +4878,15 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>388</v>
+      </c>
+      <c r="B11" t="s">
         <v>389</v>
-      </c>
-      <c r="B11" t="s">
-        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the Options menu. Must redo the editor panels.
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18990" windowHeight="8610" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18990" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="459">
   <si>
     <t>Tweaking System</t>
   </si>
@@ -1363,6 +1363,42 @@
   </si>
   <si>
     <t>A maximum of 3 waves at the same time</t>
+  </si>
+  <si>
+    <t>Change the Sell icon for a circle with an X inside</t>
+  </si>
+  <si>
+    <t>Don't show the "toggle choices" help bar message if you cannot do it</t>
+  </si>
+  <si>
+    <t>Change the Turret menu for an "always same # of clicks" style</t>
+  </si>
+  <si>
+    <t>Make the "upgrade" choice always the first selected in the turret menu</t>
+  </si>
+  <si>
+    <t>Reset the spaceship velocity when the turret is installed</t>
+  </si>
+  <si>
+    <t>Try add momentum to bullets</t>
+  </si>
+  <si>
+    <t>Ethan Larson</t>
+  </si>
+  <si>
+    <t>Level design =&gt; strategy first, timing second</t>
+  </si>
+  <si>
+    <t>Ask people when they die why they think they died</t>
+  </si>
+  <si>
+    <t>Change the menus behavior</t>
+  </si>
+  <si>
+    <t>Add a time between the end of the level and being able to go to the next level</t>
+  </si>
+  <si>
+    <t>Play Savage Moon and Comet Crash</t>
   </si>
 </sst>
 </file>
@@ -1836,9 +1872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D262"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2005,7 +2041,7 @@
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="16"/>
-      <c r="D21" s="12"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2013,7 +2049,7 @@
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="16"/>
-      <c r="D22" s="12"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -3740,10 +3776,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A130"/>
+  <dimension ref="A1:A137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3866,438 +3902,473 @@
         <v>446</v>
       </c>
     </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>451</v>
+      </c>
+    </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>83</v>
+      <c r="A26" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>152</v>
+        <v>457</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>153</v>
+      <c r="A29" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>398</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>132</v>
+      <c r="A35" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>136</v>
+        <v>398</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>184</v>
+      <c r="A38" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>338</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>365</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>390</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>392</v>
+        <v>338</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>435</v>
+        <v>365</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>443</v>
+        <v>390</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>246</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>8</v>
+      <c r="A59" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>9</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>119</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>93</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>202</v>
+      <c r="A67" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>406</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>204</v>
+      <c r="A70" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>209</v>
+        <v>406</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>271</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>289</v>
+        <v>208</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>367</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>370</v>
+        <v>210</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>366</v>
+        <v>271</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>368</v>
+        <v>289</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>433</v>
+        <v>368</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>182</v>
+      <c r="A86" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>183</v>
+        <v>432</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>445</v>
+        <v>433</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>15</v>
+      <c r="A90" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>244</v>
+        <v>450</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>256</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>128</v>
+        <v>258</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>129</v>
+      <c r="A106" s="2" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>335</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>336</v>
+      <c r="A110" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
-        <v>337</v>
+      <c r="A112" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>333</v>
+        <v>129</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
         <v>401</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>440</v>
+        <v>402</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>441</v>
+        <v>104</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>442</v>
       </c>
     </row>
@@ -4309,11 +4380,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4616,7 +4687,30 @@
       <c r="B40" s="7"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>453</v>
+      </c>
       <c r="B41" s="7"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>458</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cancelable effect + new logo
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18990" windowHeight="8610"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18990" windowHeight="8610" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="464">
   <si>
     <t>Tweaking System</t>
   </si>
@@ -1399,6 +1399,21 @@
   </si>
   <si>
     <t>Play Savage Moon and Comet Crash</t>
+  </si>
+  <si>
+    <t>When turret installed, menu should go back to this turret if possible?</t>
+  </si>
+  <si>
+    <t>System for announcements / updates</t>
+  </si>
+  <si>
+    <t>System for downloadable content</t>
+  </si>
+  <si>
+    <t>Leaderboards</t>
+  </si>
+  <si>
+    <t>A general timer object to execute tasks later in time (useful for animations)</t>
   </si>
 </sst>
 </file>
@@ -1872,9 +1887,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D262"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3247,7 +3262,7 @@
       </c>
       <c r="B190" s="10"/>
       <c r="C190" s="9"/>
-      <c r="D190" s="12"/>
+      <c r="D190" s="16"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
@@ -3287,7 +3302,7 @@
       </c>
       <c r="B195" s="10"/>
       <c r="C195" s="9"/>
-      <c r="D195" s="12"/>
+      <c r="D195" s="9"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
@@ -3295,7 +3310,7 @@
       </c>
       <c r="B196" s="10"/>
       <c r="C196" s="9"/>
-      <c r="D196" s="16"/>
+      <c r="D196" s="9"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
@@ -3335,7 +3350,7 @@
       </c>
       <c r="B201" s="10"/>
       <c r="C201" s="16"/>
-      <c r="D201" s="12"/>
+      <c r="D201" s="9"/>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
@@ -3367,7 +3382,7 @@
       </c>
       <c r="B205" s="15"/>
       <c r="C205" s="16"/>
-      <c r="D205" s="12"/>
+      <c r="D205" s="9"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
@@ -3604,7 +3619,7 @@
       </c>
       <c r="B242" s="12"/>
       <c r="C242" s="9"/>
-      <c r="D242" s="12"/>
+      <c r="D242" s="9"/>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
@@ -3628,7 +3643,7 @@
       </c>
       <c r="B245" s="12"/>
       <c r="C245" s="9"/>
-      <c r="D245" s="12"/>
+      <c r="D245" s="9"/>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
@@ -3636,7 +3651,7 @@
       </c>
       <c r="B246" s="12"/>
       <c r="C246" s="16"/>
-      <c r="D246" s="12"/>
+      <c r="D246" s="9"/>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
@@ -3776,10 +3791,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A137"/>
+  <dimension ref="A1:A141"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4202,173 +4217,198 @@
         <v>450</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
         <v>254</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
         <v>257</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>304</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+      <c r="A116" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>337</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
-        <v>104</v>
+      <c r="A129" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>436</v>
+        <v>461</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>438</v>
+        <v>462</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>439</v>
+      <c r="A133" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>440</v>
+        <v>436</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
-        <v>441</v>
+      <c r="A136" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>442</v>
       </c>
     </row>
@@ -4384,7 +4424,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added visual cue at starting path when the next wave is coming
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="464">
   <si>
     <t>Tweaking System</t>
   </si>
@@ -1414,6 +1414,9 @@
   </si>
   <si>
     <t>Close player's spaceship menus (celestial body, turret menu, etc.) when dead (avoid clutter)</t>
+  </si>
+  <si>
+    <t>Power-Up that lengthen the time for the next wave (give more time to prepare)</t>
   </si>
 </sst>
 </file>
@@ -3775,8 +3778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3907,6 +3910,11 @@
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>388</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added mini no input state when game over
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="478">
   <si>
     <t>Tweaking System</t>
   </si>
@@ -1334,9 +1334,6 @@
     <t>Asset editor -&gt; create your own space drama</t>
   </si>
   <si>
-    <t>Things to accomplish in a level, a-la achievements</t>
-  </si>
-  <si>
     <t>Canceled or already done ideas</t>
   </si>
   <si>
@@ -1449,6 +1446,18 @@
   </si>
   <si>
     <t>Change IObjectPhysique for ICollidable</t>
+  </si>
+  <si>
+    <t>Challenges, a-la achievements</t>
+  </si>
+  <si>
+    <t>Don't show the helpbar for multiplayer</t>
+  </si>
+  <si>
+    <t>(Challenge) Start all the waves manually</t>
+  </si>
+  <si>
+    <t>(Challenge) Install only x turrets (0, 1, *)</t>
   </si>
 </sst>
 </file>
@@ -1561,7 +1570,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1609,6 +1618,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1919,8 +1931,8 @@
   <dimension ref="A1:D277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A152" sqref="A152"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3043,11 +3055,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3808,11 +3820,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B91" sqref="B91"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3829,13 +3841,13 @@
         <v>427</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>428</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3864,14 +3876,14 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="21"/>
@@ -3886,10 +3898,10 @@
         <v>115</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D8" t="s">
         <v>116</v>
@@ -3900,7 +3912,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C9" t="s">
         <v>309</v>
@@ -3917,7 +3929,7 @@
         <v>305</v>
       </c>
       <c r="C10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>433</v>
@@ -3927,6 +3939,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>474</v>
+      </c>
       <c r="D11" t="s">
         <v>434</v>
       </c>
@@ -3935,16 +3950,22 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>477</v>
+      </c>
       <c r="D12" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E12" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>476</v>
+      </c>
       <c r="D13" t="s">
-        <v>438</v>
+        <v>351</v>
       </c>
       <c r="E13" t="s">
         <v>111</v>
@@ -3952,16 +3973,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>351</v>
+        <v>443</v>
       </c>
       <c r="E14" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>444</v>
-      </c>
       <c r="E15" t="s">
         <v>237</v>
       </c>
@@ -3998,7 +4016,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -4017,7 +4035,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C23" t="s">
         <v>112</v>
@@ -4028,7 +4046,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C24" t="s">
         <v>254</v>
@@ -4039,7 +4057,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E25" t="s">
         <v>282</v>
@@ -4066,7 +4084,7 @@
         <v>392</v>
       </c>
       <c r="E30" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -4074,7 +4092,7 @@
         <v>425</v>
       </c>
       <c r="C31" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E31" t="s">
         <v>164</v>
@@ -4082,7 +4100,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -4097,7 +4115,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -4105,7 +4123,7 @@
         <v>413</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -4118,27 +4136,27 @@
         <v>163</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C41" s="21"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C42" s="21"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C43" s="21"/>
     </row>
@@ -4155,7 +4173,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E46" t="s">
         <v>283</v>
@@ -4163,17 +4181,17 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -4186,10 +4204,10 @@
         <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C52" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E52" t="s">
         <v>375</v>
@@ -4197,7 +4215,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -4227,7 +4245,7 @@
         <v>349</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E58" t="s">
         <v>284</v>
@@ -4245,31 +4263,28 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="7" t="s">
-        <v>466</v>
+      <c r="B60" t="s">
+        <v>469</v>
       </c>
       <c r="E60" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="7" t="s">
-        <v>356</v>
-      </c>
       <c r="E61" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>470</v>
-      </c>
       <c r="E62" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
+      <c r="E63" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="21"/>
@@ -4277,182 +4292,191 @@
         <v>144</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="22"/>
+      <c r="E65" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+      <c r="E66" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C70" s="21"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="20" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C71" s="21"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="20" t="s">
         <v>407</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>410</v>
       </c>
-      <c r="C71" s="6"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
+      <c r="C72" s="6"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
         <v>408</v>
       </c>
-      <c r="C72" s="6"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+      <c r="C73" s="6"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>409</v>
       </c>
-      <c r="C73" s="6"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+      <c r="C74" s="6"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C75" s="21"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="20" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C76" s="21"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="C76" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+      <c r="C77" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>337</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C79" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="20" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="20" t="s">
         <v>416</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>359</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="21"/>
-    </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="20" t="s">
+      <c r="C84" s="21"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="20" t="s">
         <v>417</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>222</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
+        <v>471</v>
+      </c>
+      <c r="D85" t="s">
         <v>472</v>
       </c>
-      <c r="D84" t="s">
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>364</v>
+      </c>
+      <c r="D86" t="s">
         <v>473</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
-        <v>364</v>
-      </c>
-      <c r="D85" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D86" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D87" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C89" s="21"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C92" s="21"/>
-    </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C118" s="21"/>
-    </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C122" s="21"/>
-    </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C125" s="21"/>
-    </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C132" s="21"/>
-    </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C135" s="21"/>
-    </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C138" s="21"/>
-    </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C144" s="21"/>
-    </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C147" s="21"/>
-    </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C150" s="21"/>
-    </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C153" s="21"/>
-    </row>
-    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C156" s="21"/>
-    </row>
-    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C160" s="21"/>
-    </row>
-    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C165" s="21"/>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C90" s="21"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C93" s="21"/>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C119" s="21"/>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C123" s="21"/>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C126" s="21"/>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C133" s="21"/>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C136" s="21"/>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C139" s="21"/>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" s="21"/>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C148" s="21"/>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C151" s="21"/>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C154" s="21"/>
+    </row>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C157" s="21"/>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C161" s="21"/>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C166" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added things to do by priorities
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -4,27 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18990" windowHeight="8610" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18990" windowHeight="8610" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
     <sheet name="Completed Tasks" sheetId="14" r:id="rId2"/>
     <sheet name="Ideas" sheetId="4" r:id="rId3"/>
-    <sheet name="Experts" sheetId="5" r:id="rId4"/>
-    <sheet name="Competitions" sheetId="6" r:id="rId5"/>
-    <sheet name="Credits &amp; mentions" sheetId="8" r:id="rId6"/>
-    <sheet name="Weekly meeting #1" sheetId="9" state="hidden" r:id="rId7"/>
-    <sheet name="Playtesting" sheetId="10" r:id="rId8"/>
-    <sheet name="Tutorial" sheetId="11" r:id="rId9"/>
-    <sheet name="Git strategy" sheetId="12" r:id="rId10"/>
-    <sheet name="Future tasks" sheetId="15" r:id="rId11"/>
+    <sheet name="Priorities" sheetId="16" r:id="rId4"/>
+    <sheet name="Experts" sheetId="5" r:id="rId5"/>
+    <sheet name="Competitions" sheetId="6" r:id="rId6"/>
+    <sheet name="Credits &amp; mentions" sheetId="8" r:id="rId7"/>
+    <sheet name="Weekly meeting #1" sheetId="9" state="hidden" r:id="rId8"/>
+    <sheet name="Playtesting" sheetId="10" r:id="rId9"/>
+    <sheet name="Tutorial" sheetId="11" r:id="rId10"/>
+    <sheet name="Git strategy" sheetId="12" r:id="rId11"/>
+    <sheet name="Future tasks" sheetId="15" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="489">
   <si>
     <t>Tweaking System</t>
   </si>
@@ -1458,6 +1459,39 @@
   </si>
   <si>
     <t>(Challenge) Install only x turrets (0, 1, *)</t>
+  </si>
+  <si>
+    <t>Highest</t>
+  </si>
+  <si>
+    <t>Lowest</t>
+  </si>
+  <si>
+    <t>News controller</t>
+  </si>
+  <si>
+    <t>Downloadable content controller</t>
+  </si>
+  <si>
+    <t>PC version</t>
+  </si>
+  <si>
+    <t>Xbox 360 version</t>
+  </si>
+  <si>
+    <t>WPM7 version</t>
+  </si>
+  <si>
+    <t>PC demo</t>
+  </si>
+  <si>
+    <t>Xbox 360 demo</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Music</t>
   </si>
 </sst>
 </file>
@@ -1570,7 +1604,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1618,6 +1652,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1931,8 +1968,8 @@
   <dimension ref="A1:D277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C153" sqref="C153"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2208,7 +2245,7 @@
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="7"/>
-      <c r="D38" s="10"/>
+      <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -3040,6 +3077,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -3055,11 +3106,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>376</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3125,7 +3176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -3169,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3822,9 +3873,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4023,8 +4074,8 @@
       <c r="A22" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B22" t="s">
-        <v>421</v>
+      <c r="B22" s="7" t="s">
+        <v>450</v>
       </c>
       <c r="C22" t="s">
         <v>109</v>
@@ -4034,8 +4085,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
-        <v>450</v>
+      <c r="B23" t="s">
+        <v>451</v>
       </c>
       <c r="C23" t="s">
         <v>112</v>
@@ -4045,9 +4096,6 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>451</v>
-      </c>
       <c r="C24" t="s">
         <v>254</v>
       </c>
@@ -4073,6 +4121,11 @@
         <v>281</v>
       </c>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>421</v>
+      </c>
+    </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
         <v>394</v>
@@ -4241,31 +4294,22 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>466</v>
+      <c r="B58" t="s">
+        <v>469</v>
+      </c>
+      <c r="C58" t="s">
+        <v>166</v>
       </c>
       <c r="E58" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C59" t="s">
-        <v>166</v>
-      </c>
       <c r="E59" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>469</v>
-      </c>
       <c r="E60" t="s">
         <v>338</v>
       </c>
@@ -4313,15 +4357,24 @@
       <c r="B67" t="s">
         <v>341</v>
       </c>
+      <c r="E67" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>342</v>
       </c>
+      <c r="E68" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>343</v>
+      </c>
+      <c r="E69" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -4486,11 +4539,105 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>479</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4672,11 +4819,13 @@
       <c r="A35" t="s">
         <v>203</v>
       </c>
+      <c r="B35" s="10"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>204</v>
       </c>
+      <c r="B36" s="10"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -4710,21 +4859,25 @@
       <c r="A45" t="s">
         <v>353</v>
       </c>
+      <c r="B45" s="7"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>354</v>
       </c>
+      <c r="B46" s="10"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>355</v>
       </c>
+      <c r="B47" s="7"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>357</v>
       </c>
+      <c r="B48" s="10"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
@@ -4752,7 +4905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -4854,7 +5007,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -4933,7 +5086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A29"/>
   <sheetViews>
@@ -5078,7 +5231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
@@ -5180,18 +5333,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
First version of a ColoredText object.
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18990" windowHeight="8610" activeTab="12"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18990" windowHeight="8610" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="534">
   <si>
     <t>Tweaking System</t>
   </si>
@@ -1348,9 +1348,6 @@
     <t>Add a cost per bullet fired</t>
   </si>
   <si>
-    <t>Add a shield around the starting path object that destroy the bullets</t>
-  </si>
-  <si>
     <t>Start a maximum of 3 waves at the same time</t>
   </si>
   <si>
@@ -1514,6 +1511,123 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Know why you are indie</t>
+  </si>
+  <si>
+    <t>Know how to structure your company</t>
+  </si>
+  <si>
+    <t>Be able to do an elevator pitch</t>
+  </si>
+  <si>
+    <t>People invest in companies / business models / teams. Focus on that with investors.</t>
+  </si>
+  <si>
+    <t>How will you structure your funnel?</t>
+  </si>
+  <si>
+    <t>Pink player with red choice is unreadable</t>
+  </si>
+  <si>
+    <t>Better handling of the spaceship bullet damage (override in level descriptor?)</t>
+  </si>
+  <si>
+    <t>Make the spaceship float around a little bit when speed = = 0</t>
+  </si>
+  <si>
+    <t>2x new game =&gt; crash</t>
+  </si>
+  <si>
+    <t>Options seem to not save without a proper exit</t>
+  </si>
+  <si>
+    <t>Transmedia is making WP7 games =&gt; partnership?</t>
+  </si>
+  <si>
+    <t>Business cards</t>
+  </si>
+  <si>
+    <t>Add a "keyboard only" mode</t>
+  </si>
+  <si>
+    <t>The small planet is maybe too small</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Try to use the spacebar to make a selection, R/F to navigate choices, Left button to fire</t>
+  </si>
+  <si>
+    <t>Don't move the menus if you don't have to</t>
+  </si>
+  <si>
+    <t>Try to layout your game mechanics like this: shooting -&gt; grav. turret -&gt; upgrade turret</t>
+  </si>
+  <si>
+    <t>Preview the gravitational turret, level 2</t>
+  </si>
+  <si>
+    <t>Alienship stay red while spawning enemies</t>
+  </si>
+  <si>
+    <t>(SS addon) Shield that permit to bump in enemies</t>
+  </si>
+  <si>
+    <t>In pause menu, ghost ship</t>
+  </si>
+  <si>
+    <t>In pause menu, put the circles before the text or the text inside a tube</t>
+  </si>
+  <si>
+    <t>Add a shield around the starting path object that destroy/deflect the bullets (avoid camping)</t>
+  </si>
+  <si>
+    <t>In first levels, waves start when the player is ready</t>
+  </si>
+  <si>
+    <t>(Msg) Moons are your life</t>
+  </si>
+  <si>
+    <t>Make the next wave effect more obvious</t>
+  </si>
+  <si>
+    <t>Spaceship warp in / warp out effect</t>
+  </si>
+  <si>
+    <t>(Msg) Turret range</t>
+  </si>
+  <si>
+    <t>Next level directly in the winning bubble</t>
+  </si>
+  <si>
+    <t>Can still move when the level is completed</t>
+  </si>
+  <si>
+    <t>Find a way to make it obvious that the overlap of the turret with the path is important</t>
+  </si>
+  <si>
+    <t>(Msg) Upgrade turret</t>
+  </si>
+  <si>
+    <t>More life on the planet to protect =&gt; can make more mistakes &amp; can save more the day</t>
+  </si>
+  <si>
+    <t>Make the crash report screen more user friendly, controller specific and for Windows only</t>
+  </si>
+  <si>
+    <t>Use SlimDX for gamepad input on PC (Windows only)</t>
+  </si>
+  <si>
+    <t>Check for MonoGame (could make the game works on iOS, Android, Mac, Linux)</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Get incorporated</t>
   </si>
 </sst>
 </file>
@@ -1626,7 +1740,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1682,6 +1796,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1990,11 +2107,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D277"/>
+  <dimension ref="A1:D279"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2320,112 +2437,109 @@
       <c r="C44" s="14"/>
       <c r="D44" s="10"/>
     </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>503</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="10"/>
+    </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>399</v>
       </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="10"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="B49" s="10"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="10"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>96</v>
-      </c>
-      <c r="B50" s="12"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="14"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>97</v>
-      </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>24</v>
-      </c>
-      <c r="B52" s="8"/>
+        <v>96</v>
+      </c>
+      <c r="B52" s="12"/>
       <c r="C52" s="7"/>
       <c r="D52" s="14"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="B53" s="8"/>
-      <c r="C53" s="10"/>
+      <c r="C53" s="14"/>
       <c r="D53" s="14"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B54" s="8"/>
-      <c r="C54" s="10"/>
+      <c r="C54" s="7"/>
       <c r="D54" s="14"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="14"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="14"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>49</v>
       </c>
-      <c r="B55" s="8"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="10"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+      <c r="B57" s="8"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="10"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>21</v>
-      </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="10"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>22</v>
-      </c>
-      <c r="B59" s="8"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="10"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B60" s="8"/>
-      <c r="C60" s="10"/>
+      <c r="C60" s="7"/>
       <c r="D60" s="10"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B61" s="8"/>
-      <c r="C61" s="10"/>
+      <c r="C61" s="14"/>
       <c r="D61" s="10"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="10"/>
@@ -2433,52 +2547,52 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B63" s="8"/>
-      <c r="C63" s="14"/>
+      <c r="C63" s="10"/>
       <c r="D63" s="10"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B64" s="8"/>
-      <c r="C64" s="7"/>
+      <c r="C64" s="10"/>
       <c r="D64" s="10"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>33</v>
+      </c>
+      <c r="B65" s="8"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="10"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>50</v>
+      </c>
+      <c r="B66" s="8"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="10"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>53</v>
       </c>
-      <c r="B65" s="8"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+      <c r="B67" s="8"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>39</v>
-      </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="10"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>40</v>
-      </c>
-      <c r="B69" s="8"/>
-      <c r="C69" s="15"/>
-      <c r="D69" s="10"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B70" s="8"/>
       <c r="C70" s="15"/>
@@ -2486,7 +2600,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B71" s="8"/>
       <c r="C71" s="15"/>
@@ -2494,7 +2608,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="15"/>
@@ -2502,7 +2616,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B73" s="8"/>
       <c r="C73" s="15"/>
@@ -2510,7 +2624,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B74" s="8"/>
       <c r="C74" s="15"/>
@@ -2518,7 +2632,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B75" s="8"/>
       <c r="C75" s="15"/>
@@ -2526,7 +2640,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B76" s="8"/>
       <c r="C76" s="15"/>
@@ -2534,102 +2648,102 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B77" s="8"/>
       <c r="C77" s="15"/>
       <c r="D77" s="10"/>
     </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>44</v>
+      </c>
+      <c r="B78" s="8"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="10"/>
+    </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+      <c r="A79" t="s">
+        <v>54</v>
+      </c>
+      <c r="B79" s="8"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="10"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="B80" s="8"/>
-      <c r="C80" s="7"/>
-      <c r="D80" s="10"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
+      <c r="B82" s="8"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="10"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B81" s="8"/>
-      <c r="C81" s="7"/>
-      <c r="D81" s="10"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="B83" s="8"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="10"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>318</v>
       </c>
-      <c r="B82" s="8"/>
-      <c r="C82" s="14"/>
-      <c r="D82" s="10"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="B84" s="8"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="10"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>319</v>
       </c>
-      <c r="B83" s="8"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="10"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+      <c r="B85" s="8"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="10"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>400</v>
-      </c>
-      <c r="B86" s="8"/>
-      <c r="C86" s="7"/>
-      <c r="D86" s="10"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>320</v>
-      </c>
-      <c r="B87" s="8"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="10"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>400</v>
+      </c>
+      <c r="B88" s="8"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="10"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>320</v>
+      </c>
+      <c r="B89" s="8"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="10"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>321</v>
       </c>
-      <c r="B88" s="8"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="10"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+      <c r="B90" s="8"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="10"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>55</v>
-      </c>
-      <c r="B91" s="13"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="10"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>56</v>
-      </c>
-      <c r="B92" s="13"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B93" s="13"/>
       <c r="C93" s="7"/>
@@ -2637,15 +2751,15 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B94" s="13"/>
-      <c r="C94" s="14"/>
+      <c r="C94" s="10"/>
       <c r="D94" s="10"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B95" s="13"/>
       <c r="C95" s="7"/>
@@ -2653,31 +2767,31 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B96" s="13"/>
-      <c r="C96" s="10"/>
+      <c r="C96" s="14"/>
       <c r="D96" s="10"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B97" s="13"/>
-      <c r="C97" s="10"/>
+      <c r="C97" s="7"/>
       <c r="D97" s="10"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>137</v>
+        <v>60</v>
       </c>
       <c r="B98" s="13"/>
-      <c r="C98" s="7"/>
+      <c r="C98" s="10"/>
       <c r="D98" s="10"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B99" s="13"/>
       <c r="C99" s="10"/>
@@ -2685,115 +2799,115 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="B100" s="13"/>
-      <c r="C100" s="14"/>
+      <c r="C100" s="7"/>
       <c r="D100" s="10"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B101" s="13"/>
-      <c r="C101" s="7"/>
+      <c r="C101" s="10"/>
       <c r="D101" s="10"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B102" s="13"/>
-      <c r="C102" s="7"/>
+      <c r="C102" s="14"/>
       <c r="D102" s="10"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B103" s="13"/>
       <c r="C103" s="7"/>
       <c r="D103" s="10"/>
     </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>64</v>
+      </c>
+      <c r="B104" s="13"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="10"/>
+    </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
+      <c r="A105" t="s">
+        <v>66</v>
+      </c>
+      <c r="B105" s="13"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="10"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>210</v>
-      </c>
-      <c r="B106" s="8"/>
-      <c r="C106" s="14"/>
-      <c r="D106" s="10"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>211</v>
-      </c>
-      <c r="B107" s="8"/>
-      <c r="C107" s="14"/>
-      <c r="D107" s="10"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B108" s="8"/>
       <c r="C108" s="14"/>
       <c r="D108" s="10"/>
     </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>211</v>
+      </c>
+      <c r="B109" s="8"/>
+      <c r="C109" s="14"/>
+      <c r="D109" s="10"/>
+    </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+      <c r="A110" t="s">
+        <v>212</v>
+      </c>
+      <c r="B110" s="8"/>
+      <c r="C110" s="14"/>
+      <c r="D110" s="10"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>105</v>
       </c>
-      <c r="B111" s="9"/>
-      <c r="C111" s="7"/>
-      <c r="D111" s="10"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
+      <c r="B113" s="9"/>
+      <c r="C113" s="7"/>
+      <c r="D113" s="10"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B115"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B117"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>71</v>
-      </c>
-      <c r="B117" s="12"/>
-      <c r="C117" s="14"/>
-      <c r="D117" s="10"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>72</v>
-      </c>
-      <c r="B118" s="12"/>
-      <c r="C118" s="10"/>
-      <c r="D118" s="10"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B119" s="12"/>
       <c r="C119" s="14"/>
@@ -2801,31 +2915,31 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B120" s="12"/>
-      <c r="C120" s="7"/>
+      <c r="C120" s="10"/>
       <c r="D120" s="10"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>75</v>
-      </c>
-      <c r="B121" s="9"/>
+        <v>73</v>
+      </c>
+      <c r="B121" s="12"/>
       <c r="C121" s="14"/>
       <c r="D121" s="10"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>98</v>
-      </c>
-      <c r="B122" s="9"/>
+        <v>74</v>
+      </c>
+      <c r="B122" s="12"/>
       <c r="C122" s="7"/>
       <c r="D122" s="10"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="B123" s="9"/>
       <c r="C123" s="14"/>
@@ -2833,63 +2947,63 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>168</v>
-      </c>
-      <c r="B124" s="12"/>
+        <v>98</v>
+      </c>
+      <c r="B124" s="9"/>
       <c r="C124" s="7"/>
       <c r="D124" s="10"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>169</v>
-      </c>
-      <c r="B125" s="12"/>
-      <c r="C125" s="7"/>
+        <v>99</v>
+      </c>
+      <c r="B125" s="9"/>
+      <c r="C125" s="14"/>
       <c r="D125" s="10"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>332</v>
-      </c>
-      <c r="B126" s="13"/>
+        <v>168</v>
+      </c>
+      <c r="B126" s="12"/>
       <c r="C126" s="7"/>
       <c r="D126" s="10"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="B127" s="12"/>
-      <c r="C127" s="10"/>
+      <c r="C127" s="7"/>
       <c r="D127" s="10"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>199</v>
-      </c>
-      <c r="B128" s="12"/>
-      <c r="C128" s="10"/>
+        <v>332</v>
+      </c>
+      <c r="B128" s="13"/>
+      <c r="C128" s="7"/>
       <c r="D128" s="10"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>327</v>
-      </c>
-      <c r="B129" s="9"/>
-      <c r="C129" s="7"/>
-      <c r="D129" s="8"/>
+        <v>198</v>
+      </c>
+      <c r="B129" s="12"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>329</v>
-      </c>
-      <c r="B130" s="8"/>
+        <v>199</v>
+      </c>
+      <c r="B130" s="12"/>
       <c r="C130" s="10"/>
-      <c r="D130" s="8"/>
+      <c r="D130" s="10"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B131" s="9"/>
       <c r="C131" s="7"/>
@@ -2897,44 +3011,44 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>329</v>
+      </c>
+      <c r="B132" s="8"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="8"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>330</v>
+      </c>
+      <c r="B133" s="9"/>
+      <c r="C133" s="7"/>
+      <c r="D133" s="8"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>369</v>
       </c>
-      <c r="B132" s="8"/>
-      <c r="C132" s="7"/>
-      <c r="D132" s="8"/>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
+      <c r="B134" s="8"/>
+      <c r="C134" s="7"/>
+      <c r="D134" s="8"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>81</v>
-      </c>
-      <c r="B135" s="13"/>
-      <c r="C135" s="7"/>
-      <c r="D135" s="10"/>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>82</v>
-      </c>
-      <c r="B136" s="8"/>
-      <c r="C136" s="7"/>
-      <c r="D136" s="14"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>84</v>
-      </c>
-      <c r="B137" s="8"/>
+        <v>81</v>
+      </c>
+      <c r="B137" s="13"/>
       <c r="C137" s="7"/>
       <c r="D137" s="10"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B138" s="8"/>
       <c r="C138" s="7"/>
@@ -2942,47 +3056,47 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>167</v>
-      </c>
-      <c r="B139" s="13"/>
+        <v>84</v>
+      </c>
+      <c r="B139" s="8"/>
       <c r="C139" s="7"/>
       <c r="D139" s="10"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>213</v>
+        <v>85</v>
       </c>
       <c r="B140" s="8"/>
-      <c r="C140" s="10"/>
-      <c r="D140" s="10"/>
+      <c r="C140" s="7"/>
+      <c r="D140" s="14"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>231</v>
+        <v>167</v>
       </c>
       <c r="B141" s="13"/>
-      <c r="C141" s="10"/>
+      <c r="C141" s="7"/>
       <c r="D141" s="10"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>323</v>
+        <v>213</v>
       </c>
       <c r="B142" s="8"/>
-      <c r="C142" s="13"/>
+      <c r="C142" s="10"/>
       <c r="D142" s="10"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>322</v>
-      </c>
-      <c r="B143" s="8"/>
-      <c r="C143" s="13"/>
+        <v>231</v>
+      </c>
+      <c r="B143" s="13"/>
+      <c r="C143" s="10"/>
       <c r="D143" s="10"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>371</v>
+        <v>323</v>
       </c>
       <c r="B144" s="8"/>
       <c r="C144" s="13"/>
@@ -2990,21 +3104,31 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>372</v>
+        <v>322</v>
       </c>
       <c r="B145" s="8"/>
       <c r="C145" s="13"/>
       <c r="D145" s="10"/>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B174"/>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>371</v>
+      </c>
+      <c r="B146" s="8"/>
+      <c r="C146" s="13"/>
+      <c r="D146" s="10"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>372</v>
+      </c>
+      <c r="B147" s="8"/>
+      <c r="C147" s="13"/>
+      <c r="D147" s="10"/>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177"/>
-    </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B178"/>
     </row>
@@ -3029,14 +3153,14 @@
     <row r="185" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B185"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B188"/>
-    </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B202"/>
-    </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B203"/>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B186"/>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B187"/>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B190"/>
     </row>
     <row r="204" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B204"/>
@@ -3053,14 +3177,14 @@
     <row r="208" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B208"/>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="19"/>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B223"/>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B209"/>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B210"/>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B224"/>
+      <c r="A224" s="19"/>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B225"/>
@@ -3068,21 +3192,21 @@
     <row r="226" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B226"/>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B264"/>
-    </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B265"/>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B227"/>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B228"/>
     </row>
     <row r="266" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B266"/>
     </row>
+    <row r="267" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B267"/>
+    </row>
     <row r="268" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B268"/>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B269"/>
-    </row>
     <row r="270" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B270"/>
     </row>
@@ -3092,8 +3216,14 @@
     <row r="272" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B272"/>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" s="2"/>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B273"/>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B274"/>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3131,11 +3261,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>376</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3245,8 +3375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3257,10 +3387,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
+        <v>493</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>494</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3931,11 +4061,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B108" sqref="B108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3952,7 +4082,7 @@
         <v>427</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>428</v>
@@ -3970,32 +4100,32 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="21"/>
+      <c r="E2" s="6" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>431</v>
+        <v>438</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="21"/>
+      <c r="E3" s="6" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="21"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
-        <v>438</v>
-      </c>
       <c r="C5" s="6"/>
       <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
-        <v>439</v>
-      </c>
       <c r="C6" s="6"/>
       <c r="D6" s="21"/>
     </row>
@@ -4009,10 +4139,10 @@
         <v>115</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>440</v>
+        <v>518</v>
       </c>
       <c r="C8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D8" t="s">
         <v>116</v>
@@ -4023,7 +4153,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C9" t="s">
         <v>309</v>
@@ -4040,7 +4170,7 @@
         <v>305</v>
       </c>
       <c r="C10" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>433</v>
@@ -4050,8 +4180,11 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>501</v>
+      </c>
       <c r="C11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D11" t="s">
         <v>434</v>
@@ -4061,8 +4194,11 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>512</v>
+      </c>
       <c r="C12" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D12" t="s">
         <v>437</v>
@@ -4072,8 +4208,11 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>525</v>
+      </c>
       <c r="C13" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D13" t="s">
         <v>351</v>
@@ -4084,16 +4223,19 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E14" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>515</v>
+      </c>
       <c r="E15" t="s">
         <v>237</v>
       </c>
@@ -4130,7 +4272,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -4138,7 +4280,7 @@
         <v>108</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C22" t="s">
         <v>109</v>
@@ -4149,7 +4291,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C23" t="s">
         <v>112</v>
@@ -4160,7 +4302,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C24" t="s">
         <v>254</v>
@@ -4170,430 +4312,557 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>500</v>
+      </c>
       <c r="C25" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E25" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>502</v>
+      </c>
+      <c r="C26" t="s">
+        <v>524</v>
+      </c>
       <c r="E26" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>508</v>
+      </c>
       <c r="E27" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>511</v>
+      </c>
       <c r="E28" t="s">
         <v>421</v>
       </c>
     </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
+      <c r="B29" t="s">
+        <v>516</v>
+      </c>
+    </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="25"/>
+      <c r="B30" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>411</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C32" t="s">
         <v>392</v>
       </c>
-      <c r="E30" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>425</v>
-      </c>
-      <c r="C31" t="s">
-        <v>464</v>
-      </c>
-      <c r="E31" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>447</v>
+      <c r="E32" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>420</v>
+        <v>425</v>
+      </c>
+      <c r="C33" t="s">
+        <v>463</v>
+      </c>
+      <c r="E33" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="7" t="s">
-        <v>345</v>
+      <c r="B34" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>449</v>
+        <v>420</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>491</v>
+      <c r="B36" s="7" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
+      <c r="B38" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="25"/>
+      <c r="B39" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="25"/>
+      <c r="B40" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="25"/>
+      <c r="B41" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="25"/>
+      <c r="B42" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="25"/>
+      <c r="B43" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="24" t="s">
         <v>413</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="B45" s="7" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B48" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="C42" s="21"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>467</v>
-      </c>
-      <c r="C43" s="21"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>468</v>
-      </c>
-      <c r="C44" s="21"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" t="s">
-        <v>113</v>
-      </c>
-      <c r="E46" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>452</v>
-      </c>
-      <c r="E47" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>454</v>
+      <c r="C49" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>455</v>
+        <v>466</v>
+      </c>
+      <c r="C50" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>412</v>
-      </c>
+        <v>467</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="25"/>
+      <c r="C52" s="25"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B53" t="s">
-        <v>458</v>
-      </c>
-      <c r="C53" t="s">
-        <v>456</v>
-      </c>
-      <c r="E53" t="s">
-        <v>375</v>
-      </c>
+      <c r="A53" s="25"/>
+      <c r="C53" s="25"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>457</v>
-      </c>
+      <c r="A54" s="25"/>
+      <c r="C54" s="25"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>113</v>
+      </c>
+      <c r="E56" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>451</v>
+      </c>
+      <c r="E57" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="C58" t="s">
-        <v>339</v>
-      </c>
-      <c r="E58" t="s">
-        <v>165</v>
+      <c r="B58" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>469</v>
-      </c>
-      <c r="C59" t="s">
-        <v>166</v>
-      </c>
-      <c r="E59" t="s">
-        <v>284</v>
+        <v>453</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E60" t="s">
-        <v>286</v>
+      <c r="B60" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E61" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E62" t="s">
-        <v>229</v>
+      <c r="B61" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E64" t="s">
-        <v>465</v>
+        <v>375</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E65" t="s">
-        <v>144</v>
-      </c>
+      <c r="A65" s="25"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E66" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="B67" t="s">
-        <v>340</v>
-      </c>
-      <c r="E67" t="s">
-        <v>356</v>
-      </c>
+      <c r="A66" s="25"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="24" t="s">
+        <v>101</v>
+      </c>
       <c r="B68" t="s">
-        <v>341</v>
-      </c>
-      <c r="E68" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>342</v>
-      </c>
-      <c r="E69" t="s">
-        <v>349</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>343</v>
+      <c r="A70" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C70" t="s">
+        <v>339</v>
       </c>
       <c r="E70" t="s">
-        <v>466</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>344</v>
+        <v>468</v>
+      </c>
+      <c r="C71" t="s">
+        <v>166</v>
+      </c>
+      <c r="E71" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C72" s="21"/>
+      <c r="E72" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
-        <v>407</v>
+        <v>509</v>
       </c>
       <c r="B73" t="s">
-        <v>410</v>
-      </c>
-      <c r="C73" s="6"/>
+        <v>507</v>
+      </c>
+      <c r="E73" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
+        <v>510</v>
+      </c>
+      <c r="E74" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B79" t="s">
+        <v>340</v>
+      </c>
+      <c r="E79" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>341</v>
+      </c>
+      <c r="E80" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>342</v>
+      </c>
+      <c r="E81" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>343</v>
+      </c>
+      <c r="E82" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C84" s="21"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="24" t="s">
+        <v>407</v>
+      </c>
+      <c r="B85" t="s">
+        <v>410</v>
+      </c>
+      <c r="C85" s="6"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>408</v>
       </c>
-      <c r="C74" s="6"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+      <c r="C86" s="6"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
         <v>409</v>
       </c>
-      <c r="C75" s="6"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+      <c r="C87" s="6"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C77" s="21"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="24" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="25"/>
+      <c r="B89" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C90" s="21"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="C78" t="s">
+      <c r="B91" t="s">
+        <v>528</v>
+      </c>
+      <c r="C91" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="25"/>
+      <c r="C92" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="25"/>
+      <c r="B93" s="19"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="25"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="25"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="B97" t="s">
+        <v>337</v>
+      </c>
+      <c r="C97" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="25"/>
+      <c r="B98" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="B100" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C103" s="21"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="24" t="s">
+        <v>417</v>
+      </c>
+      <c r="B104" t="s">
+        <v>222</v>
+      </c>
+      <c r="C104" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="24" t="s">
-        <v>253</v>
-      </c>
-      <c r="B80" t="s">
-        <v>337</v>
-      </c>
-      <c r="C80" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="24" t="s">
-        <v>416</v>
-      </c>
-      <c r="B82" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="21"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="24" t="s">
-        <v>417</v>
-      </c>
-      <c r="B86" t="s">
-        <v>222</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="D104" t="s">
         <v>471</v>
       </c>
-      <c r="D86" t="s">
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="C105" t="s">
+        <v>364</v>
+      </c>
+      <c r="D105" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C87" t="s">
-        <v>364</v>
-      </c>
-      <c r="D87" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D88" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D89" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="24" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="24" t="s">
         <v>383</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B109" t="s">
+        <v>491</v>
+      </c>
+      <c r="C109" s="21"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
         <v>492</v>
       </c>
-      <c r="C91" s="21"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C94" s="21"/>
-    </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C120" s="21"/>
-    </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C124" s="21"/>
-    </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C127" s="21"/>
-    </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C134" s="21"/>
-    </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C137" s="21"/>
-    </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C140" s="21"/>
-    </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C146" s="21"/>
-    </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C149" s="21"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="24" t="s">
+        <v>532</v>
+      </c>
+      <c r="B112" t="s">
+        <v>533</v>
+      </c>
+      <c r="C112" s="21"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116" t="s">
+        <v>457</v>
+      </c>
+      <c r="C116" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C138" s="21"/>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C142" s="21"/>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" s="21"/>
     </row>
     <row r="152" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C152" s="21"/>
@@ -4604,11 +4873,26 @@
     <row r="158" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C158" s="21"/>
     </row>
-    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C162" s="21"/>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C164" s="21"/>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C167" s="21"/>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C170" s="21"/>
+    </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C173" s="21"/>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C176" s="21"/>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C180" s="21"/>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C185" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4631,37 +4915,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -4671,17 +4955,17 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
@@ -4696,12 +4980,12 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -4712,11 +4996,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4976,6 +5260,31 @@
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>363</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -4990,7 +5299,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modified things to do.
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18990" windowHeight="8610"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18990" windowHeight="8610" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="543">
   <si>
     <t>Tweaking System</t>
   </si>
@@ -1640,6 +1640,21 @@
   </si>
   <si>
     <t>Add Starting Position</t>
+  </si>
+  <si>
+    <t>Manually change starting positions for already made levels</t>
+  </si>
+  <si>
+    <t>More comprehensible pause menu</t>
+  </si>
+  <si>
+    <t>Only disable next level and stuff buttons when game is over (to let the spaceship still fly around)</t>
+  </si>
+  <si>
+    <t>Pool the animations in the GUI/Animations folder</t>
+  </si>
+  <si>
+    <t>Power-Ups</t>
   </si>
 </sst>
 </file>
@@ -1793,9 +1808,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1805,6 +1817,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2119,11 +2134,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D278"/>
+  <dimension ref="A1:D279"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A112" sqref="A112"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2172,24 +2187,21 @@
       <c r="D5" s="10"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="10"/>
+      <c r="A7" s="26" t="s">
+        <v>542</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="13"/>
-      <c r="C8" s="7"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="7"/>
@@ -2197,23 +2209,23 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>94</v>
       </c>
       <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="13"/>
-      <c r="C11" s="7"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="7"/>
@@ -2221,232 +2233,232 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="7"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>106</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="14"/>
+        <v>333</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>333</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
+        <v>313</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>334</v>
+        <v>420</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="7"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>369</v>
-      </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="10"/>
-    </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>313</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="10"/>
+      <c r="A21" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>222</v>
+        <v>397</v>
       </c>
       <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>420</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="10"/>
-    </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>404</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="10"/>
+      <c r="A24" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="14"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>397</v>
-      </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="14"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="14"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="14"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>95</v>
-      </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="14"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>96</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
+        <v>48</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="10"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="14"/>
+      <c r="A32" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B33" s="8"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="14"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="10"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B34" s="8"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="B35" s="8"/>
-      <c r="C35" s="14"/>
+      <c r="C35" s="10"/>
       <c r="D35" s="10"/>
     </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+    </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B38" s="8"/>
-      <c r="C38" s="7"/>
+      <c r="C38" s="14"/>
       <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B39" s="8"/>
-      <c r="C39" s="14"/>
+      <c r="C39" s="7"/>
       <c r="D39" s="10"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>23</v>
-      </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-    </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
+      <c r="A42" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B43" s="8"/>
-      <c r="C43" s="14"/>
+      <c r="C43" s="15"/>
       <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B44" s="8"/>
-      <c r="C44" s="7"/>
+      <c r="C44" s="15"/>
       <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B45" s="8"/>
-      <c r="C45" s="10"/>
+      <c r="C45" s="15"/>
       <c r="D45" s="10"/>
     </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="10"/>
+    </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="15"/>
@@ -2454,7 +2466,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="15"/>
@@ -2462,7 +2474,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="15"/>
@@ -2470,7 +2482,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="15"/>
@@ -2478,68 +2490,57 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="15"/>
       <c r="D52" s="10"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>41</v>
-      </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="10"/>
-    </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>42</v>
-      </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="10"/>
+      <c r="A54" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>32</v>
+      <c r="A55" s="6" t="s">
+        <v>315</v>
       </c>
       <c r="B55" s="8"/>
-      <c r="C55" s="15"/>
+      <c r="C55" s="7"/>
       <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>43</v>
+      <c r="A56" s="6" t="s">
+        <v>316</v>
       </c>
       <c r="B56" s="8"/>
-      <c r="C56" s="15"/>
+      <c r="C56" s="7"/>
       <c r="D56" s="10"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>317</v>
       </c>
       <c r="B57" s="8"/>
-      <c r="C57" s="15"/>
+      <c r="C57" s="14"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>87</v>
-      </c>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>318</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="10"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="10"/>
+      <c r="A60" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
-        <v>316</v>
+      <c r="A61" t="s">
+        <v>398</v>
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="7"/>
@@ -2547,7 +2548,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="14"/>
@@ -2555,7 +2556,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="14"/>
@@ -2563,49 +2564,60 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>88</v>
+        <v>399</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>398</v>
-      </c>
-      <c r="B66" s="8"/>
+        <v>54</v>
+      </c>
+      <c r="B66" s="13"/>
       <c r="C66" s="7"/>
       <c r="D66" s="10"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>319</v>
-      </c>
-      <c r="B67" s="8"/>
-      <c r="C67" s="14"/>
+        <v>55</v>
+      </c>
+      <c r="B67" s="13"/>
+      <c r="C67" s="10"/>
       <c r="D67" s="10"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>320</v>
-      </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="14"/>
+        <v>57</v>
+      </c>
+      <c r="B68" s="13"/>
+      <c r="C68" s="7"/>
       <c r="D68" s="10"/>
     </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>56</v>
+      </c>
+      <c r="B69" s="13"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="10"/>
+    </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>399</v>
-      </c>
+      <c r="A70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70" s="13"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="10"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B71" s="13"/>
-      <c r="C71" s="7"/>
+      <c r="C71" s="10"/>
       <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B72" s="13"/>
       <c r="C72" s="10"/>
@@ -2613,7 +2625,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>57</v>
+        <v>136</v>
       </c>
       <c r="B73" s="13"/>
       <c r="C73" s="7"/>
@@ -2621,171 +2633,171 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B74" s="13"/>
-      <c r="C74" s="14"/>
+      <c r="C74" s="10"/>
       <c r="D74" s="10"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B75" s="13"/>
-      <c r="C75" s="7"/>
+      <c r="C75" s="14"/>
       <c r="D75" s="10"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B76" s="13"/>
-      <c r="C76" s="10"/>
+      <c r="C76" s="7"/>
       <c r="D76" s="10"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B77" s="13"/>
-      <c r="C77" s="10"/>
+      <c r="C77" s="7"/>
       <c r="D77" s="10"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B78" s="13"/>
       <c r="C78" s="7"/>
       <c r="D78" s="10"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>60</v>
-      </c>
-      <c r="B79" s="13"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
-    </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>61</v>
-      </c>
-      <c r="B80" s="13"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="10"/>
+      <c r="A80" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>62</v>
-      </c>
-      <c r="B81" s="13"/>
-      <c r="C81" s="7"/>
+        <v>209</v>
+      </c>
+      <c r="B81" s="8"/>
+      <c r="C81" s="14"/>
       <c r="D81" s="10"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>63</v>
-      </c>
-      <c r="B82" s="13"/>
-      <c r="C82" s="7"/>
+        <v>210</v>
+      </c>
+      <c r="B82" s="8"/>
+      <c r="C82" s="14"/>
       <c r="D82" s="10"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>65</v>
-      </c>
-      <c r="B83" s="13"/>
-      <c r="C83" s="7"/>
+        <v>211</v>
+      </c>
+      <c r="B83" s="8"/>
+      <c r="C83" s="14"/>
       <c r="D83" s="10"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>209</v>
-      </c>
-      <c r="B86" s="8"/>
-      <c r="C86" s="14"/>
+        <v>104</v>
+      </c>
+      <c r="B86" s="9"/>
+      <c r="C86" s="7"/>
       <c r="D86" s="10"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>210</v>
-      </c>
-      <c r="B87" s="8"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="10"/>
-    </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>211</v>
-      </c>
-      <c r="B88" s="8"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="10"/>
+      <c r="A88" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="B90"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>104</v>
-      </c>
-      <c r="B91" s="9"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="10"/>
+      <c r="A91" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>70</v>
+      </c>
+      <c r="B92" s="12"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="10"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A93" t="s">
+        <v>71</v>
+      </c>
+      <c r="B93" s="12"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>396</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B94" s="12"/>
+      <c r="C94" s="14"/>
+      <c r="D94" s="10"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B95"/>
+      <c r="A95" t="s">
+        <v>73</v>
+      </c>
+      <c r="B95" s="12"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="10"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>77</v>
-      </c>
+      <c r="A96" t="s">
+        <v>74</v>
+      </c>
+      <c r="B96" s="9"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="10"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>70</v>
-      </c>
-      <c r="B97" s="12"/>
-      <c r="C97" s="14"/>
+        <v>97</v>
+      </c>
+      <c r="B97" s="9"/>
+      <c r="C97" s="7"/>
       <c r="D97" s="10"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>71</v>
-      </c>
-      <c r="B98" s="12"/>
-      <c r="C98" s="10"/>
+        <v>98</v>
+      </c>
+      <c r="B98" s="9"/>
+      <c r="C98" s="14"/>
       <c r="D98" s="10"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>72</v>
+        <v>167</v>
       </c>
       <c r="B99" s="12"/>
-      <c r="C99" s="14"/>
+      <c r="C99" s="7"/>
       <c r="D99" s="10"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>73</v>
+        <v>168</v>
       </c>
       <c r="B100" s="12"/>
       <c r="C100" s="7"/>
@@ -2793,190 +2805,102 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>74</v>
-      </c>
-      <c r="B101" s="9"/>
-      <c r="C101" s="14"/>
+        <v>331</v>
+      </c>
+      <c r="B101" s="13"/>
+      <c r="C101" s="7"/>
       <c r="D101" s="10"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>97</v>
-      </c>
-      <c r="B102" s="9"/>
-      <c r="C102" s="7"/>
+        <v>197</v>
+      </c>
+      <c r="B102" s="12"/>
+      <c r="C102" s="10"/>
       <c r="D102" s="10"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>98</v>
-      </c>
-      <c r="B103" s="9"/>
-      <c r="C103" s="14"/>
+        <v>198</v>
+      </c>
+      <c r="B103" s="12"/>
+      <c r="C103" s="10"/>
       <c r="D103" s="10"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>167</v>
-      </c>
-      <c r="B104" s="12"/>
+        <v>326</v>
+      </c>
+      <c r="B104" s="9"/>
       <c r="C104" s="7"/>
-      <c r="D104" s="10"/>
+      <c r="D104" s="8"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>168</v>
-      </c>
-      <c r="B105" s="12"/>
-      <c r="C105" s="7"/>
-      <c r="D105" s="10"/>
+        <v>328</v>
+      </c>
+      <c r="B105" s="8"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="8"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>331</v>
-      </c>
-      <c r="B106" s="13"/>
+        <v>329</v>
+      </c>
+      <c r="B106" s="9"/>
       <c r="C106" s="7"/>
-      <c r="D106" s="10"/>
+      <c r="D106" s="8"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>197</v>
-      </c>
-      <c r="B107" s="12"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
+        <v>368</v>
+      </c>
+      <c r="B107" s="8"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="8"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>198</v>
-      </c>
-      <c r="B108" s="12"/>
+        <v>537</v>
+      </c>
+      <c r="B108" s="8"/>
       <c r="C108" s="10"/>
-      <c r="D108" s="10"/>
+      <c r="D108" s="8"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>326</v>
-      </c>
-      <c r="B109" s="9"/>
+        <v>334</v>
+      </c>
+      <c r="B109" s="10"/>
       <c r="C109" s="7"/>
-      <c r="D109" s="8"/>
+      <c r="D109" s="10"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>328</v>
-      </c>
-      <c r="B110" s="8"/>
-      <c r="C110" s="10"/>
-      <c r="D110" s="8"/>
+        <v>369</v>
+      </c>
+      <c r="B110" s="15"/>
+      <c r="C110" s="14"/>
+      <c r="D110" s="10"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>329</v>
-      </c>
-      <c r="B111" s="9"/>
-      <c r="C111" s="7"/>
-      <c r="D111" s="8"/>
+      <c r="B111"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>368</v>
-      </c>
-      <c r="B112" s="8"/>
-      <c r="C112" s="7"/>
-      <c r="D112" s="8"/>
+      <c r="A112" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>537</v>
-      </c>
-      <c r="B113" s="8"/>
-      <c r="C113" s="10"/>
-      <c r="D113" s="8"/>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
         <v>80</v>
       </c>
-      <c r="B116" s="13"/>
-      <c r="C116" s="7"/>
-      <c r="D116" s="10"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>81</v>
-      </c>
-      <c r="B117" s="8"/>
-      <c r="C117" s="7"/>
-      <c r="D117" s="14"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>83</v>
-      </c>
-      <c r="B118" s="8"/>
-      <c r="C118" s="7"/>
-      <c r="D118" s="10"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>84</v>
-      </c>
-      <c r="B119" s="8"/>
-      <c r="C119" s="7"/>
-      <c r="D119" s="14"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>212</v>
-      </c>
-      <c r="B120" s="8"/>
-      <c r="C120" s="10"/>
-      <c r="D120" s="14"/>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>230</v>
-      </c>
-      <c r="B121" s="13"/>
-      <c r="C121" s="10"/>
-      <c r="D121" s="10"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>322</v>
-      </c>
-      <c r="B122" s="8"/>
-      <c r="C122" s="13"/>
-      <c r="D122" s="14"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>321</v>
-      </c>
-      <c r="B123" s="8"/>
-      <c r="C123" s="13"/>
-      <c r="D123" s="14"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>370</v>
-      </c>
-      <c r="B124" s="8"/>
-      <c r="C124" s="13"/>
-      <c r="D124" s="10"/>
-    </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B175"/>
-    </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177"/>
+      <c r="B113" s="13"/>
+      <c r="C113" s="7"/>
+      <c r="D113" s="10"/>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B176"/>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B178"/>
@@ -3005,11 +2929,11 @@
     <row r="186" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B186"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B189"/>
-    </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B203"/>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B187"/>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B190"/>
     </row>
     <row r="204" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B204"/>
@@ -3029,11 +2953,11 @@
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B209"/>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="19"/>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B210"/>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B224"/>
+      <c r="A224" s="19"/>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B225"/>
@@ -3044,8 +2968,8 @@
     <row r="227" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B227"/>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B265"/>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B228"/>
     </row>
     <row r="266" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B266"/>
@@ -3053,8 +2977,8 @@
     <row r="267" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B267"/>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B269"/>
+    <row r="268" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B268"/>
     </row>
     <row r="270" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B270"/>
@@ -3068,8 +2992,11 @@
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B273"/>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="2"/>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B274"/>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3232,10 +3159,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>491</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>492</v>
       </c>
     </row>
@@ -3243,7 +3170,7 @@
       <c r="A2" s="1">
         <v>147</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="24">
         <v>40766</v>
       </c>
     </row>
@@ -3254,10 +3181,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3268,7 +3195,7 @@
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>99</v>
       </c>
@@ -3282,55 +3209,73 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="14"/>
       <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="10"/>
       <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="10"/>
       <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3339,16 +3284,22 @@
       <c r="D8" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="14"/>
       <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3357,32 +3308,44 @@
       <c r="D10" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>195</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>194</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="14"/>
       <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>193</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="14"/>
       <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -3391,8 +3354,11 @@
       <c r="D14" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -3401,8 +3367,11 @@
       <c r="D15" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -3411,8 +3380,11 @@
       <c r="D16" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -3421,8 +3393,11 @@
       <c r="D17" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -3431,8 +3406,11 @@
       <c r="D18" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" s="6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -3441,8 +3419,11 @@
       <c r="D19" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19" s="6" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -3451,8 +3432,11 @@
       <c r="D20" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -3461,8 +3445,11 @@
       <c r="D21" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -3471,8 +3458,11 @@
       <c r="D22" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -3481,8 +3471,11 @@
       <c r="D23" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -3491,192 +3484,264 @@
       <c r="D24" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>306</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>307</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>89</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>207</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>90</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>237</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>238</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>239</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>240</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="14"/>
       <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>242</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>241</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="14"/>
       <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>66</v>
       </c>
       <c r="B36" s="13"/>
       <c r="C36" s="14"/>
       <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>233</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>75</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>76</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>169</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>179</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>327</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>330</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>332</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>78</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="14"/>
       <c r="D45" s="7"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F45" s="6" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>82</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>85</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -4053,6 +4118,112 @@
       <c r="B95" s="8"/>
       <c r="C95" s="13"/>
       <c r="D95" s="7"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>404</v>
+      </c>
+      <c r="B96" s="10"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="7"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>222</v>
+      </c>
+      <c r="B97" s="10"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>141</v>
+      </c>
+      <c r="B98" s="8"/>
+      <c r="C98" s="14"/>
+      <c r="D98" s="7"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>212</v>
+      </c>
+      <c r="B99" s="8"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="7"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>230</v>
+      </c>
+      <c r="B100" s="13"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="7"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>81</v>
+      </c>
+      <c r="B101" s="8"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="7"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>370</v>
+      </c>
+      <c r="B102" s="8"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="7"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>370</v>
+      </c>
+      <c r="B103" s="8"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="7"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>81</v>
+      </c>
+      <c r="B104" s="8"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="7"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>83</v>
+      </c>
+      <c r="B105" s="8"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="7"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>84</v>
+      </c>
+      <c r="B106" s="8"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="7"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>322</v>
+      </c>
+      <c r="B108" s="8"/>
+      <c r="C108" s="13"/>
+      <c r="D108" s="7"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>321</v>
+      </c>
+      <c r="B109" s="8"/>
+      <c r="C109" s="13"/>
+      <c r="D109" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4061,18 +4232,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E186"/>
+  <dimension ref="A1:E188"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="89.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="83.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -4092,828 +4263,688 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>427</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>428</v>
+        <v>436</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="20"/>
-      <c r="E2" s="6" t="s">
-        <v>429</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="20"/>
-      <c r="E3" s="6" t="s">
-        <v>430</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
-        <v>437</v>
-      </c>
       <c r="C4" s="6"/>
       <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="6"/>
-      <c r="D5" s="20"/>
+      <c r="A5" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>510</v>
+      </c>
+      <c r="C5" t="s">
+        <v>308</v>
+      </c>
+      <c r="D5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="6"/>
-      <c r="D6" s="20"/>
+      <c r="C6" t="s">
+        <v>471</v>
+      </c>
+      <c r="D6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="20"/>
+      <c r="C7" t="s">
+        <v>474</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="E7" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>516</v>
-      </c>
       <c r="C8" t="s">
-        <v>439</v>
+        <v>473</v>
       </c>
       <c r="D8" t="s">
-        <v>115</v>
+        <v>432</v>
       </c>
       <c r="E8" t="s">
-        <v>135</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>438</v>
-      </c>
       <c r="C9" t="s">
-        <v>308</v>
+        <v>486</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>435</v>
       </c>
       <c r="E9" t="s">
-        <v>180</v>
+        <v>458</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>304</v>
-      </c>
       <c r="C10" t="s">
-        <v>458</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>431</v>
+        <v>513</v>
+      </c>
+      <c r="D10" t="s">
+        <v>350</v>
       </c>
       <c r="E10" t="s">
-        <v>218</v>
+        <v>532</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>499</v>
-      </c>
-      <c r="C11" t="s">
-        <v>471</v>
-      </c>
       <c r="D11" t="s">
-        <v>432</v>
-      </c>
-      <c r="E11" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>510</v>
-      </c>
-      <c r="C12" t="s">
-        <v>474</v>
-      </c>
-      <c r="D12" t="s">
-        <v>435</v>
-      </c>
-      <c r="E12" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>523</v>
-      </c>
-      <c r="C13" t="s">
-        <v>473</v>
-      </c>
-      <c r="D13" t="s">
-        <v>350</v>
-      </c>
-      <c r="E13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>486</v>
-      </c>
-      <c r="D14" t="s">
         <v>440</v>
       </c>
-      <c r="E14" t="s">
-        <v>235</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
       <c r="C15" t="s">
-        <v>513</v>
-      </c>
-      <c r="E15" t="s">
-        <v>236</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
       <c r="C16" t="s">
-        <v>532</v>
-      </c>
-      <c r="E16" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-      <c r="E18" t="s">
-        <v>118</v>
+        <v>309</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>68</v>
+      <c r="A19" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>447</v>
       </c>
       <c r="C19" t="s">
-        <v>309</v>
-      </c>
-      <c r="E19" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>448</v>
+      </c>
       <c r="C20" t="s">
-        <v>442</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>498</v>
+      </c>
+      <c r="C21" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>447</v>
+      <c r="B22" t="s">
+        <v>506</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
-      </c>
-      <c r="E22" t="s">
-        <v>144</v>
+        <v>443</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>448</v>
+        <v>514</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
-      </c>
-      <c r="E23" t="s">
-        <v>279</v>
+        <v>522</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>498</v>
+        <v>515</v>
       </c>
       <c r="C24" t="s">
-        <v>253</v>
-      </c>
-      <c r="E24" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
         <v>500</v>
       </c>
-      <c r="C25" t="s">
-        <v>443</v>
-      </c>
-      <c r="E25" t="s">
-        <v>281</v>
-      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>506</v>
-      </c>
-      <c r="C26" t="s">
-        <v>522</v>
-      </c>
-      <c r="E26" t="s">
-        <v>284</v>
-      </c>
+      <c r="A26" s="23"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>514</v>
-      </c>
-      <c r="E27" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>515</v>
-      </c>
-      <c r="E28" t="s">
-        <v>419</v>
-      </c>
+      <c r="A27" s="23"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
+      <c r="A29" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="B29" t="s">
+        <v>423</v>
+      </c>
+      <c r="C29" t="s">
+        <v>391</v>
+      </c>
       <c r="E29" t="s">
-        <v>509</v>
+        <v>409</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="E30" t="s">
-        <v>487</v>
+      <c r="B30" t="s">
+        <v>444</v>
+      </c>
+      <c r="C30" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
-        <v>392</v>
-      </c>
       <c r="B32" t="s">
-        <v>409</v>
-      </c>
-      <c r="C32" t="s">
-        <v>391</v>
-      </c>
-      <c r="E32" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>423</v>
-      </c>
-      <c r="C33" t="s">
-        <v>461</v>
-      </c>
-      <c r="E33" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="7" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
+      <c r="B36" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
       <c r="B37" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="B39" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
-      <c r="B40" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
-      <c r="B41" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
-      <c r="B42" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="23"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="25"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
+        <v>411</v>
+      </c>
       <c r="B43" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+        <v>457</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="23" t="s">
-        <v>411</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B46" s="6" t="s">
         <v>459</v>
       </c>
+      <c r="C46" s="6" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="C47" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>464</v>
+      </c>
+      <c r="C48" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>465</v>
+      </c>
       <c r="C49" s="6" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="6" t="s">
-        <v>460</v>
-      </c>
-      <c r="C50" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>464</v>
-      </c>
-      <c r="C51" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>465</v>
-      </c>
-      <c r="C52" s="6" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="24"/>
-      <c r="C53" s="24"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="24"/>
-      <c r="C54" s="24"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="24"/>
-      <c r="C55" s="24"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="23" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
+      <c r="C50" s="23"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
+      <c r="C51" s="23"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="23"/>
+      <c r="C52" s="23"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
         <v>17</v>
       </c>
+      <c r="B54" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>112</v>
-      </c>
-      <c r="E57" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>449</v>
-      </c>
-      <c r="E58" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="22" t="s">
+        <v>533</v>
+      </c>
       <c r="B61" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="23" t="s">
-        <v>533</v>
-      </c>
-      <c r="B64" t="s">
-        <v>534</v>
-      </c>
-      <c r="E64" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="24"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="24"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="23" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="23"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="23"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="22" t="s">
         <v>100</v>
       </c>
+      <c r="B66" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="C68" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="C71" t="s">
-        <v>338</v>
-      </c>
-      <c r="E71" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
         <v>466</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C69" t="s">
         <v>165</v>
       </c>
-      <c r="E72" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E73" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="23" t="s">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="26"/>
+      <c r="B70" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="26"/>
+      <c r="B71" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="22" t="s">
         <v>507</v>
       </c>
+      <c r="B73" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>505</v>
-      </c>
-      <c r="E74" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
         <v>508</v>
       </c>
-      <c r="E75" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="6" t="s">
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="6" t="s">
         <v>535</v>
       </c>
-      <c r="E76" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E77" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E78" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E79" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="23" t="s">
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="22" t="s">
         <v>88</v>
       </c>
+      <c r="B79" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>339</v>
-      </c>
-      <c r="E80" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>340</v>
-      </c>
-      <c r="E81" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>341</v>
-      </c>
-      <c r="E82" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>342</v>
-      </c>
-      <c r="E83" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C85" s="20"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="23" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="20"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="22" t="s">
         <v>405</v>
       </c>
+      <c r="B85" t="s">
+        <v>408</v>
+      </c>
+      <c r="C85" s="6"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C86" s="6"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C87" s="6"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>407</v>
-      </c>
-      <c r="C88" s="6"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="23"/>
       <c r="B89" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="24"/>
-      <c r="B90" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C91" s="20"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="23" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="20"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B91" t="s">
         <v>526</v>
       </c>
+      <c r="C91" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="23"/>
       <c r="C92" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="24"/>
-      <c r="C93" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="24"/>
-      <c r="B94" s="19"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="24"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="24"/>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="23"/>
+      <c r="B93" s="19"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="23"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="23"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="B97" t="s">
+        <v>336</v>
+      </c>
+      <c r="C97" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="23" t="s">
-        <v>252</v>
-      </c>
+      <c r="A98" s="23"/>
       <c r="B98" t="s">
-        <v>336</v>
-      </c>
-      <c r="C98" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="24"/>
-      <c r="B99" t="s">
         <v>528</v>
       </c>
     </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="B100" t="s">
+        <v>358</v>
+      </c>
+    </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="23" t="s">
-        <v>414</v>
-      </c>
       <c r="B101" t="s">
-        <v>358</v>
+        <v>412</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
-        <v>413</v>
-      </c>
+      <c r="C103" s="20"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C104" s="20"/>
+      <c r="A104" s="22" t="s">
+        <v>415</v>
+      </c>
+      <c r="B104" t="s">
+        <v>221</v>
+      </c>
+      <c r="C104" t="s">
+        <v>468</v>
+      </c>
+      <c r="D104" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="23" t="s">
-        <v>415</v>
-      </c>
-      <c r="B105" t="s">
-        <v>221</v>
+      <c r="B105" s="3" t="s">
+        <v>529</v>
       </c>
       <c r="C105" t="s">
-        <v>468</v>
+        <v>363</v>
       </c>
       <c r="D105" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="3" t="s">
-        <v>529</v>
-      </c>
-      <c r="C106" t="s">
-        <v>363</v>
+      <c r="B106" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="D106" t="s">
-        <v>470</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="6" t="s">
-        <v>134</v>
+      <c r="B107" t="s">
+        <v>106</v>
       </c>
       <c r="D107" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D108" t="s">
         <v>416</v>
       </c>
     </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="22" t="s">
+        <v>382</v>
+      </c>
+      <c r="B109" t="s">
+        <v>489</v>
+      </c>
+      <c r="C109" s="20"/>
+    </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="23" t="s">
-        <v>382</v>
-      </c>
       <c r="B110" t="s">
-        <v>489</v>
-      </c>
-      <c r="C110" s="20"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
         <v>490</v>
       </c>
     </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="22" t="s">
+        <v>530</v>
+      </c>
+      <c r="B112" t="s">
+        <v>531</v>
+      </c>
+      <c r="C112" s="20"/>
+    </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="23" t="s">
-        <v>530</v>
-      </c>
       <c r="B113" t="s">
-        <v>531</v>
-      </c>
-      <c r="C113" s="20"/>
+        <v>503</v>
+      </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
         <v>504</v>
       </c>
     </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116" t="s">
+        <v>455</v>
+      </c>
+      <c r="C116" t="s">
+        <v>453</v>
+      </c>
+    </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B117" t="s">
-        <v>455</v>
-      </c>
       <c r="C117" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C118" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C139" s="20"/>
-    </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C143" s="20"/>
-    </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C146" s="20"/>
-    </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C153" s="20"/>
-    </row>
-    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C156" s="20"/>
-    </row>
-    <row r="159" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C159" s="20"/>
-    </row>
-    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C165" s="20"/>
-    </row>
-    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C168" s="20"/>
-    </row>
-    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C171" s="20"/>
-    </row>
-    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C174" s="20"/>
-    </row>
-    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C177" s="20"/>
-    </row>
-    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C181" s="20"/>
-    </row>
-    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C186" s="20"/>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C141" s="20"/>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" s="20"/>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C148" s="20"/>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C155" s="20"/>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C158" s="20"/>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C161" s="20"/>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C167" s="20"/>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C170" s="20"/>
+    </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C173" s="20"/>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C176" s="20"/>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C179" s="20"/>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C183" s="20"/>
+    </row>
+    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C188" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4935,7 +4966,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>475</v>
       </c>
     </row>
@@ -5005,7 +5036,7 @@
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="21" t="s">
         <v>476</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added things to do and modified business plan
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="545">
   <si>
     <t>Add debug mode button to reload the stats</t>
   </si>
@@ -1649,6 +1649,18 @@
   </si>
   <si>
     <t>Upgrade effect should keep going (255-&gt; 0)</t>
+  </si>
+  <si>
+    <t>Make a website that is centered on Commander</t>
+  </si>
+  <si>
+    <t>.gitignore =&gt; only one file</t>
+  </si>
+  <si>
+    <t>T-shirts</t>
+  </si>
+  <si>
+    <t>Tell my friends about the event</t>
   </si>
 </sst>
 </file>
@@ -1761,7 +1773,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1838,8 +1850,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2841,11 +2856,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>355</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2953,10 +2968,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2981,6 +2996,14 @@
         <v>40766</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>151</v>
+      </c>
+      <c r="B3" s="24">
+        <v>40778</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2991,7 +3014,7 @@
   <dimension ref="A1:F109"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3813,6 +3836,9 @@
       <c r="B72" s="8"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
+      <c r="F72" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
@@ -3821,6 +3847,9 @@
       <c r="B73" s="8"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
+      <c r="F73" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
@@ -3829,6 +3858,9 @@
       <c r="B74" s="8"/>
       <c r="C74" s="14"/>
       <c r="D74" s="7"/>
+      <c r="F74" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
@@ -3837,6 +3869,14 @@
       <c r="B75" s="8"/>
       <c r="C75" s="14"/>
       <c r="D75" s="7"/>
+      <c r="F75" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
@@ -3845,6 +3885,9 @@
       <c r="B77" s="10"/>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
+      <c r="F77" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
@@ -3853,6 +3896,9 @@
       <c r="B78" s="10"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
+      <c r="F78" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
@@ -3861,6 +3907,9 @@
       <c r="B79" s="10"/>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
+      <c r="F79" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
@@ -4105,11 +4154,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E197"/>
+  <dimension ref="A1:E199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4234,12 +4283,12 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>91</v>
       </c>
@@ -4249,83 +4298,67 @@
       <c r="C19" t="s">
         <v>92</v>
       </c>
-      <c r="E19" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
-        <v>536</v>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>493</v>
       </c>
       <c r="C20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>493</v>
-      </c>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>372</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>403</v>
+        <v>424</v>
       </c>
       <c r="C29" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
-        <v>424</v>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>426</v>
       </c>
       <c r="C30" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="7" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="7" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
         <v>537</v>
       </c>
     </row>
@@ -4359,7 +4392,7 @@
       <c r="A46" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="B46" s="34" t="s">
+      <c r="B46" t="s">
         <v>439</v>
       </c>
       <c r="C46" s="6" t="s">
@@ -4367,7 +4400,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="34" t="s">
+      <c r="B47" t="s">
         <v>440</v>
       </c>
       <c r="C47" t="s">
@@ -4375,7 +4408,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="7" t="s">
+      <c r="B48" t="s">
         <v>444</v>
       </c>
       <c r="C48" t="s">
@@ -4383,7 +4416,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="7" t="s">
+      <c r="B49" t="s">
         <v>445</v>
       </c>
       <c r="C49" s="6" t="s">
@@ -4454,7 +4487,7 @@
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="23"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="22" t="s">
         <v>84</v>
       </c>
@@ -4462,7 +4495,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="22" t="s">
         <v>66</v>
       </c>
@@ -4472,11 +4505,8 @@
       <c r="C68" t="s">
         <v>319</v>
       </c>
-      <c r="E68" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>517</v>
       </c>
@@ -4484,45 +4514,42 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="26"/>
       <c r="B70" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="26"/>
-      <c r="B71" s="7" t="s">
+      <c r="B71" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="30"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="31"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="31"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="32"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>528</v>
+      <c r="B77" t="s">
+        <v>506</v>
       </c>
       <c r="D77" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>506</v>
-      </c>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
         <v>518</v>
       </c>
@@ -4562,7 +4589,7 @@
       <c r="A89" s="22" t="s">
         <v>385</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B89" t="s">
         <v>388</v>
       </c>
       <c r="C89" s="6"/>
@@ -4586,309 +4613,321 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="23"/>
-      <c r="B93" s="7" t="s">
-        <v>505</v>
+      <c r="B93" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="31"/>
-      <c r="B94" s="7" t="s">
-        <v>525</v>
+      <c r="B94" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="31"/>
-      <c r="B95" s="7" t="s">
-        <v>534</v>
+      <c r="B95" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="33"/>
-      <c r="B96" s="7" t="s">
-        <v>538</v>
-      </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C97" s="20"/>
+      <c r="A97" s="34"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="22" t="s">
+      <c r="C98" s="20"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>504</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>447</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="23"/>
-      <c r="C99" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="23"/>
-      <c r="B100" s="19"/>
+      <c r="C100" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="23"/>
+      <c r="B101" s="19"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="23"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="23"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="22" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="23"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="23"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="22" t="s">
         <v>394</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D108" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C110" s="20"/>
-    </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="22" t="s">
+      <c r="C111" s="20"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="22" t="s">
         <v>395</v>
       </c>
-      <c r="B111" s="29" t="s">
+      <c r="B112" s="29" t="s">
         <v>507</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C112" t="s">
         <v>448</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D112" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B112" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
         <v>524</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C113" t="s">
         <v>343</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D113" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D113" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>542</v>
+      </c>
+      <c r="D114" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D114" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D115" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
         <v>205</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="27"/>
-      <c r="D116" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="27"/>
-      <c r="D117" s="6" t="s">
+      <c r="D117" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="27"/>
+      <c r="D118" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="22" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="22" t="s">
         <v>362</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B120" t="s">
         <v>469</v>
       </c>
-      <c r="C119" s="20"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B120" t="s">
+      <c r="C120" s="20"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="22" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="22" t="s">
         <v>508</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B123" t="s">
         <v>509</v>
       </c>
-      <c r="C122" s="20"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
-        <v>483</v>
-      </c>
+      <c r="C123" s="20"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="7" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="22" t="s">
+      <c r="A126" s="35"/>
+      <c r="B126" s="7" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B128" t="s">
         <v>435</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C128" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C127" t="s">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B129" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="C129" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="28" t="s">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B131" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B130" t="s">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B132" t="s">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B133" t="s">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B134" t="s">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B135" t="s">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B136" t="s">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B137" t="s">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B138" t="s">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B139" t="s">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B140" t="s">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B141" t="s">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B142" t="s">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
         <v>309</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B143" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B144" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>515</v>
+        <v>310</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>315</v>
+        <v>348</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C150" s="20"/>
-    </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C154" s="20"/>
-    </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C157" s="20"/>
-    </row>
-    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C164" s="20"/>
-    </row>
-    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C167" s="20"/>
-    </row>
-    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C170" s="20"/>
-    </row>
-    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C176" s="20"/>
-    </row>
-    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C179" s="20"/>
-    </row>
-    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C182" s="20"/>
-    </row>
-    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C185" s="20"/>
-    </row>
-    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C188" s="20"/>
-    </row>
-    <row r="192" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C192" s="20"/>
-    </row>
-    <row r="197" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C197" s="20"/>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C152" s="20"/>
+    </row>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C156" s="20"/>
+    </row>
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C159" s="20"/>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C166" s="20"/>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C169" s="20"/>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C172" s="20"/>
+    </row>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C178" s="20"/>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C181" s="20"/>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C184" s="20"/>
+    </row>
+    <row r="187" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C187" s="20"/>
+    </row>
+    <row r="190" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C190" s="20"/>
+    </row>
+    <row r="194" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C194" s="20"/>
+    </row>
+    <row r="199" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C199" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Replug the temporary Cheats controller.
</commit_message>
<xml_diff>
--- a/Utilities/Tasks.xlsx
+++ b/Utilities/Tasks.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="601">
   <si>
     <t>Add debug mode button to reload the stats</t>
   </si>
@@ -1826,6 +1826,9 @@
   </si>
   <si>
     <t>Be able to skip some levels</t>
+  </si>
+  <si>
+    <t>Make the Cheats controller Input-dependant</t>
   </si>
 </sst>
 </file>
@@ -2042,10 +2045,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent2" xfId="2" builtinId="33"/>
@@ -2355,8 +2358,8 @@
   <dimension ref="A1:D268"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3051,11 +3054,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>354</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -4588,8 +4591,8 @@
   <dimension ref="A1:E200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4640,7 +4643,7 @@
       <c r="A5" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="41" t="s">
         <v>482</v>
       </c>
       <c r="C5" t="s">
@@ -4704,7 +4707,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="41" t="s">
         <v>482</v>
       </c>
     </row>
@@ -5005,6 +5008,9 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>600</v>
+      </c>
       <c r="D78" t="s">
         <v>511</v>
       </c>

</xml_diff>